<commit_message>
Overall results now show widths < 1000
</commit_message>
<xml_diff>
--- a/results/overall.xlsx
+++ b/results/overall.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21231"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{78B08C9F-3EC4-4FFA-8750-18B20330B269}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2D0070BC-B6F2-4749-AB88-2E63EC4597BC}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Length" sheetId="1" r:id="rId1"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="237" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="236" uniqueCount="49">
   <si>
     <t>Python</t>
   </si>
@@ -176,9 +176,6 @@
   </si>
   <si>
     <t>spring-framework</t>
-  </si>
-  <si>
-    <t>Without javascript, the average was around 64</t>
   </si>
 </sst>
 </file>
@@ -251,11 +248,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -542,8 +538,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:O44"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="J2" sqref="J2:O7"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J11" sqref="J10:J11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -590,13 +586,13 @@
         <v>1</v>
       </c>
       <c r="E2" s="1">
-        <v>19.16631092138029</v>
+        <v>19.130612972202425</v>
       </c>
       <c r="F2" s="1">
-        <v>39.707140069275432</v>
+        <v>39.724643065669298</v>
       </c>
       <c r="G2" s="1">
-        <v>0.52956977169696184</v>
+        <v>0.53027502424260975</v>
       </c>
       <c r="K2" s="2" t="s">
         <v>11</v>
@@ -638,7 +634,7 @@
       </c>
       <c r="K3" s="1">
         <f>MAX(C2:C44)</f>
-        <v>42716</v>
+        <v>16517</v>
       </c>
       <c r="L3" s="1">
         <f>MIN(C2:C44)</f>
@@ -646,15 +642,15 @@
       </c>
       <c r="M3" s="1">
         <f>AVERAGE(C2:C44)</f>
-        <v>2836.9250000000002</v>
+        <v>2032.675</v>
       </c>
       <c r="N3" s="1">
         <f>_xlfn.STDEV.P(C2:C44)</f>
-        <v>6980.2360898020488</v>
+        <v>3580.3960631995728</v>
       </c>
       <c r="O3" s="1">
         <f>N3/SQRT(COUNT(C2:C44))</f>
-        <v>1103.6722324741049</v>
+        <v>566.11032426054112</v>
       </c>
     </row>
     <row r="4" spans="1:15" x14ac:dyDescent="0.25">
@@ -732,15 +728,15 @@
       </c>
       <c r="M5" s="1">
         <f>AVERAGE(E2:E44)</f>
-        <v>33.383041453010932</v>
+        <v>30.199290061247517</v>
       </c>
       <c r="N5" s="1">
         <f>_xlfn.STDEV.P(E2:E44)</f>
-        <v>78.924437016690248</v>
+        <v>77.172847802762647</v>
       </c>
       <c r="O5" s="1">
         <f>N5/SQRT(COUNT(E2:E44))</f>
-        <v>12.479049200962292</v>
+        <v>12.202098628912536</v>
       </c>
     </row>
     <row r="6" spans="1:15" x14ac:dyDescent="0.25">
@@ -754,13 +750,13 @@
         <v>1</v>
       </c>
       <c r="E6" s="1">
-        <v>22.476512360915962</v>
+        <v>22.472590510200206</v>
       </c>
       <c r="F6" s="1">
-        <v>60.459767305915278</v>
+        <v>60.465062164100772</v>
       </c>
       <c r="G6" s="1">
-        <v>0.37257722335793592</v>
+        <v>0.37268062214648062</v>
       </c>
       <c r="J6" s="2" t="s">
         <v>14</v>
@@ -775,15 +771,15 @@
       </c>
       <c r="M6" s="1">
         <f>AVERAGE(F2:F44)</f>
-        <v>97.754494454621678</v>
+        <v>78.289419644954336</v>
       </c>
       <c r="N6" s="1">
         <f>_xlfn.STDEV.P(F2:F44)</f>
-        <v>237.08373178787144</v>
+        <v>218.85146779379858</v>
       </c>
       <c r="O6" s="1">
         <f>N6/SQRT(COUNT(F2:F44))</f>
-        <v>37.486229431106885</v>
+        <v>34.603455374969435</v>
       </c>
     </row>
     <row r="7" spans="1:15" x14ac:dyDescent="0.25">
@@ -818,15 +814,15 @@
       </c>
       <c r="M7" s="1">
         <f>AVERAGE(G2:G44)</f>
-        <v>2.4309404680252733</v>
+        <v>1.9930877888506167</v>
       </c>
       <c r="N7" s="1">
         <f>_xlfn.STDEV.P(G2:G44)</f>
-        <v>6.7949044154664984</v>
+        <v>6.2937306934318134</v>
       </c>
       <c r="O7" s="1">
         <f>N7/SQRT(COUNT(G2:G44))</f>
-        <v>1.0743687218004594</v>
+        <v>0.99512619854777329</v>
       </c>
     </row>
     <row r="8" spans="1:15" x14ac:dyDescent="0.25">
@@ -940,7 +936,7 @@
       </c>
     </row>
     <row r="14" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="B14" s="3" t="s">
+      <c r="B14" s="2" t="s">
         <v>40</v>
       </c>
       <c r="C14" s="1">
@@ -960,7 +956,7 @@
       </c>
     </row>
     <row r="15" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="B15" s="3" t="s">
+      <c r="B15" s="2" t="s">
         <v>41</v>
       </c>
       <c r="C15" s="1">
@@ -980,7 +976,7 @@
       </c>
     </row>
     <row r="16" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="B16" s="3" t="s">
+      <c r="B16" s="2" t="s">
         <v>42</v>
       </c>
       <c r="C16" s="1">
@@ -1000,7 +996,7 @@
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B17" s="3" t="s">
+      <c r="B17" s="2" t="s">
         <v>43</v>
       </c>
       <c r="C17" s="1">
@@ -1020,7 +1016,7 @@
       </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B18" s="3" t="s">
+      <c r="B18" s="2" t="s">
         <v>44</v>
       </c>
       <c r="C18" s="1">
@@ -1040,7 +1036,7 @@
       </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B19" s="3" t="s">
+      <c r="B19" s="2" t="s">
         <v>45</v>
       </c>
       <c r="C19" s="1">
@@ -1060,7 +1056,7 @@
       </c>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B20" s="3" t="s">
+      <c r="B20" s="2" t="s">
         <v>46</v>
       </c>
       <c r="C20" s="1">
@@ -1080,7 +1076,7 @@
       </c>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B21" s="3" t="s">
+      <c r="B21" s="2" t="s">
         <v>47</v>
       </c>
       <c r="C21" s="1">
@@ -1100,7 +1096,7 @@
       </c>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B22" s="3" t="s">
+      <c r="B22" s="2" t="s">
         <v>48</v>
       </c>
       <c r="C22" s="1">
@@ -1130,7 +1126,7 @@
       <c r="G23" s="1"/>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B24" s="3" t="s">
+      <c r="B24" s="2" t="s">
         <v>17</v>
       </c>
       <c r="C24" s="1">
@@ -1140,17 +1136,17 @@
         <v>1</v>
       </c>
       <c r="E24" s="1">
-        <v>30.58907510862818</v>
+        <v>30.592414921835317</v>
       </c>
       <c r="F24" s="1">
-        <v>165.05880087036488</v>
+        <v>165.06781659292028</v>
       </c>
       <c r="G24" s="1">
-        <v>1.239922591352723</v>
+        <v>1.2400602963634322</v>
       </c>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B25" s="3" t="s">
+      <c r="B25" s="2" t="s">
         <v>18</v>
       </c>
       <c r="C25" s="1">
@@ -1170,7 +1166,7 @@
       </c>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B26" s="3" t="s">
+      <c r="B26" s="2" t="s">
         <v>19</v>
       </c>
       <c r="C26" s="1">
@@ -1180,17 +1176,17 @@
         <v>1</v>
       </c>
       <c r="E26" s="1">
-        <v>16.292759706190974</v>
+        <v>17.486425339366516</v>
       </c>
       <c r="F26" s="1">
-        <v>63.646216222949164</v>
+        <v>65.934415147148016</v>
       </c>
       <c r="G26" s="1">
-        <v>2.0617031741953791</v>
+        <v>2.2176143628772422</v>
       </c>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B27" s="3" t="s">
+      <c r="B27" s="2" t="s">
         <v>20</v>
       </c>
       <c r="C27" s="1">
@@ -1200,17 +1196,17 @@
         <v>1</v>
       </c>
       <c r="E27" s="1">
-        <v>47.717131474103589</v>
+        <v>46.356000000000002</v>
       </c>
       <c r="F27" s="1">
-        <v>72.6073025514888</v>
+        <v>69.482985428088796</v>
       </c>
       <c r="G27" s="1">
-        <v>4.5829322994528576</v>
+        <v>4.3944898516210049</v>
       </c>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B28" s="3" t="s">
+      <c r="B28" s="2" t="s">
         <v>21</v>
       </c>
       <c r="C28" s="1">
@@ -1230,47 +1226,47 @@
       </c>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B29" s="3" t="s">
+      <c r="B29" s="2" t="s">
         <v>22</v>
       </c>
       <c r="C29" s="1">
-        <v>6417</v>
+        <v>730</v>
       </c>
       <c r="D29" s="1">
         <v>1</v>
       </c>
       <c r="E29" s="1">
-        <v>137.4275956284153</v>
+        <v>18.134529147982065</v>
       </c>
       <c r="F29" s="1">
-        <v>499.51864146687006</v>
+        <v>64.150186873456377</v>
       </c>
       <c r="G29" s="1">
-        <v>18.462740250532065</v>
+        <v>2.4801895136795258</v>
       </c>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B30" s="3" t="s">
+      <c r="B30" s="2" t="s">
         <v>23</v>
       </c>
       <c r="C30" s="1">
-        <v>746</v>
+        <v>462</v>
       </c>
       <c r="D30" s="1">
         <v>1</v>
       </c>
       <c r="E30" s="1">
-        <v>29.20257234726688</v>
+        <v>27.366403607666292</v>
       </c>
       <c r="F30" s="1">
-        <v>67.371287419174394</v>
+        <v>54.91756576103699</v>
       </c>
       <c r="G30" s="1">
-        <v>2.2056369293743083</v>
+        <v>1.8439513932942531</v>
       </c>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B31" s="3" t="s">
+      <c r="B31" s="2" t="s">
         <v>24</v>
       </c>
       <c r="C31" s="1">
@@ -1280,37 +1276,37 @@
         <v>1</v>
       </c>
       <c r="E31" s="1">
-        <v>29.718722073279714</v>
+        <v>29.977682596934176</v>
       </c>
       <c r="F31" s="1">
-        <v>196.37502129389887</v>
+        <v>197.23938232098257</v>
       </c>
       <c r="G31" s="1">
-        <v>2.9352237054630828</v>
+        <v>2.9614054075571348</v>
       </c>
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B32" s="3" t="s">
+      <c r="B32" s="2" t="s">
         <v>25</v>
       </c>
       <c r="C32" s="1">
-        <v>42716</v>
+        <v>16517</v>
       </c>
       <c r="D32" s="1">
         <v>1</v>
       </c>
       <c r="E32" s="1">
-        <v>26.958872752244577</v>
+        <v>20.685010958464744</v>
       </c>
       <c r="F32" s="1">
-        <v>502.21295658861345</v>
+        <v>171.37448111493558</v>
       </c>
       <c r="G32" s="1">
-        <v>1.7909469791980743</v>
+        <v>0.62648991469281545</v>
       </c>
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B33" s="3" t="s">
+      <c r="B33" s="2" t="s">
         <v>26</v>
       </c>
       <c r="C33" s="1">
@@ -1350,13 +1346,13 @@
         <v>2</v>
       </c>
       <c r="E35" s="1">
-        <v>17.749833935018049</v>
+        <v>17.747660582255083</v>
       </c>
       <c r="F35" s="1">
-        <v>29.036514326488128</v>
+        <v>29.034117260006202</v>
       </c>
       <c r="G35" s="1">
-        <v>0.15604490367643917</v>
+        <v>0.15603427483907159</v>
       </c>
     </row>
     <row r="36" spans="1:7" x14ac:dyDescent="0.25">
@@ -1550,7 +1546,7 @@
   <dimension ref="A1:O44"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="K3" sqref="K3"/>
+      <selection activeCell="L18" sqref="L18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1583,19 +1579,19 @@
         <v>28</v>
       </c>
       <c r="C2" s="1">
-        <v>6177</v>
+        <v>501</v>
       </c>
       <c r="D2" s="1">
         <v>14</v>
       </c>
       <c r="E2" s="1">
-        <v>91.123977232301669</v>
+        <v>85.162687099073409</v>
       </c>
       <c r="F2" s="1">
-        <v>164.12861363011388</v>
+        <v>43.77879353212866</v>
       </c>
       <c r="G2" s="1">
-        <v>2.1889653170033587</v>
+        <v>0.58439293622311617</v>
       </c>
       <c r="K2" s="2" t="s">
         <v>11</v>
@@ -1637,7 +1633,7 @@
       </c>
       <c r="K3" s="1">
         <f>MAX(C2:C44)</f>
-        <v>286809</v>
+        <v>976</v>
       </c>
       <c r="L3" s="1">
         <f>MIN(C2:C44)</f>
@@ -1645,15 +1641,15 @@
       </c>
       <c r="M3" s="1">
         <f>AVERAGE(C2:C44)</f>
-        <v>9640.35</v>
+        <v>277.72500000000002</v>
       </c>
       <c r="N3" s="1">
         <f>_xlfn.STDEV.P(C2:C44)</f>
-        <v>44749.010875967972</v>
+        <v>219.83004657007194</v>
       </c>
       <c r="O3" s="1">
         <f>N3/SQRT(COUNT(C2:C44))</f>
-        <v>7075.4398703852676</v>
+        <v>34.758182265115643</v>
       </c>
     </row>
     <row r="4" spans="1:15" x14ac:dyDescent="0.25">
@@ -1723,7 +1719,7 @@
       </c>
       <c r="K5" s="1">
         <f>MAX(E2:E44)</f>
-        <v>6460.2866826054887</v>
+        <v>85.73737956024047</v>
       </c>
       <c r="L5" s="1">
         <f>MIN(E2:E44)</f>
@@ -1731,15 +1727,15 @@
       </c>
       <c r="M5" s="1">
         <f>AVERAGE(E2:E44)</f>
-        <v>282.95981075640901</v>
+        <v>66.725055503063132</v>
       </c>
       <c r="N5" s="1">
         <f>_xlfn.STDEV.P(E2:E44)</f>
-        <v>1013.6381222122596</v>
+        <v>14.144911397330981</v>
       </c>
       <c r="O5" s="1">
         <f>N5/SQRT(COUNT(E2:E44))</f>
-        <v>160.27025946834269</v>
+        <v>2.2365068658420428</v>
       </c>
     </row>
     <row r="6" spans="1:15" x14ac:dyDescent="0.25">
@@ -1747,26 +1743,26 @@
         <v>32</v>
       </c>
       <c r="C6" s="1">
-        <v>2846</v>
+        <v>933</v>
       </c>
       <c r="D6" s="1">
         <v>1</v>
       </c>
       <c r="E6" s="1">
-        <v>80.328371245205631</v>
+        <v>79.794096417581585</v>
       </c>
       <c r="F6" s="1">
-        <v>41.383076905718191</v>
+        <v>29.690620675024672</v>
       </c>
       <c r="G6" s="1">
-        <v>0.25501904116709856</v>
+        <v>0.18300020853452328</v>
       </c>
       <c r="J6" s="2" t="s">
         <v>14</v>
       </c>
       <c r="K6" s="1">
         <f>MAX(F2:F44)</f>
-        <v>33719.839059556762</v>
+        <v>54.106356974901608</v>
       </c>
       <c r="L6" s="1">
         <f>MIN(F2:F44)</f>
@@ -1774,15 +1770,15 @@
       </c>
       <c r="M6" s="1">
         <f>AVERAGE(F2:F44)</f>
-        <v>1094.7188776456906</v>
+        <v>26.499764811363356</v>
       </c>
       <c r="N6" s="1">
         <f>_xlfn.STDEV.P(F2:F44)</f>
-        <v>5283.9381012244676</v>
+        <v>10.825632019278917</v>
       </c>
       <c r="O6" s="1">
         <f>N6/SQRT(COUNT(F2:F44))</f>
-        <v>835.46397076073288</v>
+        <v>1.711682714588461</v>
       </c>
     </row>
     <row r="7" spans="1:15" x14ac:dyDescent="0.25">
@@ -1809,7 +1805,7 @@
       </c>
       <c r="K7" s="1">
         <f>MAX(G2:G44)</f>
-        <v>147.15223214676354</v>
+        <v>12.526589795113582</v>
       </c>
       <c r="L7" s="1">
         <f>MIN(G2:G44)</f>
@@ -1817,15 +1813,15 @@
       </c>
       <c r="M7" s="1">
         <f>AVERAGE(G2:G44)</f>
-        <v>11.797014847219257</v>
+        <v>1.21486614310792</v>
       </c>
       <c r="N7" s="1">
         <f>_xlfn.STDEV.P(G2:G44)</f>
-        <v>31.679794006322577</v>
+        <v>2.4811627586020211</v>
       </c>
       <c r="O7" s="1">
         <f>N7/SQRT(COUNT(G2:G44))</f>
-        <v>5.0090152432465</v>
+        <v>0.39230627813844599</v>
       </c>
     </row>
     <row r="8" spans="1:15" x14ac:dyDescent="0.25">
@@ -1887,13 +1883,11 @@
       <c r="G10" s="1">
         <v>6.0917069553424373E-2</v>
       </c>
-      <c r="K10" s="4" t="s">
-        <v>49</v>
-      </c>
-      <c r="L10" s="4"/>
-      <c r="M10" s="4"/>
-      <c r="N10" s="4"/>
-      <c r="O10" s="4"/>
+      <c r="K10" s="3"/>
+      <c r="L10" s="3"/>
+      <c r="M10" s="3"/>
+      <c r="N10" s="3"/>
+      <c r="O10" s="3"/>
     </row>
     <row r="11" spans="1:15" x14ac:dyDescent="0.25">
       <c r="B11" s="2" t="s">
@@ -1941,7 +1935,7 @@
       </c>
     </row>
     <row r="14" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="B14" s="3" t="s">
+      <c r="B14" s="2" t="s">
         <v>40</v>
       </c>
       <c r="C14" s="1">
@@ -1961,7 +1955,7 @@
       </c>
     </row>
     <row r="15" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="B15" s="3" t="s">
+      <c r="B15" s="2" t="s">
         <v>41</v>
       </c>
       <c r="C15" s="1">
@@ -1981,7 +1975,7 @@
       </c>
     </row>
     <row r="16" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="B16" s="3" t="s">
+      <c r="B16" s="2" t="s">
         <v>42</v>
       </c>
       <c r="C16" s="1">
@@ -2001,7 +1995,7 @@
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B17" s="3" t="s">
+      <c r="B17" s="2" t="s">
         <v>43</v>
       </c>
       <c r="C17" s="1">
@@ -2021,7 +2015,7 @@
       </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B18" s="3" t="s">
+      <c r="B18" s="2" t="s">
         <v>44</v>
       </c>
       <c r="C18" s="1">
@@ -2041,7 +2035,7 @@
       </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B19" s="3" t="s">
+      <c r="B19" s="2" t="s">
         <v>45</v>
       </c>
       <c r="C19" s="1">
@@ -2061,7 +2055,7 @@
       </c>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B20" s="3" t="s">
+      <c r="B20" s="2" t="s">
         <v>46</v>
       </c>
       <c r="C20" s="1">
@@ -2081,7 +2075,7 @@
       </c>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B21" s="3" t="s">
+      <c r="B21" s="2" t="s">
         <v>47</v>
       </c>
       <c r="C21" s="1">
@@ -2101,7 +2095,7 @@
       </c>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B22" s="3" t="s">
+      <c r="B22" s="2" t="s">
         <v>48</v>
       </c>
       <c r="C22" s="1">
@@ -2126,27 +2120,27 @@
       </c>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B24" s="3" t="s">
+      <c r="B24" s="2" t="s">
         <v>17</v>
       </c>
       <c r="C24" s="1">
-        <v>27815</v>
+        <v>544</v>
       </c>
       <c r="D24" s="1">
         <v>18</v>
       </c>
       <c r="E24" s="1">
-        <v>88.188533378477516</v>
+        <v>85.617529205937132</v>
       </c>
       <c r="F24" s="1">
-        <v>252.36128086046429</v>
+        <v>48.583826805518378</v>
       </c>
       <c r="G24" s="1">
-        <v>1.8957392860702631</v>
+        <v>0.36498256238221033</v>
       </c>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B25" s="3" t="s">
+      <c r="B25" s="2" t="s">
         <v>18</v>
       </c>
       <c r="C25" s="1">
@@ -2166,47 +2160,47 @@
       </c>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B26" s="3" t="s">
+      <c r="B26" s="2" t="s">
         <v>19</v>
       </c>
       <c r="C26" s="1">
-        <v>17595</v>
+        <v>124</v>
       </c>
       <c r="D26" s="1">
         <v>25</v>
       </c>
       <c r="E26" s="1">
-        <v>1335.3714585519413</v>
+        <v>66.237556561085967</v>
       </c>
       <c r="F26" s="1">
-        <v>4542.6921305282794</v>
+        <v>20.9204513894251</v>
       </c>
       <c r="G26" s="1">
-        <v>147.15223214676354</v>
+        <v>0.70363092438943098</v>
       </c>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B27" s="3" t="s">
+      <c r="B27" s="2" t="s">
         <v>20</v>
       </c>
       <c r="C27" s="1">
-        <v>7287</v>
+        <v>232</v>
       </c>
       <c r="D27" s="1">
         <v>17</v>
       </c>
       <c r="E27" s="1">
-        <v>107.2191235059761</v>
+        <v>78.5</v>
       </c>
       <c r="F27" s="1">
-        <v>456.09914063553634</v>
+        <v>42.85708809520311</v>
       </c>
       <c r="G27" s="1">
-        <v>28.788722482686836</v>
+        <v>2.7105202452665802</v>
       </c>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B28" s="3" t="s">
+      <c r="B28" s="2" t="s">
         <v>21</v>
       </c>
       <c r="C28" s="1">
@@ -2226,87 +2220,87 @@
       </c>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B29" s="3" t="s">
+      <c r="B29" s="2" t="s">
         <v>22</v>
       </c>
       <c r="C29" s="1">
-        <v>15293</v>
+        <v>479</v>
       </c>
       <c r="D29" s="1">
         <v>23</v>
       </c>
       <c r="E29" s="1">
-        <v>670.00136612021856</v>
+        <v>82.139013452914796</v>
       </c>
       <c r="F29" s="1">
-        <v>2117.1388818592181</v>
+        <v>54.106356974901608</v>
       </c>
       <c r="G29" s="1">
-        <v>78.251704751765729</v>
+        <v>2.0918726153871567</v>
       </c>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B30" s="3" t="s">
+      <c r="B30" s="2" t="s">
         <v>23</v>
       </c>
       <c r="C30" s="1">
-        <v>11185</v>
+        <v>313</v>
       </c>
       <c r="D30" s="1">
         <v>23</v>
       </c>
       <c r="E30" s="1">
-        <v>393.15541264737408</v>
+        <v>66.096956031567075</v>
       </c>
       <c r="F30" s="1">
-        <v>1472.0181050780466</v>
+        <v>32.155654089834329</v>
       </c>
       <c r="G30" s="1">
-        <v>48.191709222758355</v>
+        <v>1.0796811974376637</v>
       </c>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B31" s="3" t="s">
+      <c r="B31" s="2" t="s">
         <v>24</v>
       </c>
       <c r="C31" s="1">
-        <v>3506</v>
+        <v>804</v>
       </c>
       <c r="D31" s="1">
         <v>17</v>
       </c>
       <c r="E31" s="1">
-        <v>107.60232350312779</v>
+        <v>76.958521190261493</v>
       </c>
       <c r="F31" s="1">
-        <v>325.76680699776369</v>
+        <v>44.74458213320132</v>
       </c>
       <c r="G31" s="1">
-        <v>4.8692468525403072</v>
+        <v>0.67180725232909289</v>
       </c>
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B32" s="3" t="s">
+      <c r="B32" s="2" t="s">
         <v>25</v>
       </c>
       <c r="C32" s="1">
-        <v>286809</v>
+        <v>976</v>
       </c>
       <c r="D32" s="1">
         <v>13</v>
       </c>
       <c r="E32" s="1">
-        <v>6460.2866826054887</v>
+        <v>63.415847009140961</v>
       </c>
       <c r="F32" s="1">
-        <v>33719.839059556762</v>
+        <v>46.607155118333665</v>
       </c>
       <c r="G32" s="1">
-        <v>120.24867759878825</v>
+        <v>0.17038075006381415</v>
       </c>
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B33" s="3" t="s">
+      <c r="B33" s="2" t="s">
         <v>26</v>
       </c>
       <c r="C33" s="1">
@@ -2335,19 +2329,19 @@
         <v>1</v>
       </c>
       <c r="C35" s="1">
-        <v>1295</v>
+        <v>397</v>
       </c>
       <c r="D35" s="1">
         <v>17</v>
       </c>
       <c r="E35" s="1">
-        <v>77.332389891696749</v>
+        <v>77.297221580406656</v>
       </c>
       <c r="F35" s="1">
-        <v>27.760053644251826</v>
+        <v>26.978107509501992</v>
       </c>
       <c r="G35" s="1">
-        <v>0.14918508634552002</v>
+        <v>0.14498492942212343</v>
       </c>
     </row>
     <row r="36" spans="1:7" x14ac:dyDescent="0.25">
@@ -2543,7 +2537,7 @@
   <dimension ref="A1:O44"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="M5" sqref="M5"/>
+      <selection activeCell="C35" sqref="C35:G35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2582,13 +2576,13 @@
         <v>0</v>
       </c>
       <c r="E2" s="1">
-        <v>4.2959800782639634</v>
+        <v>4.2965074839629365</v>
       </c>
       <c r="F2" s="1">
-        <v>5.2351922110480738</v>
+        <v>5.2398394967795516</v>
       </c>
       <c r="G2" s="1">
-        <v>6.9821184279642109E-2</v>
+        <v>6.9945399171715536E-2</v>
       </c>
       <c r="K2" s="2" t="s">
         <v>11</v>
@@ -2716,7 +2710,7 @@
       </c>
       <c r="K5" s="1">
         <f>MAX(E2:E44)</f>
-        <v>10.228447653429603</v>
+        <v>10.22851201478743</v>
       </c>
       <c r="L5" s="1">
         <f>MIN(E2:E44)</f>
@@ -2724,15 +2718,15 @@
       </c>
       <c r="M5" s="1">
         <f>AVERAGE(E2:E44)</f>
-        <v>5.5145069795846036</v>
+        <v>5.5395658169460802</v>
       </c>
       <c r="N5" s="1">
         <f>_xlfn.STDEV.P(E2:E44)</f>
-        <v>2.3727053761420933</v>
+        <v>2.365301258664569</v>
       </c>
       <c r="O5" s="1">
         <f>N5/SQRT(COUNT(E2:E44))</f>
-        <v>0.37515766025677766</v>
+        <v>0.37398696649215574</v>
       </c>
     </row>
     <row r="6" spans="1:15" x14ac:dyDescent="0.25">
@@ -2746,13 +2740,13 @@
         <v>0</v>
       </c>
       <c r="E6" s="1">
-        <v>5.0718869859112141</v>
+        <v>5.0697108992136153</v>
       </c>
       <c r="F6" s="1">
-        <v>7.3551453203292096</v>
+        <v>7.3555253130403271</v>
       </c>
       <c r="G6" s="1">
-        <v>4.5325341842231359E-2</v>
+        <v>4.5336292592213584E-2</v>
       </c>
       <c r="J6" s="2" t="s">
         <v>14</v>
@@ -2767,15 +2761,15 @@
       </c>
       <c r="M6" s="1">
         <f>AVERAGE(F2:F44)</f>
-        <v>4.6440710518722419</v>
+        <v>4.638882216466425</v>
       </c>
       <c r="N6" s="1">
         <f>_xlfn.STDEV.P(F2:F44)</f>
-        <v>2.6800342809337989</v>
+        <v>2.6849134287269156</v>
       </c>
       <c r="O6" s="1">
         <f>N6/SQRT(COUNT(F2:F44))</f>
-        <v>0.4237506267541189</v>
+        <v>0.42452208775746053</v>
       </c>
     </row>
     <row r="7" spans="1:15" x14ac:dyDescent="0.25">
@@ -2810,15 +2804,15 @@
       </c>
       <c r="M7" s="1">
         <f>AVERAGE(G2:G44)</f>
-        <v>0.12968813083619316</v>
+        <v>0.12978335127285223</v>
       </c>
       <c r="N7" s="1">
         <f>_xlfn.STDEV.P(G2:G44)</f>
-        <v>0.19869326765208006</v>
+        <v>0.1986873838748909</v>
       </c>
       <c r="O7" s="1">
         <f>N7/SQRT(COUNT(G2:G44))</f>
-        <v>3.1416164076101462E-2</v>
+        <v>3.1415233769243329E-2</v>
       </c>
     </row>
     <row r="8" spans="1:15" x14ac:dyDescent="0.25">
@@ -2932,7 +2926,7 @@
       </c>
     </row>
     <row r="14" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="B14" s="3" t="s">
+      <c r="B14" s="2" t="s">
         <v>40</v>
       </c>
       <c r="C14" s="1">
@@ -2952,7 +2946,7 @@
       </c>
     </row>
     <row r="15" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="B15" s="3" t="s">
+      <c r="B15" s="2" t="s">
         <v>41</v>
       </c>
       <c r="C15" s="1">
@@ -2972,7 +2966,7 @@
       </c>
     </row>
     <row r="16" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="B16" s="3" t="s">
+      <c r="B16" s="2" t="s">
         <v>42</v>
       </c>
       <c r="C16" s="1">
@@ -2992,7 +2986,7 @@
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B17" s="3" t="s">
+      <c r="B17" s="2" t="s">
         <v>43</v>
       </c>
       <c r="C17" s="1">
@@ -3012,7 +3006,7 @@
       </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B18" s="3" t="s">
+      <c r="B18" s="2" t="s">
         <v>44</v>
       </c>
       <c r="C18" s="1">
@@ -3032,7 +3026,7 @@
       </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B19" s="3" t="s">
+      <c r="B19" s="2" t="s">
         <v>45</v>
       </c>
       <c r="C19" s="1">
@@ -3052,7 +3046,7 @@
       </c>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B20" s="3" t="s">
+      <c r="B20" s="2" t="s">
         <v>46</v>
       </c>
       <c r="C20" s="1">
@@ -3072,7 +3066,7 @@
       </c>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B21" s="3" t="s">
+      <c r="B21" s="2" t="s">
         <v>47</v>
       </c>
       <c r="C21" s="1">
@@ -3092,7 +3086,7 @@
       </c>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B22" s="3" t="s">
+      <c r="B22" s="2" t="s">
         <v>48</v>
       </c>
       <c r="C22" s="1">
@@ -3122,7 +3116,7 @@
       <c r="G23" s="1"/>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B24" s="3" t="s">
+      <c r="B24" s="2" t="s">
         <v>17</v>
       </c>
       <c r="C24" s="1">
@@ -3132,17 +3126,17 @@
         <v>0</v>
       </c>
       <c r="E24" s="1">
-        <v>6.9030528751199141</v>
+        <v>6.9038320446977819</v>
       </c>
       <c r="F24" s="1">
-        <v>4.1777789510723577</v>
+        <v>4.1773709170154349</v>
       </c>
       <c r="G24" s="1">
-        <v>3.1383497734125083E-2</v>
+        <v>3.1382203534861076E-2</v>
       </c>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B25" s="3" t="s">
+      <c r="B25" s="2" t="s">
         <v>18</v>
       </c>
       <c r="C25" s="1">
@@ -3162,7 +3156,7 @@
       </c>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B26" s="3" t="s">
+      <c r="B26" s="2" t="s">
         <v>19</v>
       </c>
       <c r="C26" s="1">
@@ -3172,17 +3166,17 @@
         <v>0</v>
       </c>
       <c r="E26" s="1">
-        <v>4.570828961175236</v>
+        <v>4.9276018099547514</v>
       </c>
       <c r="F26" s="1">
-        <v>3.5962947361260311</v>
+        <v>3.4906738247717946</v>
       </c>
       <c r="G26" s="1">
-        <v>0.11649541344045679</v>
+        <v>0.11740406573195188</v>
       </c>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B27" s="3" t="s">
+      <c r="B27" s="2" t="s">
         <v>20</v>
       </c>
       <c r="C27" s="1">
@@ -3192,17 +3186,17 @@
         <v>0</v>
       </c>
       <c r="E27" s="1">
-        <v>4.5577689243027892</v>
+        <v>4.5759999999999996</v>
       </c>
       <c r="F27" s="1">
-        <v>3.3075504293991296</v>
+        <v>3.3015487274913875</v>
       </c>
       <c r="G27" s="1">
-        <v>0.20877073190004661</v>
+        <v>0.20880827569806712</v>
       </c>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B28" s="3" t="s">
+      <c r="B28" s="2" t="s">
         <v>21</v>
       </c>
       <c r="C28" s="1">
@@ -3222,7 +3216,7 @@
       </c>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B29" s="3" t="s">
+      <c r="B29" s="2" t="s">
         <v>22</v>
       </c>
       <c r="C29" s="1">
@@ -3232,17 +3226,17 @@
         <v>0</v>
       </c>
       <c r="E29" s="1">
-        <v>5.2950819672131146</v>
+        <v>5.6591928251121075</v>
       </c>
       <c r="F29" s="1">
-        <v>2.7045454288822612</v>
+        <v>2.4793002424606447</v>
       </c>
       <c r="G29" s="1">
-        <v>9.9962875464636267E-2</v>
+        <v>9.5855285265869478E-2</v>
       </c>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B30" s="3" t="s">
+      <c r="B30" s="2" t="s">
         <v>23</v>
       </c>
       <c r="C30" s="1">
@@ -3252,17 +3246,17 @@
         <v>0</v>
       </c>
       <c r="E30" s="1">
-        <v>4.542336548767417</v>
+        <v>4.5839909808342725</v>
       </c>
       <c r="F30" s="1">
-        <v>3.4733062149070575</v>
+        <v>3.5539794092547603</v>
       </c>
       <c r="G30" s="1">
-        <v>0.11371094049249185</v>
+        <v>0.11933094980848359</v>
       </c>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B31" s="3" t="s">
+      <c r="B31" s="2" t="s">
         <v>24</v>
       </c>
       <c r="C31" s="1">
@@ -3272,17 +3266,17 @@
         <v>0</v>
       </c>
       <c r="E31" s="1">
-        <v>2.0694816800714926</v>
+        <v>2.088142470694319</v>
       </c>
       <c r="F31" s="1">
-        <v>5.7886786519579747</v>
+        <v>5.8113670889284741</v>
       </c>
       <c r="G31" s="1">
-        <v>8.652356440540343E-2</v>
+        <v>8.7253436509172985E-2</v>
       </c>
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B32" s="3" t="s">
+      <c r="B32" s="2" t="s">
         <v>25</v>
       </c>
       <c r="C32" s="1">
@@ -3292,17 +3286,17 @@
         <v>0</v>
       </c>
       <c r="E32" s="1">
-        <v>4.0230180329119722</v>
+        <v>4.2267466723686322</v>
       </c>
       <c r="F32" s="1">
-        <v>4.552282856930983</v>
+        <v>4.5735202024716397</v>
       </c>
       <c r="G32" s="1">
-        <v>1.6233944433564563E-2</v>
+        <v>1.6719317035134778E-2</v>
       </c>
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B33" s="3" t="s">
+      <c r="B33" s="2" t="s">
         <v>26</v>
       </c>
       <c r="C33" s="1">
@@ -3342,13 +3336,13 @@
         <v>0</v>
       </c>
       <c r="E35" s="1">
-        <v>10.228447653429603</v>
+        <v>10.22851201478743</v>
       </c>
       <c r="F35" s="1">
-        <v>7.3360333748465685</v>
+        <v>7.3361295370529866</v>
       </c>
       <c r="G35" s="1">
-        <v>3.9424519364598599E-2</v>
+        <v>3.9425605476090586E-2</v>
       </c>
     </row>
     <row r="36" spans="1:7" x14ac:dyDescent="0.25">
@@ -3540,8 +3534,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AE15F7AD-A0DC-4382-9A54-4AAD142EDBC9}">
   <dimension ref="A1:O44"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L13" sqref="L13"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="J26" sqref="J26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3580,13 +3574,13 @@
         <v>0</v>
       </c>
       <c r="E2" s="1">
-        <v>1.2451085023123443E-3</v>
+        <v>1.2473271560940842E-3</v>
       </c>
       <c r="F2" s="1">
-        <v>3.5264120677110523E-2</v>
+        <v>3.529548598701758E-2</v>
       </c>
       <c r="G2" s="1">
-        <v>4.7031370941070909E-4</v>
+        <v>4.7115123618556541E-4</v>
       </c>
       <c r="K2" s="2" t="s">
         <v>11</v>
@@ -3714,7 +3708,7 @@
       </c>
       <c r="K5" s="1">
         <f>MAX(E2:E44)</f>
-        <v>2.1177390527256481</v>
+        <v>2.1368349864743013</v>
       </c>
       <c r="L5" s="1">
         <f>MIN(E2:E44)</f>
@@ -3722,15 +3716,15 @@
       </c>
       <c r="M5" s="1">
         <f>AVERAGE(E2:E44)</f>
-        <v>0.16388621324234431</v>
+        <v>0.16467610611476191</v>
       </c>
       <c r="N5" s="1">
         <f>_xlfn.STDEV.P(E2:E44)</f>
-        <v>0.52751978115361808</v>
+        <v>0.52927433787707734</v>
       </c>
       <c r="O5" s="1">
         <f>N5/SQRT(COUNT(E2:E44))</f>
-        <v>8.3408200961949938E-2</v>
+        <v>8.3685620738454619E-2</v>
       </c>
     </row>
     <row r="6" spans="1:15" x14ac:dyDescent="0.25">
@@ -3757,7 +3751,7 @@
       </c>
       <c r="K6" s="1">
         <f>MAX(F2:F44)</f>
-        <v>1.750459630640391</v>
+        <v>1.7466921696279536</v>
       </c>
       <c r="L6" s="1">
         <f>MIN(F2:F44)</f>
@@ -3765,15 +3759,15 @@
       </c>
       <c r="M6" s="1">
         <f>AVERAGE(F2:F44)</f>
-        <v>0.13726296689999579</v>
+        <v>0.13758902505641976</v>
       </c>
       <c r="N6" s="1">
         <f>_xlfn.STDEV.P(F2:F44)</f>
-        <v>0.36541437714456365</v>
+        <v>0.36520258887600243</v>
       </c>
       <c r="O6" s="1">
         <f>N6/SQRT(COUNT(F2:F44))</f>
-        <v>5.7777086077429818E-2</v>
+        <v>5.7743599411911976E-2</v>
       </c>
     </row>
     <row r="7" spans="1:15" x14ac:dyDescent="0.25">
@@ -3808,15 +3802,15 @@
       </c>
       <c r="M7" s="1">
         <f>AVERAGE(G2:G44)</f>
-        <v>2.1801813937845005E-3</v>
+        <v>2.2028238529402367E-3</v>
       </c>
       <c r="N7" s="1">
         <f>_xlfn.STDEV.P(G2:G44)</f>
-        <v>6.7488251283324124E-3</v>
+        <v>6.7820694223171656E-3</v>
       </c>
       <c r="O7" s="1">
         <f>N7/SQRT(COUNT(G2:G44))</f>
-        <v>1.0670829467854291E-3</v>
+        <v>1.0723393311952319E-3</v>
       </c>
     </row>
     <row r="8" spans="1:15" x14ac:dyDescent="0.25">
@@ -3930,7 +3924,7 @@
       </c>
     </row>
     <row r="14" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="B14" s="3" t="s">
+      <c r="B14" s="2" t="s">
         <v>40</v>
       </c>
       <c r="C14" s="1">
@@ -3950,7 +3944,7 @@
       </c>
     </row>
     <row r="15" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="B15" s="3" t="s">
+      <c r="B15" s="2" t="s">
         <v>41</v>
       </c>
       <c r="C15" s="1">
@@ -3970,7 +3964,7 @@
       </c>
     </row>
     <row r="16" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="B16" s="3" t="s">
+      <c r="B16" s="2" t="s">
         <v>42</v>
       </c>
       <c r="C16" s="1">
@@ -3990,7 +3984,7 @@
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B17" s="3" t="s">
+      <c r="B17" s="2" t="s">
         <v>43</v>
       </c>
       <c r="C17" s="1">
@@ -4010,7 +4004,7 @@
       </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B18" s="3" t="s">
+      <c r="B18" s="2" t="s">
         <v>44</v>
       </c>
       <c r="C18" s="1">
@@ -4030,7 +4024,7 @@
       </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B19" s="3" t="s">
+      <c r="B19" s="2" t="s">
         <v>45</v>
       </c>
       <c r="C19" s="1">
@@ -4050,7 +4044,7 @@
       </c>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B20" s="3" t="s">
+      <c r="B20" s="2" t="s">
         <v>46</v>
       </c>
       <c r="C20" s="1">
@@ -4070,7 +4064,7 @@
       </c>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B21" s="3" t="s">
+      <c r="B21" s="2" t="s">
         <v>47</v>
       </c>
       <c r="C21" s="1">
@@ -4090,7 +4084,7 @@
       </c>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B22" s="3" t="s">
+      <c r="B22" s="2" t="s">
         <v>48</v>
       </c>
       <c r="C22" s="1">
@@ -4120,7 +4114,7 @@
       <c r="G23" s="1"/>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B24" s="3" t="s">
+      <c r="B24" s="2" t="s">
         <v>17</v>
       </c>
       <c r="C24" s="1">
@@ -4140,7 +4134,7 @@
       </c>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B25" s="3" t="s">
+      <c r="B25" s="2" t="s">
         <v>18</v>
       </c>
       <c r="C25" s="1">
@@ -4160,7 +4154,7 @@
       </c>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B26" s="3" t="s">
+      <c r="B26" s="2" t="s">
         <v>19</v>
       </c>
       <c r="C26" s="1">
@@ -4170,17 +4164,17 @@
         <v>0</v>
       </c>
       <c r="E26" s="1">
-        <v>0.14060860440713535</v>
+        <v>0.15158371040723981</v>
       </c>
       <c r="F26" s="1">
-        <v>0.3476173539595126</v>
+        <v>0.35861691140604879</v>
       </c>
       <c r="G26" s="1">
-        <v>1.1260430620937812E-2</v>
+        <v>1.2061591988491745E-2</v>
       </c>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B27" s="3" t="s">
+      <c r="B27" s="2" t="s">
         <v>20</v>
       </c>
       <c r="C27" s="1">
@@ -4200,7 +4194,7 @@
       </c>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B28" s="3" t="s">
+      <c r="B28" s="2" t="s">
         <v>21</v>
       </c>
       <c r="C28" s="1">
@@ -4220,7 +4214,7 @@
       </c>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B29" s="3" t="s">
+      <c r="B29" s="2" t="s">
         <v>22</v>
       </c>
       <c r="C29" s="1">
@@ -4240,7 +4234,7 @@
       </c>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B30" s="3" t="s">
+      <c r="B30" s="2" t="s">
         <v>23</v>
       </c>
       <c r="C30" s="1">
@@ -4260,7 +4254,7 @@
       </c>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B31" s="3" t="s">
+      <c r="B31" s="2" t="s">
         <v>24</v>
       </c>
       <c r="C31" s="1">
@@ -4270,17 +4264,17 @@
         <v>0</v>
       </c>
       <c r="E31" s="1">
-        <v>2.1177390527256481</v>
+        <v>2.1368349864743013</v>
       </c>
       <c r="F31" s="1">
-        <v>1.750459630640391</v>
+        <v>1.7466921696279536</v>
       </c>
       <c r="G31" s="1">
-        <v>2.6164175919411899E-2</v>
+        <v>2.6225308432856777E-2</v>
       </c>
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B32" s="3" t="s">
+      <c r="B32" s="2" t="s">
         <v>25</v>
       </c>
       <c r="C32" s="1">
@@ -4290,17 +4284,17 @@
         <v>0</v>
       </c>
       <c r="E32" s="1">
-        <v>3.1246025892107739E-2</v>
+        <v>3.2768482386272516E-2</v>
       </c>
       <c r="F32" s="1">
-        <v>0.23938747371298078</v>
+        <v>0.24516633822593475</v>
       </c>
       <c r="G32" s="1">
-        <v>8.5368222241090981E-4</v>
+        <v>8.9624918086669446E-4</v>
       </c>
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B33" s="3" t="s">
+      <c r="B33" s="2" t="s">
         <v>26</v>
       </c>
       <c r="C33" s="1">

</xml_diff>

<commit_message>
Changed to STDEV.S for cpp files
</commit_message>
<xml_diff>
--- a/results/overall.xlsx
+++ b/results/overall.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10211"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2D0070BC-B6F2-4749-AB88-2E63EC4597BC}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5EBBA449-DAE3-8740-B967-24F6D9B34482}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="960" yWindow="460" windowWidth="27840" windowHeight="17540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Length" sheetId="1" r:id="rId1"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="236" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="247" uniqueCount="50">
   <si>
     <t>Python</t>
   </si>
@@ -176,6 +176,9 @@
   </si>
   <si>
     <t>spring-framework</t>
+  </si>
+  <si>
+    <t>CPP</t>
   </si>
 </sst>
 </file>
@@ -248,13 +251,14 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Calculation" xfId="1" builtinId="22"/>
@@ -539,22 +543,22 @@
   <dimension ref="A1:O44"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J11" sqref="J10:J11"/>
+      <selection activeCell="J18" sqref="J18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="9.5703125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="20.85546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="9.5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="20.83203125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="6" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="4.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="4.83203125" bestFit="1" customWidth="1"/>
     <col min="5" max="7" width="12" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="9" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="11" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="12" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
         <v>27</v>
       </c>
@@ -575,7 +579,7 @@
       </c>
       <c r="J1" s="2"/>
     </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:15" x14ac:dyDescent="0.2">
       <c r="B2" s="2" t="s">
         <v>28</v>
       </c>
@@ -610,7 +614,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:15" x14ac:dyDescent="0.2">
       <c r="B3" s="2" t="s">
         <v>29</v>
       </c>
@@ -645,15 +649,15 @@
         <v>2032.675</v>
       </c>
       <c r="N3" s="1">
-        <f>_xlfn.STDEV.P(C2:C44)</f>
-        <v>3580.3960631995728</v>
+        <f>_xlfn.STDEV.S(C2:C44)</f>
+        <v>3626.0080429535869</v>
       </c>
       <c r="O3" s="1">
         <f>N3/SQRT(COUNT(C2:C44))</f>
-        <v>566.11032426054112</v>
-      </c>
-    </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
+        <v>573.32221149114957</v>
+      </c>
+    </row>
+    <row r="4" spans="1:15" x14ac:dyDescent="0.2">
       <c r="B4" s="2" t="s">
         <v>30</v>
       </c>
@@ -688,15 +692,15 @@
         <v>2.0499999999999998</v>
       </c>
       <c r="N4" s="1">
-        <f>_xlfn.STDEV.P(D2:D44)</f>
-        <v>4.0555517503787328</v>
+        <f>_xlfn.STDEV.S(D2:D44)</f>
+        <v>4.1072169128536133</v>
       </c>
       <c r="O4" s="1">
         <f>N4/SQRT(COUNT(D2:D44))</f>
-        <v>0.64123903499397172</v>
-      </c>
-    </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
+        <v>0.64940801444913587</v>
+      </c>
+    </row>
+    <row r="5" spans="1:15" x14ac:dyDescent="0.2">
       <c r="B5" s="2" t="s">
         <v>31</v>
       </c>
@@ -731,15 +735,15 @@
         <v>30.199290061247517</v>
       </c>
       <c r="N5" s="1">
-        <f>_xlfn.STDEV.P(E2:E44)</f>
-        <v>77.172847802762647</v>
+        <f>_xlfn.STDEV.S(E2:E44)</f>
+        <v>78.15598103981398</v>
       </c>
       <c r="O5" s="1">
         <f>N5/SQRT(COUNT(E2:E44))</f>
-        <v>12.202098628912536</v>
-      </c>
-    </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
+        <v>12.357545642537358</v>
+      </c>
+    </row>
+    <row r="6" spans="1:15" x14ac:dyDescent="0.2">
       <c r="B6" s="2" t="s">
         <v>32</v>
       </c>
@@ -774,15 +778,15 @@
         <v>78.289419644954336</v>
       </c>
       <c r="N6" s="1">
-        <f>_xlfn.STDEV.P(F2:F44)</f>
-        <v>218.85146779379858</v>
+        <f>_xlfn.STDEV.S(F2:F44)</f>
+        <v>221.63949697882299</v>
       </c>
       <c r="O6" s="1">
         <f>N6/SQRT(COUNT(F2:F44))</f>
-        <v>34.603455374969435</v>
-      </c>
-    </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
+        <v>35.044281495354447</v>
+      </c>
+    </row>
+    <row r="7" spans="1:15" x14ac:dyDescent="0.2">
       <c r="B7" s="2" t="s">
         <v>33</v>
       </c>
@@ -817,15 +821,15 @@
         <v>1.9930877888506167</v>
       </c>
       <c r="N7" s="1">
-        <f>_xlfn.STDEV.P(G2:G44)</f>
-        <v>6.2937306934318134</v>
+        <f>_xlfn.STDEV.S(G2:G44)</f>
+        <v>6.3739088390611816</v>
       </c>
       <c r="O7" s="1">
         <f>N7/SQRT(COUNT(G2:G44))</f>
-        <v>0.99512619854777329</v>
-      </c>
-    </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
+        <v>1.0078034764856472</v>
+      </c>
+    </row>
+    <row r="8" spans="1:15" x14ac:dyDescent="0.2">
       <c r="B8" s="2" t="s">
         <v>34</v>
       </c>
@@ -845,7 +849,7 @@
         <v>0.25744513071085023</v>
       </c>
     </row>
-    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:15" x14ac:dyDescent="0.2">
       <c r="B9" s="2" t="s">
         <v>35</v>
       </c>
@@ -865,7 +869,7 @@
         <v>0.28847113143317576</v>
       </c>
     </row>
-    <row r="10" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:15" x14ac:dyDescent="0.2">
       <c r="B10" s="2" t="s">
         <v>36</v>
       </c>
@@ -884,8 +888,11 @@
       <c r="G10" s="1">
         <v>0.23710295140328733</v>
       </c>
-    </row>
-    <row r="11" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="J10" s="4" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="11" spans="1:15" x14ac:dyDescent="0.2">
       <c r="B11" s="2" t="s">
         <v>37</v>
       </c>
@@ -904,8 +911,23 @@
       <c r="G11" s="1">
         <v>0.58020793910761048</v>
       </c>
-    </row>
-    <row r="12" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="K11" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="L11" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="M11" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="N11" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="O11" s="2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="12" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A12" s="2" t="s">
         <v>38</v>
       </c>
@@ -914,8 +936,23 @@
       <c r="E12" s="1"/>
       <c r="F12" s="1"/>
       <c r="G12" s="1"/>
-    </row>
-    <row r="13" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="J12" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="K12">
+        <f>MAX(C2:C11)</f>
+        <v>6888</v>
+      </c>
+      <c r="L12">
+        <f>MIN(C2:C11)</f>
+        <v>178</v>
+      </c>
+      <c r="M12">
+        <f>AVERAGE(C2:C11)</f>
+        <v>2096.9</v>
+      </c>
+    </row>
+    <row r="13" spans="1:15" x14ac:dyDescent="0.2">
       <c r="B13" s="2" t="s">
         <v>39</v>
       </c>
@@ -934,8 +971,11 @@
       <c r="G13" s="1">
         <v>5.3991022431659381E-2</v>
       </c>
-    </row>
-    <row r="14" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="J13" s="2" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="14" spans="1:15" x14ac:dyDescent="0.2">
       <c r="B14" s="2" t="s">
         <v>40</v>
       </c>
@@ -954,8 +994,11 @@
       <c r="G14" s="1">
         <v>4.9755809005011351E-2</v>
       </c>
-    </row>
-    <row r="15" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="J14" s="2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="15" spans="1:15" x14ac:dyDescent="0.2">
       <c r="B15" s="2" t="s">
         <v>41</v>
       </c>
@@ -974,8 +1017,11 @@
       <c r="G15" s="1">
         <v>0.40178060081536426</v>
       </c>
-    </row>
-    <row r="16" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="J15" s="2" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="16" spans="1:15" x14ac:dyDescent="0.2">
       <c r="B16" s="2" t="s">
         <v>42</v>
       </c>
@@ -994,8 +1040,11 @@
       <c r="G16" s="1">
         <v>0.12320918107308468</v>
       </c>
-    </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="J16" s="2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B17" s="2" t="s">
         <v>43</v>
       </c>
@@ -1015,7 +1064,7 @@
         <v>0.50606759321841865</v>
       </c>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B18" s="2" t="s">
         <v>44</v>
       </c>
@@ -1035,7 +1084,7 @@
         <v>0.16556719384585963</v>
       </c>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B19" s="2" t="s">
         <v>45</v>
       </c>
@@ -1055,7 +1104,7 @@
         <v>0.35099135344384824</v>
       </c>
     </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B20" s="2" t="s">
         <v>46</v>
       </c>
@@ -1075,7 +1124,7 @@
         <v>9.1826797264275228E-2</v>
       </c>
     </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B21" s="2" t="s">
         <v>47</v>
       </c>
@@ -1095,7 +1144,7 @@
         <v>3.1390013331077431E-2</v>
       </c>
     </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B22" s="2" t="s">
         <v>48</v>
       </c>
@@ -1115,7 +1164,7 @@
         <v>4.6267886526358687E-2</v>
       </c>
     </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A23" s="2" t="s">
         <v>16</v>
       </c>
@@ -1125,7 +1174,7 @@
       <c r="F23" s="1"/>
       <c r="G23" s="1"/>
     </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B24" s="2" t="s">
         <v>17</v>
       </c>
@@ -1145,7 +1194,7 @@
         <v>1.2400602963634322</v>
       </c>
     </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B25" s="2" t="s">
         <v>18</v>
       </c>
@@ -1165,7 +1214,7 @@
         <v>40.258357430161986</v>
       </c>
     </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B26" s="2" t="s">
         <v>19</v>
       </c>
@@ -1185,7 +1234,7 @@
         <v>2.2176143628772422</v>
       </c>
     </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B27" s="2" t="s">
         <v>20</v>
       </c>
@@ -1205,7 +1254,7 @@
         <v>4.3944898516210049</v>
       </c>
     </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B28" s="2" t="s">
         <v>21</v>
       </c>
@@ -1225,7 +1274,7 @@
         <v>0.98270364158678503</v>
       </c>
     </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B29" s="2" t="s">
         <v>22</v>
       </c>
@@ -1245,7 +1294,7 @@
         <v>2.4801895136795258</v>
       </c>
     </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B30" s="2" t="s">
         <v>23</v>
       </c>
@@ -1265,7 +1314,7 @@
         <v>1.8439513932942531</v>
       </c>
     </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B31" s="2" t="s">
         <v>24</v>
       </c>
@@ -1285,7 +1334,7 @@
         <v>2.9614054075571348</v>
       </c>
     </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B32" s="2" t="s">
         <v>25</v>
       </c>
@@ -1305,7 +1354,7 @@
         <v>0.62648991469281545</v>
       </c>
     </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B33" s="2" t="s">
         <v>26</v>
       </c>
@@ -1325,7 +1374,7 @@
         <v>4.9545019960785748</v>
       </c>
     </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A34" s="2" t="s">
         <v>0</v>
       </c>
@@ -1335,7 +1384,7 @@
       <c r="F34" s="1"/>
       <c r="G34" s="1"/>
     </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B35" s="2" t="s">
         <v>1</v>
       </c>
@@ -1355,7 +1404,7 @@
         <v>0.15603427483907159</v>
       </c>
     </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B36" s="2" t="s">
         <v>2</v>
       </c>
@@ -1375,7 +1424,7 @@
         <v>2.1213203435596424</v>
       </c>
     </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B37" s="2" t="s">
         <v>3</v>
       </c>
@@ -1395,7 +1444,7 @@
         <v>8.9500968392268287E-2</v>
       </c>
     </row>
-    <row r="38" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B38" s="2" t="s">
         <v>4</v>
       </c>
@@ -1415,7 +1464,7 @@
         <v>0.64753879116162472</v>
       </c>
     </row>
-    <row r="39" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B39" s="2" t="s">
         <v>5</v>
       </c>
@@ -1435,7 +1484,7 @@
         <v>0.43027925242772791</v>
       </c>
     </row>
-    <row r="40" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B40" s="2" t="s">
         <v>6</v>
       </c>
@@ -1455,7 +1504,7 @@
         <v>6.6231328850346936</v>
       </c>
     </row>
-    <row r="41" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B41" s="2" t="s">
         <v>7</v>
       </c>
@@ -1475,7 +1524,7 @@
         <v>0.52092183578955342</v>
       </c>
     </row>
-    <row r="42" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B42" s="2" t="s">
         <v>8</v>
       </c>
@@ -1495,7 +1544,7 @@
         <v>0.32010577816968244</v>
       </c>
     </row>
-    <row r="43" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B43" s="2" t="s">
         <v>9</v>
       </c>
@@ -1515,7 +1564,7 @@
         <v>0.15434369966651265</v>
       </c>
     </row>
-    <row r="44" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B44" s="2" t="s">
         <v>10</v>
       </c>
@@ -1549,12 +1598,12 @@
       <selection activeCell="L18" sqref="L18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" width="20.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="20.83203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
         <v>27</v>
       </c>
@@ -1574,7 +1623,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:15" x14ac:dyDescent="0.2">
       <c r="B2" s="2" t="s">
         <v>28</v>
       </c>
@@ -1609,7 +1658,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:15" x14ac:dyDescent="0.2">
       <c r="B3" s="2" t="s">
         <v>29</v>
       </c>
@@ -1652,7 +1701,7 @@
         <v>34.758182265115643</v>
       </c>
     </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:15" x14ac:dyDescent="0.2">
       <c r="B4" s="2" t="s">
         <v>30</v>
       </c>
@@ -1695,7 +1744,7 @@
         <v>0.90407929685398725</v>
       </c>
     </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:15" x14ac:dyDescent="0.2">
       <c r="B5" s="2" t="s">
         <v>31</v>
       </c>
@@ -1738,7 +1787,7 @@
         <v>2.2365068658420428</v>
       </c>
     </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:15" x14ac:dyDescent="0.2">
       <c r="B6" s="2" t="s">
         <v>32</v>
       </c>
@@ -1781,7 +1830,7 @@
         <v>1.711682714588461</v>
       </c>
     </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:15" x14ac:dyDescent="0.2">
       <c r="B7" s="2" t="s">
         <v>33</v>
       </c>
@@ -1824,7 +1873,7 @@
         <v>0.39230627813844599</v>
       </c>
     </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:15" x14ac:dyDescent="0.2">
       <c r="B8" s="2" t="s">
         <v>34</v>
       </c>
@@ -1844,7 +1893,7 @@
         <v>0.19875685521859038</v>
       </c>
     </row>
-    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:15" x14ac:dyDescent="0.2">
       <c r="B9" s="2" t="s">
         <v>35</v>
       </c>
@@ -1864,7 +1913,7 @@
         <v>7.775831657130669E-2</v>
       </c>
     </row>
-    <row r="10" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:15" x14ac:dyDescent="0.2">
       <c r="B10" s="2" t="s">
         <v>36</v>
       </c>
@@ -1889,7 +1938,7 @@
       <c r="N10" s="3"/>
       <c r="O10" s="3"/>
     </row>
-    <row r="11" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:15" x14ac:dyDescent="0.2">
       <c r="B11" s="2" t="s">
         <v>37</v>
       </c>
@@ -1909,12 +1958,12 @@
         <v>0.53234537666580184</v>
       </c>
     </row>
-    <row r="12" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A12" s="2" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="13" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:15" x14ac:dyDescent="0.2">
       <c r="B13" s="2" t="s">
         <v>39</v>
       </c>
@@ -1934,7 +1983,7 @@
         <v>0.10737451815753295</v>
       </c>
     </row>
-    <row r="14" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:15" x14ac:dyDescent="0.2">
       <c r="B14" s="2" t="s">
         <v>40</v>
       </c>
@@ -1954,7 +2003,7 @@
         <v>0.11837618451144184</v>
       </c>
     </row>
-    <row r="15" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:15" x14ac:dyDescent="0.2">
       <c r="B15" s="2" t="s">
         <v>41</v>
       </c>
@@ -1974,7 +2023,7 @@
         <v>0.91629630447740862</v>
       </c>
     </row>
-    <row r="16" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:15" x14ac:dyDescent="0.2">
       <c r="B16" s="2" t="s">
         <v>42</v>
       </c>
@@ -1994,7 +2043,7 @@
         <v>0.43733539244157782</v>
       </c>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B17" s="2" t="s">
         <v>43</v>
       </c>
@@ -2014,7 +2063,7 @@
         <v>0.62828231212416652</v>
       </c>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B18" s="2" t="s">
         <v>44</v>
       </c>
@@ -2034,7 +2083,7 @@
         <v>0.26708974016357978</v>
       </c>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B19" s="2" t="s">
         <v>45</v>
       </c>
@@ -2054,7 +2103,7 @@
         <v>0.50776015099578575</v>
       </c>
     </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B20" s="2" t="s">
         <v>46</v>
       </c>
@@ -2074,7 +2123,7 @@
         <v>0.18511170430852586</v>
       </c>
     </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B21" s="2" t="s">
         <v>47</v>
       </c>
@@ -2094,7 +2143,7 @@
         <v>0.11152679658524194</v>
       </c>
     </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B22" s="2" t="s">
         <v>48</v>
       </c>
@@ -2114,12 +2163,12 @@
         <v>0.1030004424178271</v>
       </c>
     </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A23" s="2" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B24" s="2" t="s">
         <v>17</v>
       </c>
@@ -2139,7 +2188,7 @@
         <v>0.36498256238221033</v>
       </c>
     </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B25" s="2" t="s">
         <v>18</v>
       </c>
@@ -2159,7 +2208,7 @@
         <v>1.1456694455808718</v>
       </c>
     </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B26" s="2" t="s">
         <v>19</v>
       </c>
@@ -2179,7 +2228,7 @@
         <v>0.70363092438943098</v>
       </c>
     </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B27" s="2" t="s">
         <v>20</v>
       </c>
@@ -2199,7 +2248,7 @@
         <v>2.7105202452665802</v>
       </c>
     </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B28" s="2" t="s">
         <v>21</v>
       </c>
@@ -2219,7 +2268,7 @@
         <v>8.0988407102794735</v>
       </c>
     </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B29" s="2" t="s">
         <v>22</v>
       </c>
@@ -2239,7 +2288,7 @@
         <v>2.0918726153871567</v>
       </c>
     </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B30" s="2" t="s">
         <v>23</v>
       </c>
@@ -2259,7 +2308,7 @@
         <v>1.0796811974376637</v>
       </c>
     </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B31" s="2" t="s">
         <v>24</v>
       </c>
@@ -2279,7 +2328,7 @@
         <v>0.67180725232909289</v>
       </c>
     </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B32" s="2" t="s">
         <v>25</v>
       </c>
@@ -2299,7 +2348,7 @@
         <v>0.17038075006381415</v>
       </c>
     </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B33" s="2" t="s">
         <v>26</v>
       </c>
@@ -2319,12 +2368,12 @@
         <v>0.34351242759909445</v>
       </c>
     </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A34" s="2" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B35" s="2" t="s">
         <v>1</v>
       </c>
@@ -2344,7 +2393,7 @@
         <v>0.14498492942212343</v>
       </c>
     </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B36" s="2" t="s">
         <v>2</v>
       </c>
@@ -2364,7 +2413,7 @@
         <v>7.7781745930520225</v>
       </c>
     </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B37" s="2" t="s">
         <v>3</v>
       </c>
@@ -2384,7 +2433,7 @@
         <v>0.14181023815212646</v>
       </c>
     </row>
-    <row r="38" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B38" s="2" t="s">
         <v>4</v>
       </c>
@@ -2404,7 +2453,7 @@
         <v>0.84316122886250799</v>
       </c>
     </row>
-    <row r="39" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B39" s="2" t="s">
         <v>5</v>
       </c>
@@ -2424,7 +2473,7 @@
         <v>0.34846214329364755</v>
       </c>
     </row>
-    <row r="40" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B40" s="2" t="s">
         <v>6</v>
       </c>
@@ -2444,7 +2493,7 @@
         <v>12.526589795113582</v>
       </c>
     </row>
-    <row r="41" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B41" s="2" t="s">
         <v>7</v>
       </c>
@@ -2464,7 +2513,7 @@
         <v>0.76817892369895147</v>
       </c>
     </row>
-    <row r="42" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B42" s="2" t="s">
         <v>8</v>
       </c>
@@ -2484,7 +2533,7 @@
         <v>1.3729595463875914</v>
       </c>
     </row>
-    <row r="43" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B43" s="2" t="s">
         <v>9</v>
       </c>
@@ -2504,7 +2553,7 @@
         <v>0.51015054494418899</v>
       </c>
     </row>
-    <row r="44" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B44" s="2" t="s">
         <v>10</v>
       </c>
@@ -2540,12 +2589,12 @@
       <selection activeCell="C35" sqref="C35:G35"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" width="20.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="20.83203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
         <v>27</v>
       </c>
@@ -2565,7 +2614,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:15" x14ac:dyDescent="0.2">
       <c r="B2" s="2" t="s">
         <v>28</v>
       </c>
@@ -2600,7 +2649,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:15" x14ac:dyDescent="0.2">
       <c r="B3" s="2" t="s">
         <v>29</v>
       </c>
@@ -2643,7 +2692,7 @@
         <v>5.2903154442811813</v>
       </c>
     </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:15" x14ac:dyDescent="0.2">
       <c r="B4" s="2" t="s">
         <v>30</v>
       </c>
@@ -2686,7 +2735,7 @@
         <v>0.17606816861659008</v>
       </c>
     </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:15" x14ac:dyDescent="0.2">
       <c r="B5" s="2" t="s">
         <v>31</v>
       </c>
@@ -2729,7 +2778,7 @@
         <v>0.37398696649215574</v>
       </c>
     </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:15" x14ac:dyDescent="0.2">
       <c r="B6" s="2" t="s">
         <v>32</v>
       </c>
@@ -2772,7 +2821,7 @@
         <v>0.42452208775746053</v>
       </c>
     </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:15" x14ac:dyDescent="0.2">
       <c r="B7" s="2" t="s">
         <v>33</v>
       </c>
@@ -2815,7 +2864,7 @@
         <v>3.1415233769243329E-2</v>
       </c>
     </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:15" x14ac:dyDescent="0.2">
       <c r="B8" s="2" t="s">
         <v>34</v>
       </c>
@@ -2835,7 +2884,7 @@
         <v>7.7762774327540848E-2</v>
       </c>
     </row>
-    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:15" x14ac:dyDescent="0.2">
       <c r="B9" s="2" t="s">
         <v>35</v>
       </c>
@@ -2855,7 +2904,7 @@
         <v>7.8410817433920935E-2</v>
       </c>
     </row>
-    <row r="10" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:15" x14ac:dyDescent="0.2">
       <c r="B10" s="2" t="s">
         <v>36</v>
       </c>
@@ -2875,7 +2924,7 @@
         <v>4.7874452915207498E-2</v>
       </c>
     </row>
-    <row r="11" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:15" x14ac:dyDescent="0.2">
       <c r="B11" s="2" t="s">
         <v>37</v>
       </c>
@@ -2895,7 +2944,7 @@
         <v>6.7832591331493622E-2</v>
       </c>
     </row>
-    <row r="12" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A12" s="2" t="s">
         <v>38</v>
       </c>
@@ -2905,7 +2954,7 @@
       <c r="F12" s="1"/>
       <c r="G12" s="1"/>
     </row>
-    <row r="13" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:15" x14ac:dyDescent="0.2">
       <c r="B13" s="2" t="s">
         <v>39</v>
       </c>
@@ -2925,7 +2974,7 @@
         <v>2.0028808934777147E-2</v>
       </c>
     </row>
-    <row r="14" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:15" x14ac:dyDescent="0.2">
       <c r="B14" s="2" t="s">
         <v>40</v>
       </c>
@@ -2945,7 +2994,7 @@
         <v>1.0934518376390015E-2</v>
       </c>
     </row>
-    <row r="15" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:15" x14ac:dyDescent="0.2">
       <c r="B15" s="2" t="s">
         <v>41</v>
       </c>
@@ -2965,7 +3014,7 @@
         <v>0.19959239949754212</v>
       </c>
     </row>
-    <row r="16" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:15" x14ac:dyDescent="0.2">
       <c r="B16" s="2" t="s">
         <v>42</v>
       </c>
@@ -2985,7 +3034,7 @@
         <v>3.7085236505680616E-2</v>
       </c>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B17" s="2" t="s">
         <v>43</v>
       </c>
@@ -3005,7 +3054,7 @@
         <v>0.1057778909528467</v>
       </c>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B18" s="2" t="s">
         <v>44</v>
       </c>
@@ -3025,7 +3074,7 @@
         <v>3.2829418236729496E-2</v>
       </c>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B19" s="2" t="s">
         <v>45</v>
       </c>
@@ -3045,7 +3094,7 @@
         <v>6.6104363732220284E-2</v>
       </c>
     </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B20" s="2" t="s">
         <v>46</v>
       </c>
@@ -3065,7 +3114,7 @@
         <v>2.9842438598646541E-2</v>
       </c>
     </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B21" s="2" t="s">
         <v>47</v>
       </c>
@@ -3085,7 +3134,7 @@
         <v>2.2007983243639502E-4</v>
       </c>
     </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B22" s="2" t="s">
         <v>48</v>
       </c>
@@ -3105,7 +3154,7 @@
         <v>2.367081956829979E-3</v>
       </c>
     </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A23" s="2" t="s">
         <v>16</v>
       </c>
@@ -3115,7 +3164,7 @@
       <c r="F23" s="1"/>
       <c r="G23" s="1"/>
     </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B24" s="2" t="s">
         <v>17</v>
       </c>
@@ -3135,7 +3184,7 @@
         <v>3.1382203534861076E-2</v>
       </c>
     </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B25" s="2" t="s">
         <v>18</v>
       </c>
@@ -3155,7 +3204,7 @@
         <v>8.7023245216123785E-2</v>
       </c>
     </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B26" s="2" t="s">
         <v>19</v>
       </c>
@@ -3175,7 +3224,7 @@
         <v>0.11740406573195188</v>
       </c>
     </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B27" s="2" t="s">
         <v>20</v>
       </c>
@@ -3195,7 +3244,7 @@
         <v>0.20880827569806712</v>
       </c>
     </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B28" s="2" t="s">
         <v>21</v>
       </c>
@@ -3215,7 +3264,7 @@
         <v>0.87645626416290601</v>
       </c>
     </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B29" s="2" t="s">
         <v>22</v>
       </c>
@@ -3235,7 +3284,7 @@
         <v>9.5855285265869478E-2</v>
       </c>
     </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B30" s="2" t="s">
         <v>23</v>
       </c>
@@ -3255,7 +3304,7 @@
         <v>0.11933094980848359</v>
       </c>
     </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B31" s="2" t="s">
         <v>24</v>
       </c>
@@ -3275,7 +3324,7 @@
         <v>8.7253436509172985E-2</v>
       </c>
     </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B32" s="2" t="s">
         <v>25</v>
       </c>
@@ -3295,7 +3344,7 @@
         <v>1.6719317035134778E-2</v>
       </c>
     </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B33" s="2" t="s">
         <v>26</v>
       </c>
@@ -3315,7 +3364,7 @@
         <v>6.1809073430821614E-2</v>
       </c>
     </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A34" s="2" t="s">
         <v>0</v>
       </c>
@@ -3325,7 +3374,7 @@
       <c r="F34" s="1"/>
       <c r="G34" s="1"/>
     </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B35" s="2" t="s">
         <v>1</v>
       </c>
@@ -3345,7 +3394,7 @@
         <v>3.9425605476090586E-2</v>
       </c>
     </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B36" s="2" t="s">
         <v>2</v>
       </c>
@@ -3365,7 +3414,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B37" s="2" t="s">
         <v>3</v>
       </c>
@@ -3385,7 +3434,7 @@
         <v>2.5333613617020082E-2</v>
       </c>
     </row>
-    <row r="38" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B38" s="2" t="s">
         <v>4</v>
       </c>
@@ -3405,7 +3454,7 @@
         <v>0.23416783029956437</v>
       </c>
     </row>
-    <row r="39" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B39" s="2" t="s">
         <v>5</v>
       </c>
@@ -3425,7 +3474,7 @@
         <v>0.13944384181171246</v>
       </c>
     </row>
-    <row r="40" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B40" s="2" t="s">
         <v>6</v>
       </c>
@@ -3445,7 +3494,7 @@
         <v>1.0101525445522106</v>
       </c>
     </row>
-    <row r="41" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B41" s="2" t="s">
         <v>7</v>
       </c>
@@ -3465,7 +3514,7 @@
         <v>0.13285079880130551</v>
       </c>
     </row>
-    <row r="42" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B42" s="2" t="s">
         <v>8</v>
       </c>
@@ -3485,7 +3534,7 @@
         <v>0.22885796869230571</v>
       </c>
     </row>
-    <row r="43" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B43" s="2" t="s">
         <v>9</v>
       </c>
@@ -3505,7 +3554,7 @@
         <v>0.14877455780064802</v>
       </c>
     </row>
-    <row r="44" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B44" s="2" t="s">
         <v>10</v>
       </c>
@@ -3538,12 +3587,12 @@
       <selection activeCell="J26" sqref="J26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" width="20.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="20.83203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
         <v>27</v>
       </c>
@@ -3563,7 +3612,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:15" x14ac:dyDescent="0.2">
       <c r="B2" s="2" t="s">
         <v>28</v>
       </c>
@@ -3598,7 +3647,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:15" x14ac:dyDescent="0.2">
       <c r="B3" s="2" t="s">
         <v>29</v>
       </c>
@@ -3641,7 +3690,7 @@
         <v>0.49598387070548977</v>
       </c>
     </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:15" x14ac:dyDescent="0.2">
       <c r="B4" s="2" t="s">
         <v>30</v>
       </c>
@@ -3684,7 +3733,7 @@
         <v>2.4685522072664372E-2</v>
       </c>
     </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:15" x14ac:dyDescent="0.2">
       <c r="B5" s="2" t="s">
         <v>31</v>
       </c>
@@ -3727,7 +3776,7 @@
         <v>8.3685620738454619E-2</v>
       </c>
     </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:15" x14ac:dyDescent="0.2">
       <c r="B6" s="2" t="s">
         <v>32</v>
       </c>
@@ -3770,7 +3819,7 @@
         <v>5.7743599411911976E-2</v>
       </c>
     </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:15" x14ac:dyDescent="0.2">
       <c r="B7" s="2" t="s">
         <v>33</v>
       </c>
@@ -3813,7 +3862,7 @@
         <v>1.0723393311952319E-3</v>
       </c>
     </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:15" x14ac:dyDescent="0.2">
       <c r="B8" s="2" t="s">
         <v>34</v>
       </c>
@@ -3833,7 +3882,7 @@
         <v>1.3839060006400557E-4</v>
       </c>
     </row>
-    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:15" x14ac:dyDescent="0.2">
       <c r="B9" s="2" t="s">
         <v>35</v>
       </c>
@@ -3853,7 +3902,7 @@
         <v>4.0106683754657913E-5</v>
       </c>
     </row>
-    <row r="10" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:15" x14ac:dyDescent="0.2">
       <c r="B10" s="2" t="s">
         <v>36</v>
       </c>
@@ -3873,7 +3922,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:15" x14ac:dyDescent="0.2">
       <c r="B11" s="2" t="s">
         <v>37</v>
       </c>
@@ -3893,7 +3942,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A12" s="2" t="s">
         <v>38</v>
       </c>
@@ -3903,7 +3952,7 @@
       <c r="F12" s="1"/>
       <c r="G12" s="1"/>
     </row>
-    <row r="13" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:15" x14ac:dyDescent="0.2">
       <c r="B13" s="2" t="s">
         <v>39</v>
       </c>
@@ -3923,7 +3972,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:15" x14ac:dyDescent="0.2">
       <c r="B14" s="2" t="s">
         <v>40</v>
       </c>
@@ -3943,7 +3992,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:15" x14ac:dyDescent="0.2">
       <c r="B15" s="2" t="s">
         <v>41</v>
       </c>
@@ -3963,7 +4012,7 @@
         <v>3.3701282815944256E-2</v>
       </c>
     </row>
-    <row r="16" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:15" x14ac:dyDescent="0.2">
       <c r="B16" s="2" t="s">
         <v>42</v>
       </c>
@@ -3983,7 +4032,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B17" s="2" t="s">
         <v>43</v>
       </c>
@@ -4003,7 +4052,7 @@
         <v>2.0169763773763812E-3</v>
       </c>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B18" s="2" t="s">
         <v>44</v>
       </c>
@@ -4023,7 +4072,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B19" s="2" t="s">
         <v>45</v>
       </c>
@@ -4043,7 +4092,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B20" s="2" t="s">
         <v>46</v>
       </c>
@@ -4063,7 +4112,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B21" s="2" t="s">
         <v>47</v>
       </c>
@@ -4083,7 +4132,7 @@
         <v>6.3143589003309868E-3</v>
       </c>
     </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B22" s="2" t="s">
         <v>48</v>
       </c>
@@ -4103,7 +4152,7 @@
         <v>3.7909099943266027E-3</v>
       </c>
     </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A23" s="2" t="s">
         <v>16</v>
       </c>
@@ -4113,7 +4162,7 @@
       <c r="F23" s="1"/>
       <c r="G23" s="1"/>
     </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B24" s="2" t="s">
         <v>17</v>
       </c>
@@ -4133,7 +4182,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B25" s="2" t="s">
         <v>18</v>
       </c>
@@ -4153,7 +4202,7 @@
         <v>2.3589859607805017E-3</v>
       </c>
     </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B26" s="2" t="s">
         <v>19</v>
       </c>
@@ -4173,7 +4222,7 @@
         <v>1.2061591988491745E-2</v>
       </c>
     </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B27" s="2" t="s">
         <v>20</v>
       </c>
@@ -4193,7 +4242,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B28" s="2" t="s">
         <v>21</v>
       </c>
@@ -4213,7 +4262,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B29" s="2" t="s">
         <v>22</v>
       </c>
@@ -4233,7 +4282,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B30" s="2" t="s">
         <v>23</v>
       </c>
@@ -4253,7 +4302,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B31" s="2" t="s">
         <v>24</v>
       </c>
@@ -4273,7 +4322,7 @@
         <v>2.6225308432856777E-2</v>
       </c>
     </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B32" s="2" t="s">
         <v>25</v>
       </c>
@@ -4293,7 +4342,7 @@
         <v>8.9624918086669446E-4</v>
       </c>
     </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B33" s="2" t="s">
         <v>26</v>
       </c>
@@ -4313,7 +4362,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A34" s="2" t="s">
         <v>0</v>
       </c>
@@ -4323,7 +4372,7 @@
       <c r="F34" s="1"/>
       <c r="G34" s="1"/>
     </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B35" s="2" t="s">
         <v>1</v>
       </c>
@@ -4343,7 +4392,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B36" s="2" t="s">
         <v>2</v>
       </c>
@@ -4363,7 +4412,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B37" s="2" t="s">
         <v>3</v>
       </c>
@@ -4383,7 +4432,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="38" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B38" s="2" t="s">
         <v>4</v>
       </c>
@@ -4403,7 +4452,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="39" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B39" s="2" t="s">
         <v>5</v>
       </c>
@@ -4423,7 +4472,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="40" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B40" s="2" t="s">
         <v>6</v>
       </c>
@@ -4443,7 +4492,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="41" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B41" s="2" t="s">
         <v>7</v>
       </c>
@@ -4463,7 +4512,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="42" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B42" s="2" t="s">
         <v>8</v>
       </c>
@@ -4483,7 +4532,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="43" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B43" s="2" t="s">
         <v>9</v>
       </c>
@@ -4503,7 +4552,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="44" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B44" s="2" t="s">
         <v>10</v>
       </c>

</xml_diff>

<commit_message>
STDEV changed for everything
</commit_message>
<xml_diff>
--- a/results/overall.xlsx
+++ b/results/overall.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10211"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21328"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5EBBA449-DAE3-8740-B967-24F6D9B34482}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D03BCCBF-59E9-4B66-AAF1-D523CBB6E38A}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="960" yWindow="460" windowWidth="27840" windowHeight="17540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Length" sheetId="1" r:id="rId1"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="247" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="236" uniqueCount="49">
   <si>
     <t>Python</t>
   </si>
@@ -176,9 +176,6 @@
   </si>
   <si>
     <t>spring-framework</t>
-  </si>
-  <si>
-    <t>CPP</t>
   </si>
 </sst>
 </file>
@@ -251,14 +248,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Calculation" xfId="1" builtinId="22"/>
@@ -542,23 +538,23 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:O44"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J18" sqref="J18"/>
+    <sheetView topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="C44" sqref="C44:G44"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="9.5" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="20.83203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="9.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="20.85546875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="6" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="4.83203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="4.85546875" bestFit="1" customWidth="1"/>
     <col min="5" max="7" width="12" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="9" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="11" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="12" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>27</v>
       </c>
@@ -579,7 +575,7 @@
       </c>
       <c r="J1" s="2"/>
     </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
       <c r="B2" s="2" t="s">
         <v>28</v>
       </c>
@@ -593,10 +589,10 @@
         <v>19.130612972202425</v>
       </c>
       <c r="F2" s="1">
-        <v>39.724643065669298</v>
+        <v>39.72818279773832</v>
       </c>
       <c r="G2" s="1">
-        <v>0.53027502424260975</v>
+        <v>0.53032227530300591</v>
       </c>
       <c r="K2" s="2" t="s">
         <v>11</v>
@@ -614,7 +610,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
       <c r="B3" s="2" t="s">
         <v>29</v>
       </c>
@@ -628,10 +624,10 @@
         <v>18.98860009119927</v>
       </c>
       <c r="F3" s="1">
-        <v>38.367310117301088</v>
+        <v>38.376060786845208</v>
       </c>
       <c r="G3" s="1">
-        <v>0.81929826769823633</v>
+        <v>0.81948513011774859</v>
       </c>
       <c r="J3" s="2" t="s">
         <v>11</v>
@@ -657,7 +653,7 @@
         <v>573.32221149114957</v>
       </c>
     </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
       <c r="B4" s="2" t="s">
         <v>30</v>
       </c>
@@ -671,10 +667,10 @@
         <v>10.242315573770492</v>
       </c>
       <c r="F4" s="1">
-        <v>14.285840475125749</v>
+        <v>14.287670468148708</v>
       </c>
       <c r="G4" s="1">
-        <v>0.22863930520677264</v>
+        <v>0.22866859353139246</v>
       </c>
       <c r="J4" s="2" t="s">
         <v>12</v>
@@ -700,7 +696,7 @@
         <v>0.64940801444913587</v>
       </c>
     </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
       <c r="B5" s="2" t="s">
         <v>31</v>
       </c>
@@ -714,10 +710,10 @@
         <v>12.99933155080214</v>
       </c>
       <c r="F5" s="1">
-        <v>17.066302745256451</v>
+        <v>17.072009584655298</v>
       </c>
       <c r="G5" s="1">
-        <v>0.4412387531650156</v>
+        <v>0.44138629998511175</v>
       </c>
       <c r="J5" s="2" t="s">
         <v>13</v>
@@ -743,7 +739,7 @@
         <v>12.357545642537358</v>
       </c>
     </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
       <c r="B6" s="2" t="s">
         <v>32</v>
       </c>
@@ -757,36 +753,36 @@
         <v>22.472590510200206</v>
       </c>
       <c r="F6" s="1">
-        <v>60.465062164100772</v>
+        <v>60.466210718311935</v>
       </c>
       <c r="G6" s="1">
-        <v>0.37268062214648062</v>
+        <v>0.37268770134035994</v>
       </c>
       <c r="J6" s="2" t="s">
         <v>14</v>
       </c>
       <c r="K6" s="1">
         <f>MAX(F2:F44)</f>
-        <v>1393.4277666544704</v>
+        <v>1394.0096951687317</v>
       </c>
       <c r="L6" s="1">
         <f>MIN(F2:F44)</f>
-        <v>2.9481109247603552</v>
+        <v>3.1269438398822866</v>
       </c>
       <c r="M6" s="1">
         <f>AVERAGE(F2:F44)</f>
-        <v>78.289419644954336</v>
+        <v>78.385347104890656</v>
       </c>
       <c r="N6" s="1">
         <f>_xlfn.STDEV.S(F2:F44)</f>
-        <v>221.63949697882299</v>
+        <v>221.70632885690702</v>
       </c>
       <c r="O6" s="1">
         <f>N6/SQRT(COUNT(F2:F44))</f>
-        <v>35.044281495354447</v>
-      </c>
-    </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.2">
+        <v>35.054848543107056</v>
+      </c>
+    </row>
+    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
       <c r="B7" s="2" t="s">
         <v>33</v>
       </c>
@@ -800,36 +796,36 @@
         <v>18.676984669465874</v>
       </c>
       <c r="F7" s="1">
-        <v>34.802694755977811</v>
+        <v>34.804394064821672</v>
       </c>
       <c r="G7" s="1">
-        <v>0.34390753348894054</v>
+        <v>0.34392432543902446</v>
       </c>
       <c r="J7" s="2" t="s">
         <v>15</v>
       </c>
       <c r="K7" s="1">
         <f>MAX(G2:G44)</f>
-        <v>40.258357430161986</v>
+        <v>40.275170275927344</v>
       </c>
       <c r="L7" s="1">
         <f>MIN(G2:G44)</f>
-        <v>3.1390013331077431E-2</v>
+        <v>3.1390597586767523E-2</v>
       </c>
       <c r="M7" s="1">
         <f>AVERAGE(G2:G44)</f>
-        <v>1.9930877888506167</v>
+        <v>2.0306751246008488</v>
       </c>
       <c r="N7" s="1">
         <f>_xlfn.STDEV.S(G2:G44)</f>
-        <v>6.3739088390611816</v>
+        <v>6.3886649843751773</v>
       </c>
       <c r="O7" s="1">
         <f>N7/SQRT(COUNT(G2:G44))</f>
-        <v>1.0078034764856472</v>
-      </c>
-    </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.2">
+        <v>1.0101366279194794</v>
+      </c>
+    </row>
+    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
       <c r="B8" s="2" t="s">
         <v>34</v>
       </c>
@@ -843,13 +839,13 @@
         <v>13.809551771383832</v>
       </c>
       <c r="F8" s="1">
-        <v>26.023615356988625</v>
+        <v>26.02488887067247</v>
       </c>
       <c r="G8" s="1">
-        <v>0.25744513071085023</v>
-      </c>
-    </row>
-    <row r="9" spans="1:15" x14ac:dyDescent="0.2">
+        <v>0.25745772926382998</v>
+      </c>
+    </row>
+    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
       <c r="B9" s="2" t="s">
         <v>35</v>
       </c>
@@ -863,13 +859,13 @@
         <v>21.356435246460514</v>
       </c>
       <c r="F9" s="1">
-        <v>45.550130592375929</v>
+        <v>45.551044070513619</v>
       </c>
       <c r="G9" s="1">
-        <v>0.28847113143317576</v>
-      </c>
-    </row>
-    <row r="10" spans="1:15" x14ac:dyDescent="0.2">
+        <v>0.28847691653342666</v>
+      </c>
+    </row>
+    <row r="10" spans="1:15" x14ac:dyDescent="0.25">
       <c r="B10" s="2" t="s">
         <v>36</v>
       </c>
@@ -883,16 +879,14 @@
         <v>19.849602062826964</v>
       </c>
       <c r="F10" s="1">
-        <v>47.617569374663034</v>
+        <v>47.618159690965449</v>
       </c>
       <c r="G10" s="1">
-        <v>0.23710295140328733</v>
-      </c>
-      <c r="J10" s="4" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="11" spans="1:15" x14ac:dyDescent="0.2">
+        <v>0.23710589077502348</v>
+      </c>
+      <c r="J10" s="2"/>
+    </row>
+    <row r="11" spans="1:15" x14ac:dyDescent="0.25">
       <c r="B11" s="2" t="s">
         <v>37</v>
       </c>
@@ -906,53 +900,24 @@
         <v>18.748313090418353</v>
       </c>
       <c r="F11" s="1">
-        <v>38.687297774271649</v>
+        <v>38.691649306569786</v>
       </c>
       <c r="G11" s="1">
-        <v>0.58020793910761048</v>
-      </c>
-      <c r="K11" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="L11" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="M11" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="N11" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="O11" s="2" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="12" spans="1:15" x14ac:dyDescent="0.2">
+        <v>0.58027320067230792</v>
+      </c>
+      <c r="K11" s="2"/>
+      <c r="L11" s="2"/>
+      <c r="M11" s="2"/>
+      <c r="N11" s="2"/>
+      <c r="O11" s="2"/>
+    </row>
+    <row r="12" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="C12" s="1"/>
-      <c r="D12" s="1"/>
-      <c r="E12" s="1"/>
-      <c r="F12" s="1"/>
-      <c r="G12" s="1"/>
-      <c r="J12" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="K12">
-        <f>MAX(C2:C11)</f>
-        <v>6888</v>
-      </c>
-      <c r="L12">
-        <f>MIN(C2:C11)</f>
-        <v>178</v>
-      </c>
-      <c r="M12">
-        <f>AVERAGE(C2:C11)</f>
-        <v>2096.9</v>
-      </c>
-    </row>
-    <row r="13" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="J12" s="2"/>
+    </row>
+    <row r="13" spans="1:15" x14ac:dyDescent="0.25">
       <c r="B13" s="2" t="s">
         <v>39</v>
       </c>
@@ -966,16 +931,14 @@
         <v>11.341215103351725</v>
       </c>
       <c r="F13" s="1">
-        <v>16.827885286167419</v>
+        <v>16.827971899932589</v>
       </c>
       <c r="G13" s="1">
-        <v>5.3991022431659381E-2</v>
-      </c>
-      <c r="J13" s="2" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="14" spans="1:15" x14ac:dyDescent="0.2">
+        <v>5.3991300325503956E-2</v>
+      </c>
+      <c r="J13" s="2"/>
+    </row>
+    <row r="14" spans="1:15" x14ac:dyDescent="0.25">
       <c r="B14" s="2" t="s">
         <v>40</v>
       </c>
@@ -989,16 +952,14 @@
         <v>7.6979904915077499</v>
       </c>
       <c r="F14" s="1">
-        <v>11.835295383445155</v>
+        <v>11.835399972019646</v>
       </c>
       <c r="G14" s="1">
-        <v>4.9755809005011351E-2</v>
-      </c>
-      <c r="J14" s="2" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="15" spans="1:15" x14ac:dyDescent="0.2">
+        <v>4.9756248697386388E-2</v>
+      </c>
+      <c r="J14" s="2"/>
+    </row>
+    <row r="15" spans="1:15" x14ac:dyDescent="0.25">
       <c r="B15" s="2" t="s">
         <v>41</v>
       </c>
@@ -1012,16 +973,14 @@
         <v>16.149425287356323</v>
       </c>
       <c r="F15" s="1">
-        <v>11.242679879948001</v>
+        <v>11.24986599757529</v>
       </c>
       <c r="G15" s="1">
-        <v>0.40178060081536426</v>
-      </c>
-      <c r="J15" s="2" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="16" spans="1:15" x14ac:dyDescent="0.2">
+        <v>0.40203741170819873</v>
+      </c>
+      <c r="J15" s="2"/>
+    </row>
+    <row r="16" spans="1:15" x14ac:dyDescent="0.25">
       <c r="B16" s="2" t="s">
         <v>42</v>
       </c>
@@ -1035,16 +994,14 @@
         <v>6.7940388479571334</v>
       </c>
       <c r="F16" s="1">
-        <v>6.7326799916445381</v>
+        <v>6.73380764930116</v>
       </c>
       <c r="G16" s="1">
-        <v>0.12320918107308468</v>
-      </c>
-      <c r="J16" s="2" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.2">
+        <v>0.12322981739867503</v>
+      </c>
+      <c r="J16" s="2"/>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B17" s="2" t="s">
         <v>43</v>
       </c>
@@ -1058,13 +1015,13 @@
         <v>11.938989513822689</v>
       </c>
       <c r="F17" s="1">
-        <v>23.179884596014322</v>
+        <v>23.185410852999745</v>
       </c>
       <c r="G17" s="1">
-        <v>0.50606759321841865</v>
-      </c>
-    </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.2">
+        <v>0.50618824349864477</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B18" s="2" t="s">
         <v>44</v>
       </c>
@@ -1078,13 +1035,13 @@
         <v>11.251460885956645</v>
       </c>
       <c r="F18" s="1">
-        <v>12.059157913044759</v>
+        <v>12.060294657913481</v>
       </c>
       <c r="G18" s="1">
-        <v>0.16556719384585963</v>
-      </c>
-    </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.2">
+        <v>0.16558280087741112</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B19" s="2" t="s">
         <v>45</v>
       </c>
@@ -1098,13 +1055,13 @@
         <v>11.284793814432989</v>
       </c>
       <c r="F19" s="1">
-        <v>13.827455718913674</v>
+        <v>13.831912594361857</v>
       </c>
       <c r="G19" s="1">
-        <v>0.35099135344384824</v>
-      </c>
-    </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.2">
+        <v>0.35110448522871801</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B20" s="2" t="s">
         <v>46</v>
       </c>
@@ -1118,13 +1075,13 @@
         <v>12.255259012139746</v>
       </c>
       <c r="F20" s="1">
-        <v>13.490103488745529</v>
+        <v>13.490416030963672</v>
       </c>
       <c r="G20" s="1">
-        <v>9.1826797264275228E-2</v>
-      </c>
-    </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.2">
+        <v>9.1828924731342174E-2</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B21" s="2" t="s">
         <v>47</v>
       </c>
@@ -1138,13 +1095,13 @@
         <v>6.4846262656343061</v>
       </c>
       <c r="F21" s="1">
-        <v>5.1448988345310616</v>
+        <v>5.1449945954467173</v>
       </c>
       <c r="G21" s="1">
-        <v>3.1390013331077431E-2</v>
-      </c>
-    </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.2">
+        <v>3.1390597586767523E-2</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B22" s="2" t="s">
         <v>48</v>
       </c>
@@ -1158,23 +1115,18 @@
         <v>8.0226078676035986</v>
       </c>
       <c r="F22" s="1">
-        <v>11.418704425056442</v>
+        <v>11.418798163522922</v>
       </c>
       <c r="G22" s="1">
-        <v>4.6267886526358687E-2</v>
-      </c>
-    </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.2">
+        <v>4.6268266348847197E-2</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A23" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="C23" s="1"/>
-      <c r="D23" s="1"/>
-      <c r="E23" s="1"/>
-      <c r="F23" s="1"/>
-      <c r="G23" s="1"/>
-    </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.2">
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B24" s="2" t="s">
         <v>17</v>
       </c>
@@ -1188,13 +1140,13 @@
         <v>30.592414921835317</v>
       </c>
       <c r="F24" s="1">
-        <v>165.06781659292028</v>
+        <v>165.07247472271936</v>
       </c>
       <c r="G24" s="1">
-        <v>1.2400602963634322</v>
-      </c>
-    </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.2">
+        <v>1.240095290234063</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B25" s="2" t="s">
         <v>18</v>
       </c>
@@ -1208,13 +1160,13 @@
         <v>505.93656093489147</v>
       </c>
       <c r="F25" s="1">
-        <v>1393.4277666544704</v>
+        <v>1394.0096951687317</v>
       </c>
       <c r="G25" s="1">
-        <v>40.258357430161986</v>
-      </c>
-    </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.2">
+        <v>40.275170275927344</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B26" s="2" t="s">
         <v>19</v>
       </c>
@@ -1228,13 +1180,13 @@
         <v>17.486425339366516</v>
       </c>
       <c r="F26" s="1">
-        <v>65.934415147148016</v>
+        <v>65.971740038417749</v>
       </c>
       <c r="G26" s="1">
-        <v>2.2176143628772422</v>
-      </c>
-    </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.2">
+        <v>2.218869734822043</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B27" s="2" t="s">
         <v>20</v>
       </c>
@@ -1248,13 +1200,13 @@
         <v>46.356000000000002</v>
       </c>
       <c r="F27" s="1">
-        <v>69.482985428088796</v>
+        <v>69.622369691398632</v>
       </c>
       <c r="G27" s="1">
-        <v>4.3944898516210049</v>
-      </c>
-    </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.2">
+        <v>4.4033052864618796</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B28" s="2" t="s">
         <v>21</v>
       </c>
@@ -1268,13 +1220,13 @@
         <v>6.4444444444444446</v>
       </c>
       <c r="F28" s="1">
-        <v>2.9481109247603552</v>
+        <v>3.1269438398822866</v>
       </c>
       <c r="G28" s="1">
-        <v>0.98270364158678503</v>
-      </c>
-    </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.2">
+        <v>1.0423146132940955</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B29" s="2" t="s">
         <v>22</v>
       </c>
@@ -1288,13 +1240,13 @@
         <v>18.134529147982065</v>
       </c>
       <c r="F29" s="1">
-        <v>64.150186873456377</v>
+        <v>64.198185523548801</v>
       </c>
       <c r="G29" s="1">
-        <v>2.4801895136795258</v>
-      </c>
-    </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.2">
+        <v>2.4820452487043485</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B30" s="2" t="s">
         <v>23</v>
       </c>
@@ -1308,13 +1260,13 @@
         <v>27.366403607666292</v>
       </c>
       <c r="F30" s="1">
-        <v>54.91756576103699</v>
+        <v>54.948548875355627</v>
       </c>
       <c r="G30" s="1">
-        <v>1.8439513932942531</v>
-      </c>
-    </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.2">
+        <v>1.8449917044592643</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B31" s="2" t="s">
         <v>24</v>
       </c>
@@ -1328,13 +1280,13 @@
         <v>29.977682596934176</v>
       </c>
       <c r="F31" s="1">
-        <v>197.23938232098257</v>
+        <v>197.26161775111026</v>
       </c>
       <c r="G31" s="1">
-        <v>2.9614054075571348</v>
-      </c>
-    </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.2">
+        <v>2.961739256316164</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B32" s="2" t="s">
         <v>25</v>
       </c>
@@ -1348,13 +1300,13 @@
         <v>20.685010958464744</v>
       </c>
       <c r="F32" s="1">
-        <v>171.37448111493558</v>
+        <v>171.37562624910205</v>
       </c>
       <c r="G32" s="1">
-        <v>0.62648991469281545</v>
-      </c>
-    </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.2">
+        <v>0.62649410093455704</v>
+      </c>
+    </row>
+    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B33" s="2" t="s">
         <v>26</v>
       </c>
@@ -1368,23 +1320,18 @@
         <v>74.464872521246463</v>
       </c>
       <c r="F33" s="1">
-        <v>294.36580610337103</v>
+        <v>294.40750983753276</v>
       </c>
       <c r="G33" s="1">
-        <v>4.9545019960785748</v>
-      </c>
-    </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.2">
+        <v>4.955203916036206</v>
+      </c>
+    </row>
+    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A34" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="C34" s="1"/>
-      <c r="D34" s="1"/>
-      <c r="E34" s="1"/>
-      <c r="F34" s="1"/>
-      <c r="G34" s="1"/>
-    </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.2">
+    </row>
+    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B35" s="2" t="s">
         <v>1</v>
       </c>
@@ -1398,13 +1345,13 @@
         <v>17.747660582255083</v>
       </c>
       <c r="F35" s="1">
-        <v>29.034117260006202</v>
+        <v>29.034536546428789</v>
       </c>
       <c r="G35" s="1">
-        <v>0.15603427483907159</v>
-      </c>
-    </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.2">
+        <v>0.1560365281554825</v>
+      </c>
+    </row>
+    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B36" s="2" t="s">
         <v>2</v>
       </c>
@@ -1418,13 +1365,13 @@
         <v>30</v>
       </c>
       <c r="F36" s="1">
-        <v>3</v>
+        <v>4.2426406871192848</v>
       </c>
       <c r="G36" s="1">
-        <v>2.1213203435596424</v>
-      </c>
-    </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.2">
+        <v>2.9999999999999996</v>
+      </c>
+    </row>
+    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B37" s="2" t="s">
         <v>3</v>
       </c>
@@ -1438,13 +1385,13 @@
         <v>10.379232992536991</v>
       </c>
       <c r="F37" s="1">
-        <v>13.626797992105423</v>
+        <v>13.627091923318281</v>
       </c>
       <c r="G37" s="1">
-        <v>8.9500968392268287E-2</v>
-      </c>
-    </row>
-    <row r="38" spans="1:7" x14ac:dyDescent="0.2">
+        <v>8.9502898935907862E-2</v>
+      </c>
+    </row>
+    <row r="38" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B38" s="2" t="s">
         <v>4</v>
       </c>
@@ -1458,13 +1405,13 @@
         <v>9.4623376623376618</v>
       </c>
       <c r="F38" s="1">
-        <v>12.705628561103831</v>
+        <v>12.722161591599541</v>
       </c>
       <c r="G38" s="1">
-        <v>0.64753879116162472</v>
-      </c>
-    </row>
-    <row r="39" spans="1:7" x14ac:dyDescent="0.2">
+        <v>0.64838139241743387</v>
+      </c>
+    </row>
+    <row r="39" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B39" s="2" t="s">
         <v>5</v>
       </c>
@@ -1478,13 +1425,13 @@
         <v>15.227255709472107</v>
       </c>
       <c r="F39" s="1">
-        <v>22.237571087493809</v>
+        <v>22.241735036802371</v>
       </c>
       <c r="G39" s="1">
-        <v>0.43027925242772791</v>
-      </c>
-    </row>
-    <row r="40" spans="1:7" x14ac:dyDescent="0.2">
+        <v>0.43035982152354263</v>
+      </c>
+    </row>
+    <row r="40" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B40" s="2" t="s">
         <v>6</v>
       </c>
@@ -1498,13 +1445,13 @@
         <v>22.714285714285715</v>
       </c>
       <c r="F40" s="1">
-        <v>17.523162513935546</v>
+        <v>18.927178744812849</v>
       </c>
       <c r="G40" s="1">
-        <v>6.6231328850346936</v>
-      </c>
-    </row>
-    <row r="41" spans="1:7" x14ac:dyDescent="0.2">
+        <v>7.1538011398346351</v>
+      </c>
+    </row>
+    <row r="41" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B41" s="2" t="s">
         <v>7</v>
       </c>
@@ -1518,13 +1465,13 @@
         <v>10.785831960461286</v>
       </c>
       <c r="F41" s="1">
-        <v>12.834144003961915</v>
+        <v>12.844728866795323</v>
       </c>
       <c r="G41" s="1">
-        <v>0.52092183578955342</v>
-      </c>
-    </row>
-    <row r="42" spans="1:7" x14ac:dyDescent="0.2">
+        <v>0.52135146211890249</v>
+      </c>
+    </row>
+    <row r="42" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B42" s="2" t="s">
         <v>8</v>
       </c>
@@ -1538,13 +1485,13 @@
         <v>4.4391891891891895</v>
       </c>
       <c r="F42" s="1">
-        <v>3.8942548663649958</v>
+        <v>3.9074781807031815</v>
       </c>
       <c r="G42" s="1">
-        <v>0.32010577816968244</v>
-      </c>
-    </row>
-    <row r="43" spans="1:7" x14ac:dyDescent="0.2">
+        <v>0.32119272791269149</v>
+      </c>
+    </row>
+    <row r="43" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B43" s="2" t="s">
         <v>9</v>
       </c>
@@ -1558,13 +1505,13 @@
         <v>5.0473559589581685</v>
       </c>
       <c r="F43" s="1">
-        <v>5.4938552632088893</v>
+        <v>5.4960246039699223</v>
       </c>
       <c r="G43" s="1">
-        <v>0.15434369966651265</v>
-      </c>
-    </row>
-    <row r="44" spans="1:7" x14ac:dyDescent="0.2">
+        <v>0.15440464486125366</v>
+      </c>
+    </row>
+    <row r="44" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B44" s="2" t="s">
         <v>10</v>
       </c>
@@ -1578,10 +1525,10 @@
         <v>25.229363579080026</v>
       </c>
       <c r="F44" s="1">
-        <v>43.969525389581051</v>
+        <v>43.976453542998279</v>
       </c>
       <c r="G44" s="1">
-        <v>0.78045580751321231</v>
+        <v>0.78057878172141471</v>
       </c>
     </row>
   </sheetData>
@@ -1594,16 +1541,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{74F2D45E-113D-4FBB-9FB8-E8607006C13E}">
   <dimension ref="A1:O44"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="L18" sqref="L18"/>
+    <sheetView topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="C44" sqref="C44:G44"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="20.83203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="20.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>27</v>
       </c>
@@ -1623,7 +1570,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
       <c r="B2" s="2" t="s">
         <v>28</v>
       </c>
@@ -1637,10 +1584,10 @@
         <v>85.162687099073409</v>
       </c>
       <c r="F2" s="1">
-        <v>43.77879353212866</v>
+        <v>43.782694516189167</v>
       </c>
       <c r="G2" s="1">
-        <v>0.58439293622311617</v>
+        <v>0.58444500955235501</v>
       </c>
       <c r="K2" s="2" t="s">
         <v>11</v>
@@ -1658,7 +1605,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
       <c r="B3" s="2" t="s">
         <v>29</v>
       </c>
@@ -1672,10 +1619,10 @@
         <v>66.291837665298672</v>
       </c>
       <c r="F3" s="1">
-        <v>12.674630129742162</v>
+        <v>12.677520910970248</v>
       </c>
       <c r="G3" s="1">
-        <v>0.27065495280397572</v>
+        <v>0.27071668275181998</v>
       </c>
       <c r="J3" s="2" t="s">
         <v>11</v>
@@ -1693,15 +1640,15 @@
         <v>277.72500000000002</v>
       </c>
       <c r="N3" s="1">
-        <f>_xlfn.STDEV.P(C2:C44)</f>
-        <v>219.83004657007194</v>
+        <f>_xlfn.STDEV.S(C2:C44)</f>
+        <v>222.63054222934764</v>
       </c>
       <c r="O3" s="1">
         <f>N3/SQRT(COUNT(C2:C44))</f>
-        <v>34.758182265115643</v>
-      </c>
-    </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.2">
+        <v>35.200979508151946</v>
+      </c>
+    </row>
+    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
       <c r="B4" s="2" t="s">
         <v>30</v>
       </c>
@@ -1715,10 +1662,10 @@
         <v>65.229252049180332</v>
       </c>
       <c r="F4" s="1">
-        <v>14.040849174716142</v>
+        <v>14.042647784750375</v>
       </c>
       <c r="G4" s="1">
-        <v>0.22471831499237904</v>
+        <v>0.22474710104450393</v>
       </c>
       <c r="J4" s="2" t="s">
         <v>12</v>
@@ -1736,15 +1683,15 @@
         <v>15.425000000000001</v>
       </c>
       <c r="N4" s="1">
-        <f>_xlfn.STDEV.P(D2:D44)</f>
-        <v>5.7178995269242012</v>
+        <f>_xlfn.STDEV.S(D2:D44)</f>
+        <v>5.7907419479452118</v>
       </c>
       <c r="O4" s="1">
         <f>N4/SQRT(COUNT(D2:D44))</f>
-        <v>0.90407929685398725</v>
-      </c>
-    </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.2">
+        <v>0.91559669488935336</v>
+      </c>
+    </row>
+    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
       <c r="B5" s="2" t="s">
         <v>31</v>
       </c>
@@ -1758,10 +1705,10 @@
         <v>71.090909090909093</v>
       </c>
       <c r="F5" s="1">
-        <v>19.89977622552475</v>
+        <v>19.906430556500087</v>
       </c>
       <c r="G5" s="1">
-        <v>0.51449646599371968</v>
+        <v>0.51466850962534472</v>
       </c>
       <c r="J5" s="2" t="s">
         <v>13</v>
@@ -1779,15 +1726,15 @@
         <v>66.725055503063132</v>
       </c>
       <c r="N5" s="1">
-        <f>_xlfn.STDEV.P(E2:E44)</f>
-        <v>14.144911397330981</v>
+        <f>_xlfn.STDEV.S(E2:E44)</f>
+        <v>14.32510861598751</v>
       </c>
       <c r="O5" s="1">
         <f>N5/SQRT(COUNT(E2:E44))</f>
-        <v>2.2365068658420428</v>
-      </c>
-    </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.2">
+        <v>2.2649985477911434</v>
+      </c>
+    </row>
+    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
       <c r="B6" s="2" t="s">
         <v>32</v>
       </c>
@@ -1801,36 +1748,36 @@
         <v>79.794096417581585</v>
       </c>
       <c r="F6" s="1">
-        <v>29.690620675024672</v>
+        <v>29.691184658359642</v>
       </c>
       <c r="G6" s="1">
-        <v>0.18300020853452328</v>
+        <v>0.18300368468509082</v>
       </c>
       <c r="J6" s="2" t="s">
         <v>14</v>
       </c>
       <c r="K6" s="1">
         <f>MAX(F2:F44)</f>
-        <v>54.106356974901608</v>
+        <v>54.146840599701285</v>
       </c>
       <c r="L6" s="1">
         <f>MIN(F2:F44)</f>
-        <v>11</v>
+        <v>12.234173926273595</v>
       </c>
       <c r="M6" s="1">
         <f>AVERAGE(F2:F44)</f>
-        <v>26.499764811363356</v>
+        <v>26.72570113470498</v>
       </c>
       <c r="N6" s="1">
-        <f>_xlfn.STDEV.P(F2:F44)</f>
-        <v>10.825632019278917</v>
+        <f>_xlfn.STDEV.S(F2:F44)</f>
+        <v>10.868610331231242</v>
       </c>
       <c r="O6" s="1">
         <f>N6/SQRT(COUNT(F2:F44))</f>
-        <v>1.711682714588461</v>
-      </c>
-    </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.2">
+        <v>1.7184781823763902</v>
+      </c>
+    </row>
+    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
       <c r="B7" s="2" t="s">
         <v>33</v>
       </c>
@@ -1844,36 +1791,36 @@
         <v>73.978322429450245</v>
       </c>
       <c r="F7" s="1">
-        <v>26.778183379841785</v>
+        <v>26.779490876406612</v>
       </c>
       <c r="G7" s="1">
-        <v>0.26461223942706702</v>
+        <v>0.26462515963114336</v>
       </c>
       <c r="J7" s="2" t="s">
         <v>15</v>
       </c>
       <c r="K7" s="1">
         <f>MAX(G2:G44)</f>
-        <v>12.526589795113582</v>
+        <v>13.530263382908862</v>
       </c>
       <c r="L7" s="1">
         <f>MIN(G2:G44)</f>
-        <v>6.0917069553424373E-2</v>
+        <v>6.0917824743992204E-2</v>
       </c>
       <c r="M7" s="1">
         <f>AVERAGE(G2:G44)</f>
-        <v>1.21486614310792</v>
+        <v>1.333204911168185</v>
       </c>
       <c r="N7" s="1">
-        <f>_xlfn.STDEV.P(G2:G44)</f>
-        <v>2.4811627586020211</v>
+        <f>_xlfn.STDEV.S(G2:G44)</f>
+        <v>2.9048757245747021</v>
       </c>
       <c r="O7" s="1">
         <f>N7/SQRT(COUNT(G2:G44))</f>
-        <v>0.39230627813844599</v>
-      </c>
-    </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.2">
+        <v>0.45930118046940072</v>
+      </c>
+    </row>
+    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
       <c r="B8" s="2" t="s">
         <v>34</v>
       </c>
@@ -1887,13 +1834,13 @@
         <v>70.088569191622625</v>
       </c>
       <c r="F8" s="1">
-        <v>20.091162476025339</v>
+        <v>20.092145674170045</v>
       </c>
       <c r="G8" s="1">
-        <v>0.19875685521859038</v>
-      </c>
-    </row>
-    <row r="9" spans="1:15" x14ac:dyDescent="0.2">
+        <v>0.19876658175240999</v>
+      </c>
+    </row>
+    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
       <c r="B9" s="2" t="s">
         <v>35</v>
       </c>
@@ -1907,13 +1854,13 @@
         <v>70.382705651145073</v>
       </c>
       <c r="F9" s="1">
-        <v>12.278183459362239</v>
+        <v>12.27842969031733</v>
       </c>
       <c r="G9" s="1">
-        <v>7.775831657130669E-2</v>
-      </c>
-    </row>
-    <row r="10" spans="1:15" x14ac:dyDescent="0.2">
+        <v>7.775987596359131E-2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:15" x14ac:dyDescent="0.25">
       <c r="B10" s="2" t="s">
         <v>36</v>
       </c>
@@ -1927,10 +1874,10 @@
         <v>71.374556814519124</v>
       </c>
       <c r="F10" s="1">
-        <v>12.234022260766936</v>
+        <v>12.234173926273595</v>
       </c>
       <c r="G10" s="1">
-        <v>6.0917069553424373E-2</v>
+        <v>6.0917824743992204E-2</v>
       </c>
       <c r="K10" s="3"/>
       <c r="L10" s="3"/>
@@ -1938,7 +1885,7 @@
       <c r="N10" s="3"/>
       <c r="O10" s="3"/>
     </row>
-    <row r="11" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:15" x14ac:dyDescent="0.25">
       <c r="B11" s="2" t="s">
         <v>37</v>
       </c>
@@ -1952,18 +1899,18 @@
         <v>80.39878542510121</v>
       </c>
       <c r="F11" s="1">
-        <v>35.495901930440397</v>
+        <v>35.499894495767734</v>
       </c>
       <c r="G11" s="1">
-        <v>0.53234537666580184</v>
-      </c>
-    </row>
-    <row r="12" spans="1:15" x14ac:dyDescent="0.2">
+        <v>0.53240525466797817</v>
+      </c>
+    </row>
+    <row r="12" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="13" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:15" x14ac:dyDescent="0.25">
       <c r="B13" s="2" t="s">
         <v>39</v>
       </c>
@@ -1977,13 +1924,13 @@
         <v>85.73737956024047</v>
       </c>
       <c r="F13" s="1">
-        <v>33.466417060347034</v>
+        <v>33.466589313267654</v>
       </c>
       <c r="G13" s="1">
-        <v>0.10737451815753295</v>
-      </c>
-    </row>
-    <row r="14" spans="1:15" x14ac:dyDescent="0.2">
+        <v>0.10737507081825906</v>
+      </c>
+    </row>
+    <row r="14" spans="1:15" x14ac:dyDescent="0.25">
       <c r="B14" s="2" t="s">
         <v>40</v>
       </c>
@@ -1997,13 +1944,13 @@
         <v>72.967833725102068</v>
       </c>
       <c r="F14" s="1">
-        <v>28.157860118745344</v>
+        <v>28.158108949919825</v>
       </c>
       <c r="G14" s="1">
-        <v>0.11837618451144184</v>
-      </c>
-    </row>
-    <row r="15" spans="1:15" x14ac:dyDescent="0.2">
+        <v>0.1183772306024764</v>
+      </c>
+    </row>
+    <row r="15" spans="1:15" x14ac:dyDescent="0.25">
       <c r="B15" s="2" t="s">
         <v>41</v>
       </c>
@@ -2017,13 +1964,13 @@
         <v>66.722860791826307</v>
       </c>
       <c r="F15" s="1">
-        <v>25.639928870415815</v>
+        <v>25.656317449187561</v>
       </c>
       <c r="G15" s="1">
-        <v>0.91629630447740862</v>
-      </c>
-    </row>
-    <row r="16" spans="1:15" x14ac:dyDescent="0.2">
+        <v>0.91688198450172087</v>
+      </c>
+    </row>
+    <row r="16" spans="1:15" x14ac:dyDescent="0.25">
       <c r="B16" s="2" t="s">
         <v>42</v>
       </c>
@@ -2037,13 +1984,13 @@
         <v>57.847622237106499</v>
       </c>
       <c r="F16" s="1">
-        <v>23.897888296026036</v>
+        <v>23.901890957187341</v>
       </c>
       <c r="G16" s="1">
-        <v>0.43733539244157782</v>
-      </c>
-    </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.2">
+        <v>0.43740864181692457</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B17" s="2" t="s">
         <v>43</v>
       </c>
@@ -2057,13 +2004,13 @@
         <v>65.124880838894185</v>
       </c>
       <c r="F17" s="1">
-        <v>28.777799021147011</v>
+        <v>28.784659862589372</v>
       </c>
       <c r="G17" s="1">
-        <v>0.62828231212416652</v>
-      </c>
-    </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.2">
+        <v>0.62843209930286481</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B18" s="2" t="s">
         <v>44</v>
       </c>
@@ -2077,13 +2024,13 @@
         <v>73.598303487276155</v>
       </c>
       <c r="F18" s="1">
-        <v>19.453596324071821</v>
+        <v>19.45543009853262</v>
       </c>
       <c r="G18" s="1">
-        <v>0.26708974016357978</v>
-      </c>
-    </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.2">
+        <v>0.26711491711986562</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B19" s="2" t="s">
         <v>45</v>
       </c>
@@ -2097,13 +2044,13 @@
         <v>73.744845360824741</v>
       </c>
       <c r="F19" s="1">
-        <v>20.003430098304047</v>
+        <v>20.009877618245298</v>
       </c>
       <c r="G19" s="1">
-        <v>0.50776015099578575</v>
-      </c>
-    </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.2">
+        <v>0.50792381261195996</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B20" s="2" t="s">
         <v>46</v>
       </c>
@@ -2117,13 +2064,13 @@
         <v>75.567000278009459</v>
       </c>
       <c r="F20" s="1">
-        <v>27.194415165251439</v>
+        <v>27.1950452125186</v>
       </c>
       <c r="G20" s="1">
-        <v>0.18511170430852586</v>
-      </c>
-    </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.2">
+        <v>0.18511599302452547</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B21" s="2" t="s">
         <v>47</v>
       </c>
@@ -2137,13 +2084,13 @@
         <v>64.976958010720665</v>
       </c>
       <c r="F21" s="1">
-        <v>18.279510738605321</v>
+        <v>18.279850971278954</v>
       </c>
       <c r="G21" s="1">
-        <v>0.11152679658524194</v>
-      </c>
-    </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.2">
+        <v>0.11152887240995774</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B22" s="2" t="s">
         <v>48</v>
       </c>
@@ -2157,18 +2104,18 @@
         <v>72.888257700137913</v>
       </c>
       <c r="F22" s="1">
-        <v>25.420041759399894</v>
+        <v>25.420250437691557</v>
       </c>
       <c r="G22" s="1">
-        <v>0.1030004424178271</v>
-      </c>
-    </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.2">
+        <v>0.10300128796940282</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A23" s="2" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B24" s="2" t="s">
         <v>17</v>
       </c>
@@ -2182,13 +2129,13 @@
         <v>85.617529205937132</v>
       </c>
       <c r="F24" s="1">
-        <v>48.583826805518378</v>
+        <v>48.585197816391783</v>
       </c>
       <c r="G24" s="1">
-        <v>0.36498256238221033</v>
-      </c>
-    </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.2">
+        <v>0.36499286200442066</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B25" s="2" t="s">
         <v>18</v>
       </c>
@@ -2202,13 +2149,13 @@
         <v>84.936560934891489</v>
       </c>
       <c r="F25" s="1">
-        <v>39.654067348609061</v>
+        <v>39.670627828490993</v>
       </c>
       <c r="G25" s="1">
-        <v>1.1456694455808718</v>
-      </c>
-    </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.2">
+        <v>1.1461479043386604</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B26" s="2" t="s">
         <v>19</v>
       </c>
@@ -2222,13 +2169,13 @@
         <v>66.237556561085967</v>
       </c>
       <c r="F26" s="1">
-        <v>20.9204513894251</v>
+        <v>20.932294272564064</v>
       </c>
       <c r="G26" s="1">
-        <v>0.70363092438943098</v>
-      </c>
-    </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.2">
+        <v>0.70402924365393393</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B27" s="2" t="s">
         <v>20</v>
       </c>
@@ -2242,13 +2189,13 @@
         <v>78.5</v>
       </c>
       <c r="F27" s="1">
-        <v>42.85708809520311</v>
+        <v>42.943060274074682</v>
       </c>
       <c r="G27" s="1">
-        <v>2.7105202452665802</v>
-      </c>
-    </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.2">
+        <v>2.7159576032794113</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B28" s="2" t="s">
         <v>21</v>
       </c>
@@ -2262,13 +2209,13 @@
         <v>67.888888888888886</v>
       </c>
       <c r="F28" s="1">
-        <v>24.296522130838419</v>
+        <v>25.770353336947309</v>
       </c>
       <c r="G28" s="1">
-        <v>8.0988407102794735</v>
-      </c>
-    </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.2">
+        <v>8.590117778982437</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B29" s="2" t="s">
         <v>22</v>
       </c>
@@ -2282,13 +2229,13 @@
         <v>82.139013452914796</v>
       </c>
       <c r="F29" s="1">
-        <v>54.106356974901608</v>
+        <v>54.146840599701285</v>
       </c>
       <c r="G29" s="1">
-        <v>2.0918726153871567</v>
-      </c>
-    </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.2">
+        <v>2.0934378027482152</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B30" s="2" t="s">
         <v>23</v>
       </c>
@@ -2302,13 +2249,13 @@
         <v>66.096956031567075</v>
       </c>
       <c r="F30" s="1">
-        <v>32.155654089834329</v>
+        <v>32.173795504022117</v>
       </c>
       <c r="G30" s="1">
-        <v>1.0796811974376637</v>
-      </c>
-    </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.2">
+        <v>1.0802903265114734</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B31" s="2" t="s">
         <v>24</v>
       </c>
@@ -2322,13 +2269,13 @@
         <v>76.958521190261493</v>
       </c>
       <c r="F31" s="1">
-        <v>44.74458213320132</v>
+        <v>44.749626333897488</v>
       </c>
       <c r="G31" s="1">
-        <v>0.67180725232909289</v>
-      </c>
-    </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.2">
+        <v>0.67188298732198659</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B32" s="2" t="s">
         <v>25</v>
       </c>
@@ -2342,13 +2289,13 @@
         <v>63.415847009140961</v>
       </c>
       <c r="F32" s="1">
-        <v>46.607155118333665</v>
+        <v>46.607466550032129</v>
       </c>
       <c r="G32" s="1">
-        <v>0.17038075006381415</v>
-      </c>
-    </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.2">
+        <v>0.17038188855781242</v>
+      </c>
+    </row>
+    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B33" s="2" t="s">
         <v>26</v>
       </c>
@@ -2362,18 +2309,18 @@
         <v>64.695184135977343</v>
       </c>
       <c r="F33" s="1">
-        <v>20.40937973922852</v>
+        <v>20.412271200564732</v>
       </c>
       <c r="G33" s="1">
-        <v>0.34351242759909445</v>
-      </c>
-    </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.2">
+        <v>0.3435610940904627</v>
+      </c>
+    </row>
+    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A34" s="2" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B35" s="2" t="s">
         <v>1</v>
       </c>
@@ -2387,13 +2334,13 @@
         <v>77.297221580406656</v>
       </c>
       <c r="F35" s="1">
-        <v>26.978107509501992</v>
+        <v>26.978497104752446</v>
       </c>
       <c r="G35" s="1">
-        <v>0.14498492942212343</v>
-      </c>
-    </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.2">
+        <v>0.14498702317313508</v>
+      </c>
+    </row>
+    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B36" s="2" t="s">
         <v>2</v>
       </c>
@@ -2407,13 +2354,13 @@
         <v>29</v>
       </c>
       <c r="F36" s="1">
-        <v>11</v>
+        <v>15.556349186104045</v>
       </c>
       <c r="G36" s="1">
-        <v>7.7781745930520225</v>
-      </c>
-    </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.2">
+        <v>10.999999999999998</v>
+      </c>
+    </row>
+    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B37" s="2" t="s">
         <v>3</v>
       </c>
@@ -2427,13 +2374,13 @@
         <v>74.649971959794655</v>
       </c>
       <c r="F37" s="1">
-        <v>21.591045362122856</v>
+        <v>21.591511082841244</v>
       </c>
       <c r="G37" s="1">
-        <v>0.14181023815212646</v>
-      </c>
-    </row>
-    <row r="38" spans="1:7" x14ac:dyDescent="0.2">
+        <v>0.14181329701124509</v>
+      </c>
+    </row>
+    <row r="38" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B38" s="2" t="s">
         <v>4</v>
       </c>
@@ -2447,13 +2394,13 @@
         <v>40.703896103896106</v>
       </c>
       <c r="F38" s="1">
-        <v>16.544017960426658</v>
+        <v>16.565545644172957</v>
       </c>
       <c r="G38" s="1">
-        <v>0.84316122886250799</v>
-      </c>
-    </row>
-    <row r="39" spans="1:7" x14ac:dyDescent="0.2">
+        <v>0.84425838121845398</v>
+      </c>
+    </row>
+    <row r="39" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B39" s="2" t="s">
         <v>5</v>
       </c>
@@ -2467,13 +2414,13 @@
         <v>42.291276675402472</v>
       </c>
       <c r="F39" s="1">
-        <v>18.009122306203921</v>
+        <v>18.01249448530027</v>
       </c>
       <c r="G39" s="1">
-        <v>0.34846214329364755</v>
-      </c>
-    </row>
-    <row r="40" spans="1:7" x14ac:dyDescent="0.2">
+        <v>0.34852739226777879</v>
+      </c>
+    </row>
+    <row r="40" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B40" s="2" t="s">
         <v>6</v>
       </c>
@@ -2487,13 +2434,13 @@
         <v>43.142857142857146</v>
       </c>
       <c r="F40" s="1">
-        <v>33.142241373590082</v>
+        <v>35.797712084380343</v>
       </c>
       <c r="G40" s="1">
-        <v>12.526589795113582</v>
-      </c>
-    </row>
-    <row r="41" spans="1:7" x14ac:dyDescent="0.2">
+        <v>13.530263382908862</v>
+      </c>
+    </row>
+    <row r="41" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B41" s="2" t="s">
         <v>7</v>
       </c>
@@ -2507,13 +2454,13 @@
         <v>43.184514003294893</v>
       </c>
       <c r="F41" s="1">
-        <v>18.925908361314516</v>
+        <v>18.941517360554386</v>
       </c>
       <c r="G41" s="1">
-        <v>0.76817892369895147</v>
-      </c>
-    </row>
-    <row r="42" spans="1:7" x14ac:dyDescent="0.2">
+        <v>0.76881247343443526</v>
+      </c>
+    </row>
+    <row r="42" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B42" s="2" t="s">
         <v>8</v>
       </c>
@@ -2527,13 +2474,13 @@
         <v>53.175675675675677</v>
       </c>
       <c r="F42" s="1">
-        <v>16.702773768763361</v>
+        <v>16.759489632373523</v>
       </c>
       <c r="G42" s="1">
-        <v>1.3729595463875914</v>
-      </c>
-    </row>
-    <row r="43" spans="1:7" x14ac:dyDescent="0.2">
+        <v>1.3776215616584211</v>
+      </c>
+    </row>
+    <row r="43" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B43" s="2" t="s">
         <v>9</v>
       </c>
@@ -2547,13 +2494,13 @@
         <v>45.722178374112076</v>
       </c>
       <c r="F43" s="1">
-        <v>18.158779803945603</v>
+        <v>18.16595010227201</v>
       </c>
       <c r="G43" s="1">
-        <v>0.51015054494418899</v>
-      </c>
-    </row>
-    <row r="44" spans="1:7" x14ac:dyDescent="0.2">
+        <v>0.51035198643079338</v>
+      </c>
+    </row>
+    <row r="44" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B44" s="2" t="s">
         <v>10</v>
       </c>
@@ -2567,10 +2514,10 @@
         <v>40.380907372400756</v>
       </c>
       <c r="F44" s="1">
-        <v>27.350501487684664</v>
+        <v>27.354811028637542</v>
       </c>
       <c r="G44" s="1">
-        <v>0.48546936850767852</v>
+        <v>0.48554586253927401</v>
       </c>
     </row>
   </sheetData>
@@ -2585,16 +2532,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CE658B17-E7D7-44A7-84B1-1333A97336CC}">
   <dimension ref="A1:O44"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C35" sqref="C35:G35"/>
+    <sheetView topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="C44" sqref="C44:G44"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="20.83203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="20.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>27</v>
       </c>
@@ -2614,7 +2561,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
       <c r="B2" s="2" t="s">
         <v>28</v>
       </c>
@@ -2628,10 +2575,10 @@
         <v>4.2965074839629365</v>
       </c>
       <c r="F2" s="1">
-        <v>5.2398394967795516</v>
+        <v>5.2403064016142311</v>
       </c>
       <c r="G2" s="1">
-        <v>6.9945399171715536E-2</v>
+        <v>6.9951631775797579E-2</v>
       </c>
       <c r="K2" s="2" t="s">
         <v>11</v>
@@ -2649,7 +2596,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
       <c r="B3" s="2" t="s">
         <v>29</v>
       </c>
@@ -2663,10 +2610,10 @@
         <v>3.2033743730050159</v>
       </c>
       <c r="F3" s="1">
-        <v>5.2528104665382083</v>
+        <v>5.2540085074858291</v>
       </c>
       <c r="G3" s="1">
-        <v>0.11216888811398</v>
+        <v>0.11219447116554176</v>
       </c>
       <c r="J3" s="2" t="s">
         <v>11</v>
@@ -2692,7 +2639,7 @@
         <v>5.2903154442811813</v>
       </c>
     </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
       <c r="B4" s="2" t="s">
         <v>30</v>
       </c>
@@ -2706,10 +2653,10 @@
         <v>5.0881147540983607</v>
       </c>
       <c r="F4" s="1">
-        <v>10.406808445417758</v>
+        <v>10.408141540721429</v>
       </c>
       <c r="G4" s="1">
-        <v>0.16655691042632517</v>
+        <v>0.16657824609674207</v>
       </c>
       <c r="J4" s="2" t="s">
         <v>12</v>
@@ -2735,7 +2682,7 @@
         <v>0.17606816861659008</v>
       </c>
     </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
       <c r="B5" s="2" t="s">
         <v>31</v>
       </c>
@@ -2749,10 +2696,10 @@
         <v>4.5060160427807485</v>
       </c>
       <c r="F5" s="1">
-        <v>9.6930134252344207</v>
+        <v>9.6962546938169822</v>
       </c>
       <c r="G5" s="1">
-        <v>0.25060689605725878</v>
+        <v>0.25069069706145924</v>
       </c>
       <c r="J5" s="2" t="s">
         <v>13</v>
@@ -2778,7 +2725,7 @@
         <v>0.37398696649215574</v>
       </c>
     </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
       <c r="B6" s="2" t="s">
         <v>32</v>
       </c>
@@ -2792,17 +2739,17 @@
         <v>5.0697108992136153</v>
       </c>
       <c r="F6" s="1">
-        <v>7.3555253130403271</v>
+        <v>7.3556650337198608</v>
       </c>
       <c r="G6" s="1">
-        <v>4.5336292592213584E-2</v>
+        <v>4.5337153770353682E-2</v>
       </c>
       <c r="J6" s="2" t="s">
         <v>14</v>
       </c>
       <c r="K6" s="1">
         <f>MAX(F2:F44)</f>
-        <v>12.381214564610293</v>
+        <v>12.381462861786957</v>
       </c>
       <c r="L6" s="1">
         <f>MIN(F2:F44)</f>
@@ -2810,18 +2757,18 @@
       </c>
       <c r="M6" s="1">
         <f>AVERAGE(F2:F44)</f>
-        <v>4.638882216466425</v>
+        <v>4.6495111504085198</v>
       </c>
       <c r="N6" s="1">
         <f>_xlfn.STDEV.P(F2:F44)</f>
-        <v>2.6849134287269156</v>
+        <v>2.6782512184416234</v>
       </c>
       <c r="O6" s="1">
         <f>N6/SQRT(COUNT(F2:F44))</f>
-        <v>0.42452208775746053</v>
-      </c>
-    </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.2">
+        <v>0.42346869981983437</v>
+      </c>
+    </row>
+    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
       <c r="B7" s="2" t="s">
         <v>33</v>
       </c>
@@ -2835,17 +2782,17 @@
         <v>3.1161019431696122</v>
       </c>
       <c r="F7" s="1">
-        <v>4.6585905644539265</v>
+        <v>4.6588180291431298</v>
       </c>
       <c r="G7" s="1">
-        <v>4.6034492495182884E-2</v>
+        <v>4.6036740218262033E-2</v>
       </c>
       <c r="J7" s="2" t="s">
         <v>15</v>
       </c>
       <c r="K7" s="1">
         <f>MAX(G2:G44)</f>
-        <v>1.0101525445522106</v>
+        <v>1.091089451179962</v>
       </c>
       <c r="L7" s="1">
         <f>MIN(G2:G44)</f>
@@ -2853,18 +2800,18 @@
       </c>
       <c r="M7" s="1">
         <f>AVERAGE(G2:G44)</f>
-        <v>0.12978335127285223</v>
+        <v>0.13319356304458946</v>
       </c>
       <c r="N7" s="1">
         <f>_xlfn.STDEV.P(G2:G44)</f>
-        <v>0.1986873838748909</v>
+        <v>0.21273143541591003</v>
       </c>
       <c r="O7" s="1">
         <f>N7/SQRT(COUNT(G2:G44))</f>
-        <v>3.1415233769243329E-2</v>
-      </c>
-    </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.2">
+        <v>3.3635793291564228E-2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
       <c r="B8" s="2" t="s">
         <v>34</v>
       </c>
@@ -2878,13 +2825,13 @@
         <v>5.4897240164415733</v>
       </c>
       <c r="F8" s="1">
-        <v>7.8605818746873801</v>
+        <v>7.8609665467801353</v>
       </c>
       <c r="G8" s="1">
-        <v>7.7762774327540848E-2</v>
-      </c>
-    </row>
-    <row r="9" spans="1:15" x14ac:dyDescent="0.2">
+        <v>7.7766579792532611E-2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
       <c r="B9" s="2" t="s">
         <v>35</v>
       </c>
@@ -2898,13 +2845,13 @@
         <v>7.4798459872458185</v>
       </c>
       <c r="F9" s="1">
-        <v>12.381214564610293</v>
+        <v>12.381462861786957</v>
       </c>
       <c r="G9" s="1">
-        <v>7.8410817433920935E-2</v>
-      </c>
-    </row>
-    <row r="10" spans="1:15" x14ac:dyDescent="0.2">
+        <v>7.8412389911684505E-2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:15" x14ac:dyDescent="0.25">
       <c r="B10" s="2" t="s">
         <v>36</v>
       </c>
@@ -2918,13 +2865,13 @@
         <v>6.2107703369449334</v>
       </c>
       <c r="F10" s="1">
-        <v>9.6146634593614149</v>
+        <v>9.6147826526057738</v>
       </c>
       <c r="G10" s="1">
-        <v>4.7874452915207498E-2</v>
-      </c>
-    </row>
-    <row r="11" spans="1:15" x14ac:dyDescent="0.2">
+        <v>4.7875046416102143E-2</v>
+      </c>
+    </row>
+    <row r="11" spans="1:15" x14ac:dyDescent="0.25">
       <c r="B11" s="2" t="s">
         <v>37</v>
       </c>
@@ -2938,23 +2885,18 @@
         <v>3.8083670715249665</v>
       </c>
       <c r="F11" s="1">
-        <v>4.5229640664314541</v>
+        <v>4.523472807681185</v>
       </c>
       <c r="G11" s="1">
-        <v>6.7832591331493622E-2</v>
-      </c>
-    </row>
-    <row r="12" spans="1:15" x14ac:dyDescent="0.2">
+        <v>6.7840221115144261E-2</v>
+      </c>
+    </row>
+    <row r="12" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="C12" s="1"/>
-      <c r="D12" s="1"/>
-      <c r="E12" s="1"/>
-      <c r="F12" s="1"/>
-      <c r="G12" s="1"/>
-    </row>
-    <row r="13" spans="1:15" x14ac:dyDescent="0.2">
+    </row>
+    <row r="13" spans="1:15" x14ac:dyDescent="0.25">
       <c r="B13" s="2" t="s">
         <v>39</v>
       </c>
@@ -2968,13 +2910,13 @@
         <v>8.6689450712344556</v>
       </c>
       <c r="F13" s="1">
-        <v>6.2425655968937361</v>
+        <v>6.2425977276161326</v>
       </c>
       <c r="G13" s="1">
-        <v>2.0028808934777147E-2</v>
-      </c>
-    </row>
-    <row r="14" spans="1:15" x14ac:dyDescent="0.2">
+        <v>2.0028912023817992E-2</v>
+      </c>
+    </row>
+    <row r="14" spans="1:15" x14ac:dyDescent="0.25">
       <c r="B14" s="2" t="s">
         <v>40</v>
       </c>
@@ -2988,13 +2930,13 @@
         <v>4.4476767819586076</v>
       </c>
       <c r="F14" s="1">
-        <v>2.6009677552876411</v>
+        <v>2.6009907400548991</v>
       </c>
       <c r="G14" s="1">
-        <v>1.0934518376390015E-2</v>
-      </c>
-    </row>
-    <row r="15" spans="1:15" x14ac:dyDescent="0.2">
+        <v>1.0934615004792828E-2</v>
+      </c>
+    </row>
+    <row r="15" spans="1:15" x14ac:dyDescent="0.25">
       <c r="B15" s="2" t="s">
         <v>41</v>
       </c>
@@ -3008,13 +2950,13 @@
         <v>7.9259259259259256</v>
       </c>
       <c r="F15" s="1">
-        <v>5.5850218986873266</v>
+        <v>5.5885917436658819</v>
       </c>
       <c r="G15" s="1">
-        <v>0.19959239949754212</v>
-      </c>
-    </row>
-    <row r="16" spans="1:15" x14ac:dyDescent="0.2">
+        <v>0.19971997534917335</v>
+      </c>
+    </row>
+    <row r="16" spans="1:15" x14ac:dyDescent="0.25">
       <c r="B16" s="2" t="s">
         <v>42</v>
       </c>
@@ -3028,13 +2970,13 @@
         <v>3.5445411922304086</v>
       </c>
       <c r="F16" s="1">
-        <v>2.0264969512222923</v>
+        <v>2.0268363695231777</v>
       </c>
       <c r="G16" s="1">
-        <v>3.7085236505680616E-2</v>
-      </c>
-    </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.2">
+        <v>3.7091447917918415E-2</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B17" s="2" t="s">
         <v>43</v>
       </c>
@@ -3048,13 +2990,13 @@
         <v>6.7106768350810295</v>
       </c>
       <c r="F17" s="1">
-        <v>4.8450431087740613</v>
+        <v>4.8461982031065469</v>
       </c>
       <c r="G17" s="1">
-        <v>0.1057778909528467</v>
-      </c>
-    </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.2">
+        <v>0.10580310918921712</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B18" s="2" t="s">
         <v>44</v>
       </c>
@@ -3068,13 +3010,13 @@
         <v>4.0071630537229028</v>
       </c>
       <c r="F18" s="1">
-        <v>2.3911448247331193</v>
+        <v>2.3913702236896208</v>
       </c>
       <c r="G18" s="1">
-        <v>3.2829418236729496E-2</v>
-      </c>
-    </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.2">
+        <v>3.2832512870118735E-2</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B19" s="2" t="s">
         <v>45</v>
       </c>
@@ -3088,13 +3030,13 @@
         <v>4.9600515463917523</v>
       </c>
       <c r="F19" s="1">
-        <v>2.6042099139073804</v>
+        <v>2.6050493047152883</v>
       </c>
       <c r="G19" s="1">
-        <v>6.6104363732220284E-2</v>
-      </c>
-    </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.2">
+        <v>6.6125670538166717E-2</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B20" s="2" t="s">
         <v>46</v>
       </c>
@@ -3108,13 +3050,13 @@
         <v>9.3811509591326097</v>
       </c>
       <c r="F20" s="1">
-        <v>4.384096985258755</v>
+        <v>4.3841985571553277</v>
       </c>
       <c r="G20" s="1">
-        <v>2.9842438598646541E-2</v>
-      </c>
-    </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.2">
+        <v>2.9843129996007731E-2</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B21" s="2" t="s">
         <v>47</v>
       </c>
@@ -3128,13 +3070,13 @@
         <v>1.3028588445503275E-3</v>
       </c>
       <c r="F21" s="1">
-        <v>3.6071614926164654E-2</v>
+        <v>3.6072286319516707E-2</v>
       </c>
       <c r="G21" s="1">
-        <v>2.2007983243639502E-4</v>
-      </c>
-    </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.2">
+        <v>2.2008392873584603E-4</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B22" s="2" t="s">
         <v>48</v>
       </c>
@@ -3148,23 +3090,18 @@
         <v>5.5378603795888881E-2</v>
       </c>
       <c r="F22" s="1">
-        <v>0.58418508482178866</v>
+        <v>0.58418988051593701</v>
       </c>
       <c r="G22" s="1">
-        <v>2.367081956829979E-3</v>
-      </c>
-    </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.2">
+        <v>2.3671013886870807E-3</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A23" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="C23" s="1"/>
-      <c r="D23" s="1"/>
-      <c r="E23" s="1"/>
-      <c r="F23" s="1"/>
-      <c r="G23" s="1"/>
-    </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.2">
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B24" s="2" t="s">
         <v>17</v>
       </c>
@@ -3178,13 +3115,13 @@
         <v>6.9038320446977819</v>
       </c>
       <c r="F24" s="1">
-        <v>4.1773709170154349</v>
+        <v>4.1774888002973007</v>
       </c>
       <c r="G24" s="1">
-        <v>3.1382203534861076E-2</v>
-      </c>
-    </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.2">
+        <v>3.138308912467782E-2</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B25" s="2" t="s">
         <v>18</v>
       </c>
@@ -3198,13 +3135,13 @@
         <v>4.2470784641068446</v>
       </c>
       <c r="F25" s="1">
-        <v>3.0120604507743272</v>
+        <v>3.0133183587225751</v>
       </c>
       <c r="G25" s="1">
-        <v>8.7023245216123785E-2</v>
-      </c>
-    </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.2">
+        <v>8.7059588189191128E-2</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B26" s="2" t="s">
         <v>19</v>
       </c>
@@ -3218,13 +3155,13 @@
         <v>4.9276018099547514</v>
       </c>
       <c r="F26" s="1">
-        <v>3.4906738247717946</v>
+        <v>3.4926498644572446</v>
       </c>
       <c r="G26" s="1">
-        <v>0.11740406573195188</v>
-      </c>
-    </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.2">
+        <v>0.11747052713876484</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B27" s="2" t="s">
         <v>20</v>
       </c>
@@ -3238,13 +3175,13 @@
         <v>4.5759999999999996</v>
       </c>
       <c r="F27" s="1">
-        <v>3.3015487274913875</v>
+        <v>3.3081717005016529</v>
       </c>
       <c r="G27" s="1">
-        <v>0.20880827569806712</v>
-      </c>
-    </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.2">
+        <v>0.20922714928995231</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B28" s="2" t="s">
         <v>21</v>
       </c>
@@ -3258,13 +3195,13 @@
         <v>3.5555555555555554</v>
       </c>
       <c r="F28" s="1">
-        <v>2.6293687924887181</v>
+        <v>2.7888667551135855</v>
       </c>
       <c r="G28" s="1">
-        <v>0.87645626416290601</v>
-      </c>
-    </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.2">
+        <v>0.9296222517045285</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B29" s="2" t="s">
         <v>22</v>
       </c>
@@ -3278,13 +3215,13 @@
         <v>5.6591928251121075</v>
       </c>
       <c r="F29" s="1">
-        <v>2.4793002424606447</v>
+        <v>2.4811553121122221</v>
       </c>
       <c r="G29" s="1">
-        <v>9.5855285265869478E-2</v>
-      </c>
-    </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.2">
+        <v>9.59270064021783E-2</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B30" s="2" t="s">
         <v>23</v>
       </c>
@@ -3298,13 +3235,13 @@
         <v>4.5839909808342725</v>
       </c>
       <c r="F30" s="1">
-        <v>3.5539794092547603</v>
+        <v>3.5559844753715319</v>
       </c>
       <c r="G30" s="1">
-        <v>0.11933094980848359</v>
-      </c>
-    </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.2">
+        <v>0.11939827333982429</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B31" s="2" t="s">
         <v>24</v>
       </c>
@@ -3318,13 +3255,13 @@
         <v>2.088142470694319</v>
       </c>
       <c r="F31" s="1">
-        <v>5.8113670889284741</v>
+        <v>5.8120222230367409</v>
       </c>
       <c r="G31" s="1">
-        <v>8.7253436509172985E-2</v>
-      </c>
-    </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.2">
+        <v>8.7263272869782443E-2</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B32" s="2" t="s">
         <v>25</v>
       </c>
@@ -3338,13 +3275,13 @@
         <v>4.2267466723686322</v>
       </c>
       <c r="F32" s="1">
-        <v>4.5735202024716397</v>
+        <v>4.5735507629974004</v>
       </c>
       <c r="G32" s="1">
-        <v>1.6719317035134778E-2</v>
-      </c>
-    </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.2">
+        <v>1.6719428754575459E-2</v>
+      </c>
+    </row>
+    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B33" s="2" t="s">
         <v>26</v>
       </c>
@@ -3358,23 +3295,18 @@
         <v>5.1269121813031164</v>
       </c>
       <c r="F33" s="1">
-        <v>3.672312119233569</v>
+        <v>3.6728323872986905</v>
       </c>
       <c r="G33" s="1">
-        <v>6.1809073430821614E-2</v>
-      </c>
-    </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.2">
+        <v>6.1817830117616393E-2</v>
+      </c>
+    </row>
+    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A34" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="C34" s="1"/>
-      <c r="D34" s="1"/>
-      <c r="E34" s="1"/>
-      <c r="F34" s="1"/>
-      <c r="G34" s="1"/>
-    </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.2">
+    </row>
+    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B35" s="2" t="s">
         <v>1</v>
       </c>
@@ -3388,13 +3320,13 @@
         <v>10.22851201478743</v>
       </c>
       <c r="F35" s="1">
-        <v>7.3361295370529866</v>
+        <v>7.3362354792960955</v>
       </c>
       <c r="G35" s="1">
-        <v>3.9425605476090586E-2</v>
-      </c>
-    </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.2">
+        <v>3.9426174827689273E-2</v>
+      </c>
+    </row>
+    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B36" s="2" t="s">
         <v>2</v>
       </c>
@@ -3414,7 +3346,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B37" s="2" t="s">
         <v>3</v>
       </c>
@@ -3428,13 +3360,13 @@
         <v>9.1760493507613994</v>
       </c>
       <c r="F37" s="1">
-        <v>3.8571206699815552</v>
+        <v>3.8572038684084582</v>
       </c>
       <c r="G37" s="1">
-        <v>2.5333613617020082E-2</v>
-      </c>
-    </row>
-    <row r="38" spans="1:7" x14ac:dyDescent="0.2">
+        <v>2.5334160065259854E-2</v>
+      </c>
+    </row>
+    <row r="38" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B38" s="2" t="s">
         <v>4</v>
       </c>
@@ -3448,13 +3380,13 @@
         <v>8.0545454545454547</v>
       </c>
       <c r="F38" s="1">
-        <v>4.5947046159327964</v>
+        <v>4.6006834143187767</v>
       </c>
       <c r="G38" s="1">
-        <v>0.23416783029956437</v>
-      </c>
-    </row>
-    <row r="39" spans="1:7" x14ac:dyDescent="0.2">
+        <v>0.23447253808012306</v>
+      </c>
+    </row>
+    <row r="39" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B39" s="2" t="s">
         <v>5</v>
       </c>
@@ -3468,13 +3400,13 @@
         <v>8.601272931486335</v>
       </c>
       <c r="F39" s="1">
-        <v>7.2066973424939667</v>
+        <v>7.2080467849442353</v>
       </c>
       <c r="G39" s="1">
-        <v>0.13944384181171246</v>
-      </c>
-    </row>
-    <row r="40" spans="1:7" x14ac:dyDescent="0.2">
+        <v>0.13946995244611635</v>
+      </c>
+    </row>
+    <row r="40" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B40" s="2" t="s">
         <v>6</v>
       </c>
@@ -3488,13 +3420,13 @@
         <v>7</v>
       </c>
       <c r="F40" s="1">
-        <v>2.6726124191242437</v>
+        <v>2.8867513459481291</v>
       </c>
       <c r="G40" s="1">
-        <v>1.0101525445522106</v>
-      </c>
-    </row>
-    <row r="41" spans="1:7" x14ac:dyDescent="0.2">
+        <v>1.091089451179962</v>
+      </c>
+    </row>
+    <row r="41" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B41" s="2" t="s">
         <v>7</v>
       </c>
@@ -3508,13 +3440,13 @@
         <v>8.1993410214168048</v>
       </c>
       <c r="F41" s="1">
-        <v>3.2730942834696939</v>
+        <v>3.2757937431314099</v>
       </c>
       <c r="G41" s="1">
-        <v>0.13285079880130551</v>
-      </c>
-    </row>
-    <row r="42" spans="1:7" x14ac:dyDescent="0.2">
+        <v>0.1329603664890443</v>
+      </c>
+    </row>
+    <row r="42" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B42" s="2" t="s">
         <v>8</v>
       </c>
@@ -3528,13 +3460,13 @@
         <v>6.756756756756757</v>
       </c>
       <c r="F42" s="1">
-        <v>2.7841773534434404</v>
+        <v>2.7936312935632373</v>
       </c>
       <c r="G42" s="1">
-        <v>0.22885796869230571</v>
-      </c>
-    </row>
-    <row r="43" spans="1:7" x14ac:dyDescent="0.2">
+        <v>0.22963507778317577</v>
+      </c>
+    </row>
+    <row r="43" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B43" s="2" t="s">
         <v>9</v>
       </c>
@@ -3548,13 +3480,13 @@
         <v>6.4656669297553275</v>
       </c>
       <c r="F43" s="1">
-        <v>5.2956219733665071</v>
+        <v>5.2977130383930611</v>
       </c>
       <c r="G43" s="1">
-        <v>0.14877455780064802</v>
-      </c>
-    </row>
-    <row r="44" spans="1:7" x14ac:dyDescent="0.2">
+        <v>0.14883330392645205</v>
+      </c>
+    </row>
+    <row r="44" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B44" s="2" t="s">
         <v>10</v>
       </c>
@@ -3568,10 +3500,10 @@
         <v>9.2340894770006301</v>
       </c>
       <c r="F44" s="1">
-        <v>3.5478132778340687</v>
+        <v>3.5483722967105913</v>
       </c>
       <c r="G44" s="1">
-        <v>6.2973421980902292E-2</v>
+        <v>6.2983344524410012E-2</v>
       </c>
     </row>
   </sheetData>
@@ -3583,16 +3515,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AE15F7AD-A0DC-4382-9A54-4AAD142EDBC9}">
   <dimension ref="A1:O44"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="J26" sqref="J26"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="P30" sqref="P30"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="20.83203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="20.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>27</v>
       </c>
@@ -3612,7 +3544,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
       <c r="B2" s="2" t="s">
         <v>28</v>
       </c>
@@ -3626,10 +3558,10 @@
         <v>1.2473271560940842E-3</v>
       </c>
       <c r="F2" s="1">
-        <v>3.529548598701758E-2</v>
+        <v>3.5298631051491371E-2</v>
       </c>
       <c r="G2" s="1">
-        <v>4.7115123618556541E-4</v>
+        <v>4.7119321891999369E-4</v>
       </c>
       <c r="K2" s="2" t="s">
         <v>11</v>
@@ -3647,7 +3579,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
       <c r="B3" s="2" t="s">
         <v>29</v>
       </c>
@@ -3690,7 +3622,7 @@
         <v>0.49598387070548977</v>
       </c>
     </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
       <c r="B4" s="2" t="s">
         <v>30</v>
       </c>
@@ -3733,7 +3665,7 @@
         <v>2.4685522072664372E-2</v>
       </c>
     </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
       <c r="B5" s="2" t="s">
         <v>31</v>
       </c>
@@ -3776,7 +3708,7 @@
         <v>8.3685620738454619E-2</v>
       </c>
     </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
       <c r="B6" s="2" t="s">
         <v>32</v>
       </c>
@@ -3800,7 +3732,7 @@
       </c>
       <c r="K6" s="1">
         <f>MAX(F2:F44)</f>
-        <v>1.7466921696279536</v>
+        <v>1.7468890798556946</v>
       </c>
       <c r="L6" s="1">
         <f>MIN(F2:F44)</f>
@@ -3808,18 +3740,18 @@
       </c>
       <c r="M6" s="1">
         <f>AVERAGE(F2:F44)</f>
-        <v>0.13758902505641976</v>
+        <v>0.1376163209383269</v>
       </c>
       <c r="N6" s="1">
         <f>_xlfn.STDEV.P(F2:F44)</f>
-        <v>0.36520258887600243</v>
+        <v>0.3652619777127506</v>
       </c>
       <c r="O6" s="1">
         <f>N6/SQRT(COUNT(F2:F44))</f>
-        <v>5.7743599411911976E-2</v>
-      </c>
-    </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.2">
+        <v>5.7752989611497579E-2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
       <c r="B7" s="2" t="s">
         <v>33</v>
       </c>
@@ -3833,17 +3765,17 @@
         <v>9.7646714188067565E-5</v>
       </c>
       <c r="F7" s="1">
-        <v>9.8811527317047305E-3</v>
+        <v>9.8816351980867811E-3</v>
       </c>
       <c r="G7" s="1">
-        <v>9.7641946631284803E-5</v>
+        <v>9.7646714188067565E-5</v>
       </c>
       <c r="J7" s="2" t="s">
         <v>15</v>
       </c>
       <c r="K7" s="1">
         <f>MAX(G2:G44)</f>
-        <v>3.3701282815944256E-2</v>
+        <v>3.3722824066348238E-2</v>
       </c>
       <c r="L7" s="1">
         <f>MIN(G2:G44)</f>
@@ -3851,18 +3783,18 @@
       </c>
       <c r="M7" s="1">
         <f>AVERAGE(G2:G44)</f>
-        <v>2.2028238529402367E-3</v>
+        <v>2.2036488696751946E-3</v>
       </c>
       <c r="N7" s="1">
         <f>_xlfn.STDEV.P(G2:G44)</f>
-        <v>6.7820694223171656E-3</v>
+        <v>6.7850825477001608E-3</v>
       </c>
       <c r="O7" s="1">
         <f>N7/SQRT(COUNT(G2:G44))</f>
-        <v>1.0723393311952319E-3</v>
-      </c>
-    </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.2">
+        <v>1.0728157481495284E-3</v>
+      </c>
+    </row>
+    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
       <c r="B8" s="2" t="s">
         <v>34</v>
       </c>
@@ -3876,13 +3808,13 @@
         <v>1.9573302016050108E-4</v>
       </c>
       <c r="F8" s="1">
-        <v>1.3989092491842346E-2</v>
+        <v>1.3989777073921685E-2</v>
       </c>
       <c r="G8" s="1">
-        <v>1.3839060006400557E-4</v>
-      </c>
-    </row>
-    <row r="9" spans="1:15" x14ac:dyDescent="0.2">
+        <v>1.3839737246363107E-4</v>
+      </c>
+    </row>
+    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
       <c r="B9" s="2" t="s">
         <v>35</v>
       </c>
@@ -3896,13 +3828,13 @@
         <v>4.0107488068022298E-5</v>
       </c>
       <c r="F9" s="1">
-        <v>6.3329202945736794E-3</v>
+        <v>6.3330472971565828E-3</v>
       </c>
       <c r="G9" s="1">
-        <v>4.0106683754657913E-5</v>
-      </c>
-    </row>
-    <row r="10" spans="1:15" x14ac:dyDescent="0.2">
+        <v>4.0107488068022305E-5</v>
+      </c>
+    </row>
+    <row r="10" spans="1:15" x14ac:dyDescent="0.25">
       <c r="B10" s="2" t="s">
         <v>36</v>
       </c>
@@ -3922,7 +3854,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:15" x14ac:dyDescent="0.25">
       <c r="B11" s="2" t="s">
         <v>37</v>
       </c>
@@ -3942,17 +3874,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="C12" s="1"/>
-      <c r="D12" s="1"/>
-      <c r="E12" s="1"/>
-      <c r="F12" s="1"/>
-      <c r="G12" s="1"/>
-    </row>
-    <row r="13" spans="1:15" x14ac:dyDescent="0.2">
+    </row>
+    <row r="13" spans="1:15" x14ac:dyDescent="0.25">
       <c r="B13" s="2" t="s">
         <v>39</v>
       </c>
@@ -3972,7 +3899,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:15" x14ac:dyDescent="0.25">
       <c r="B14" s="2" t="s">
         <v>40</v>
       </c>
@@ -3992,7 +3919,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:15" x14ac:dyDescent="0.25">
       <c r="B15" s="2" t="s">
         <v>41</v>
       </c>
@@ -4006,13 +3933,13 @@
         <v>0.36909323116219667</v>
       </c>
       <c r="F15" s="1">
-        <v>0.94303391819898141</v>
+        <v>0.94363668842236781</v>
       </c>
       <c r="G15" s="1">
-        <v>3.3701282815944256E-2</v>
-      </c>
-    </row>
-    <row r="16" spans="1:15" x14ac:dyDescent="0.2">
+        <v>3.3722824066348238E-2</v>
+      </c>
+    </row>
+    <row r="16" spans="1:15" x14ac:dyDescent="0.25">
       <c r="B16" s="2" t="s">
         <v>42</v>
       </c>
@@ -4032,7 +3959,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B17" s="2" t="s">
         <v>43</v>
       </c>
@@ -4046,13 +3973,13 @@
         <v>6.6730219256434702E-3</v>
       </c>
       <c r="F17" s="1">
-        <v>9.238544472515324E-2</v>
+        <v>9.2407470102680411E-2</v>
       </c>
       <c r="G17" s="1">
-        <v>2.0169763773763812E-3</v>
-      </c>
-    </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.2">
+        <v>2.0174572395544794E-3</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B18" s="2" t="s">
         <v>44</v>
       </c>
@@ -4072,7 +3999,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B19" s="2" t="s">
         <v>45</v>
       </c>
@@ -4092,7 +4019,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B20" s="2" t="s">
         <v>46</v>
       </c>
@@ -4112,7 +4039,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B21" s="2" t="s">
         <v>47</v>
       </c>
@@ -4126,13 +4053,13 @@
         <v>2.0328692674210838</v>
       </c>
       <c r="F21" s="1">
-        <v>1.0349386412958448</v>
+        <v>1.0349579043902468</v>
       </c>
       <c r="G21" s="1">
-        <v>6.3143589003309868E-3</v>
-      </c>
-    </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.2">
+        <v>6.3144764281599149E-3</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B22" s="2" t="s">
         <v>48</v>
       </c>
@@ -4146,23 +4073,18 @@
         <v>1.8523018322716227</v>
       </c>
       <c r="F22" s="1">
-        <v>0.93557938296030063</v>
+        <v>0.93558706332169417</v>
       </c>
       <c r="G22" s="1">
-        <v>3.7909099943266027E-3</v>
-      </c>
-    </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.2">
+        <v>3.790941114677582E-3</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A23" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="C23" s="1"/>
-      <c r="D23" s="1"/>
-      <c r="E23" s="1"/>
-      <c r="F23" s="1"/>
-      <c r="G23" s="1"/>
-    </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.2">
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B24" s="2" t="s">
         <v>17</v>
       </c>
@@ -4182,7 +4104,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B25" s="2" t="s">
         <v>18</v>
       </c>
@@ -4196,13 +4118,13 @@
         <v>3.3388981636060101E-3</v>
       </c>
       <c r="F25" s="1">
-        <v>8.1649544311435618E-2</v>
+        <v>8.1683643099437625E-2</v>
       </c>
       <c r="G25" s="1">
-        <v>2.3589859607805017E-3</v>
-      </c>
-    </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.2">
+        <v>2.3599711293182408E-3</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B26" s="2" t="s">
         <v>19</v>
       </c>
@@ -4216,13 +4138,13 @@
         <v>0.15158371040723981</v>
       </c>
       <c r="F26" s="1">
-        <v>0.35861691140604879</v>
+        <v>0.35881992127875101</v>
       </c>
       <c r="G26" s="1">
-        <v>1.2061591988491745E-2</v>
-      </c>
-    </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.2">
+        <v>1.2068419949405716E-2</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B27" s="2" t="s">
         <v>20</v>
       </c>
@@ -4242,7 +4164,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B28" s="2" t="s">
         <v>21</v>
       </c>
@@ -4262,7 +4184,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B29" s="2" t="s">
         <v>22</v>
       </c>
@@ -4282,7 +4204,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B30" s="2" t="s">
         <v>23</v>
       </c>
@@ -4302,7 +4224,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B31" s="2" t="s">
         <v>24</v>
       </c>
@@ -4316,13 +4238,13 @@
         <v>2.1368349864743013</v>
       </c>
       <c r="F31" s="1">
-        <v>1.7466921696279536</v>
+        <v>1.7468890798556946</v>
       </c>
       <c r="G31" s="1">
-        <v>2.6225308432856777E-2</v>
-      </c>
-    </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.2">
+        <v>2.622826489624849E-2</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B32" s="2" t="s">
         <v>25</v>
       </c>
@@ -4336,13 +4258,13 @@
         <v>3.2768482386272516E-2</v>
       </c>
       <c r="F32" s="1">
-        <v>0.24516633822593475</v>
+        <v>0.24516797644154623</v>
       </c>
       <c r="G32" s="1">
-        <v>8.9624918086669446E-4</v>
-      </c>
-    </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.2">
+        <v>8.9625516965541037E-4</v>
+      </c>
+    </row>
+    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B33" s="2" t="s">
         <v>26</v>
       </c>
@@ -4362,17 +4284,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A34" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="C34" s="1"/>
-      <c r="D34" s="1"/>
-      <c r="E34" s="1"/>
-      <c r="F34" s="1"/>
-      <c r="G34" s="1"/>
-    </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.2">
+    </row>
+    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B35" s="2" t="s">
         <v>1</v>
       </c>
@@ -4392,7 +4309,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B36" s="2" t="s">
         <v>2</v>
       </c>
@@ -4412,7 +4329,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B37" s="2" t="s">
         <v>3</v>
       </c>
@@ -4432,7 +4349,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="38" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B38" s="2" t="s">
         <v>4</v>
       </c>
@@ -4452,7 +4369,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="39" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B39" s="2" t="s">
         <v>5</v>
       </c>
@@ -4472,7 +4389,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="40" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B40" s="2" t="s">
         <v>6</v>
       </c>
@@ -4492,7 +4409,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="41" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B41" s="2" t="s">
         <v>7</v>
       </c>
@@ -4512,7 +4429,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="42" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B42" s="2" t="s">
         <v>8</v>
       </c>
@@ -4532,7 +4449,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="43" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B43" s="2" t="s">
         <v>9</v>
       </c>
@@ -4552,7 +4469,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="44" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B44" s="2" t="s">
         <v>10</v>
       </c>

</xml_diff>

<commit_message>
Tables for each language
</commit_message>
<xml_diff>
--- a/results/overall.xlsx
+++ b/results/overall.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10211"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D03BCCBF-59E9-4B66-AAF1-D523CBB6E38A}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8D8895FE-447C-ED4F-85F5-B4C015F430F3}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Length" sheetId="1" r:id="rId1"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="236" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="414" uniqueCount="55">
   <si>
     <t>Python</t>
   </si>
@@ -177,6 +177,24 @@
   <si>
     <t>spring-framework</t>
   </si>
+  <si>
+    <t>OVERALL</t>
+  </si>
+  <si>
+    <t>c++</t>
+  </si>
+  <si>
+    <t>java</t>
+  </si>
+  <si>
+    <t>javascript</t>
+  </si>
+  <si>
+    <t>python</t>
+  </si>
+  <si>
+    <t>overall</t>
+  </si>
 </sst>
 </file>
 
@@ -252,9 +270,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Calculation" xfId="1" builtinId="22"/>
@@ -538,23 +554,23 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:O44"/>
   <sheetViews>
-    <sheetView topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="C44" sqref="C44:G44"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="J10" sqref="J10:O39"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="9.42578125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="20.85546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="9.5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="20.83203125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="6" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="4.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="4.83203125" bestFit="1" customWidth="1"/>
     <col min="5" max="7" width="12" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="9" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="11" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="12" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
         <v>27</v>
       </c>
@@ -575,7 +591,7 @@
       </c>
       <c r="J1" s="2"/>
     </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:15" x14ac:dyDescent="0.2">
       <c r="B2" s="2" t="s">
         <v>28</v>
       </c>
@@ -594,6 +610,9 @@
       <c r="G2" s="1">
         <v>0.53032227530300591</v>
       </c>
+      <c r="J2" s="2" t="s">
+        <v>54</v>
+      </c>
       <c r="K2" s="2" t="s">
         <v>11</v>
       </c>
@@ -610,7 +629,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:15" x14ac:dyDescent="0.2">
       <c r="B3" s="2" t="s">
         <v>29</v>
       </c>
@@ -653,7 +672,7 @@
         <v>573.32221149114957</v>
       </c>
     </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:15" x14ac:dyDescent="0.2">
       <c r="B4" s="2" t="s">
         <v>30</v>
       </c>
@@ -696,7 +715,7 @@
         <v>0.64940801444913587</v>
       </c>
     </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:15" x14ac:dyDescent="0.2">
       <c r="B5" s="2" t="s">
         <v>31</v>
       </c>
@@ -739,7 +758,7 @@
         <v>12.357545642537358</v>
       </c>
     </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:15" x14ac:dyDescent="0.2">
       <c r="B6" s="2" t="s">
         <v>32</v>
       </c>
@@ -782,7 +801,7 @@
         <v>35.054848543107056</v>
       </c>
     </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:15" x14ac:dyDescent="0.2">
       <c r="B7" s="2" t="s">
         <v>33</v>
       </c>
@@ -825,7 +844,7 @@
         <v>1.0101366279194794</v>
       </c>
     </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:15" x14ac:dyDescent="0.2">
       <c r="B8" s="2" t="s">
         <v>34</v>
       </c>
@@ -845,7 +864,7 @@
         <v>0.25745772926382998</v>
       </c>
     </row>
-    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:15" x14ac:dyDescent="0.2">
       <c r="B9" s="2" t="s">
         <v>35</v>
       </c>
@@ -864,8 +883,13 @@
       <c r="G9" s="1">
         <v>0.28847691653342666</v>
       </c>
-    </row>
-    <row r="10" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="K9" s="2"/>
+      <c r="L9" s="2"/>
+      <c r="M9" s="2"/>
+      <c r="N9" s="2"/>
+      <c r="O9" s="2"/>
+    </row>
+    <row r="10" spans="1:15" x14ac:dyDescent="0.2">
       <c r="B10" s="2" t="s">
         <v>36</v>
       </c>
@@ -884,9 +908,26 @@
       <c r="G10" s="1">
         <v>0.23710589077502348</v>
       </c>
-      <c r="J10" s="2"/>
-    </row>
-    <row r="11" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="J10" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="K10" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="L10" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="M10" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="N10" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="O10" s="2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="11" spans="1:15" x14ac:dyDescent="0.2">
       <c r="B11" s="2" t="s">
         <v>37</v>
       </c>
@@ -905,19 +946,59 @@
       <c r="G11" s="1">
         <v>0.58027320067230792</v>
       </c>
-      <c r="K11" s="2"/>
-      <c r="L11" s="2"/>
-      <c r="M11" s="2"/>
-      <c r="N11" s="2"/>
-      <c r="O11" s="2"/>
-    </row>
-    <row r="12" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="J11" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="K11" s="1">
+        <f>MAX(C2:C11)</f>
+        <v>6888</v>
+      </c>
+      <c r="L11" s="1">
+        <f>MIN(C2:C11)</f>
+        <v>178</v>
+      </c>
+      <c r="M11" s="1">
+        <f>AVERAGE(C2:C11)</f>
+        <v>2096.9</v>
+      </c>
+      <c r="N11" s="1">
+        <f>_xlfn.STDEV.S(C2:C11)</f>
+        <v>2314.6637600788199</v>
+      </c>
+      <c r="O11" s="1">
+        <f>N11/SQRT(COUNT(C2:C11))</f>
+        <v>731.96094992985934</v>
+      </c>
+    </row>
+    <row r="12" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A12" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="J12" s="2"/>
-    </row>
-    <row r="13" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="J12" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="K12" s="1">
+        <f>MAX(D2:D11)</f>
+        <v>1</v>
+      </c>
+      <c r="L12" s="1">
+        <f>MIN(D2:D11)</f>
+        <v>1</v>
+      </c>
+      <c r="M12" s="1">
+        <f>AVERAGE(D2:D11)</f>
+        <v>1</v>
+      </c>
+      <c r="N12" s="1">
+        <f>STDEV(D2:D11)</f>
+        <v>0</v>
+      </c>
+      <c r="O12" s="1">
+        <f>N12/SQRT(COUNT(D2:D11))</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:15" x14ac:dyDescent="0.2">
       <c r="B13" s="2" t="s">
         <v>39</v>
       </c>
@@ -936,9 +1017,31 @@
       <c r="G13" s="1">
         <v>5.3991300325503956E-2</v>
       </c>
-      <c r="J13" s="2"/>
-    </row>
-    <row r="14" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="J13" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="K13" s="1">
+        <f>MAX(E2:E11)</f>
+        <v>22.472590510200206</v>
+      </c>
+      <c r="L13" s="1">
+        <f>MIN(E2:E11)</f>
+        <v>10.242315573770492</v>
+      </c>
+      <c r="M13" s="1">
+        <f>AVERAGE(E2:E11)</f>
+        <v>17.627433753873007</v>
+      </c>
+      <c r="N13" s="1">
+        <f>_xlfn.STDEV.S(E2:E11)</f>
+        <v>3.9345309004391047</v>
+      </c>
+      <c r="O13" s="1">
+        <f>N13/SQRT(COUNT(E2:E11))</f>
+        <v>1.2442079169700757</v>
+      </c>
+    </row>
+    <row r="14" spans="1:15" x14ac:dyDescent="0.2">
       <c r="B14" s="2" t="s">
         <v>40</v>
       </c>
@@ -957,9 +1060,31 @@
       <c r="G14" s="1">
         <v>4.9756248697386388E-2</v>
       </c>
-      <c r="J14" s="2"/>
-    </row>
-    <row r="15" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="J14" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="K14" s="1">
+        <f>MAX(F2:F11)</f>
+        <v>60.466210718311935</v>
+      </c>
+      <c r="L14" s="1">
+        <f>MIN(F2:F11)</f>
+        <v>14.287670468148708</v>
+      </c>
+      <c r="M14" s="1">
+        <f>AVERAGE(F2:F11)</f>
+        <v>36.262027035924248</v>
+      </c>
+      <c r="N14" s="1">
+        <f>_xlfn.STDEV.S(F2:F11)</f>
+        <v>14.069388918903972</v>
+      </c>
+      <c r="O14" s="1">
+        <f>N14/SQRT(COUNT(C2:C11))</f>
+        <v>4.4491314270470577</v>
+      </c>
+    </row>
+    <row r="15" spans="1:15" x14ac:dyDescent="0.2">
       <c r="B15" s="2" t="s">
         <v>41</v>
       </c>
@@ -978,9 +1103,31 @@
       <c r="G15" s="1">
         <v>0.40203741170819873</v>
       </c>
-      <c r="J15" s="2"/>
-    </row>
-    <row r="16" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="J15" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="K15" s="1">
+        <f>MAX(G2:G11)</f>
+        <v>0.81948513011774859</v>
+      </c>
+      <c r="L15" s="1">
+        <f>MIN(G2:G11)</f>
+        <v>0.22866859353139246</v>
+      </c>
+      <c r="M15" s="1">
+        <f>AVERAGE(G2:G11)</f>
+        <v>0.4099788062961231</v>
+      </c>
+      <c r="N15" s="1">
+        <f>_xlfn.STDEV.S(G2:G11)</f>
+        <v>0.18817906321048014</v>
+      </c>
+      <c r="O15" s="1">
+        <f>N15/SQRT(COUNT(F2:F11))</f>
+        <v>5.9507444770191466E-2</v>
+      </c>
+    </row>
+    <row r="16" spans="1:15" x14ac:dyDescent="0.2">
       <c r="B16" s="2" t="s">
         <v>42</v>
       </c>
@@ -1001,7 +1148,7 @@
       </c>
       <c r="J16" s="2"/>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:15" x14ac:dyDescent="0.2">
       <c r="B17" s="2" t="s">
         <v>43</v>
       </c>
@@ -1021,7 +1168,7 @@
         <v>0.50618824349864477</v>
       </c>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:15" x14ac:dyDescent="0.2">
       <c r="B18" s="2" t="s">
         <v>44</v>
       </c>
@@ -1040,8 +1187,26 @@
       <c r="G18" s="1">
         <v>0.16558280087741112</v>
       </c>
-    </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="J18" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="K18" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="L18" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="M18" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="N18" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="O18" s="2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="19" spans="1:15" x14ac:dyDescent="0.2">
       <c r="B19" s="2" t="s">
         <v>45</v>
       </c>
@@ -1060,8 +1225,31 @@
       <c r="G19" s="1">
         <v>0.35110448522871801</v>
       </c>
-    </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="J19" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="K19" s="1">
+        <f>MAX(C13:C22)</f>
+        <v>1133</v>
+      </c>
+      <c r="L19" s="1">
+        <f>MIN(C13:C22)</f>
+        <v>101</v>
+      </c>
+      <c r="M19" s="1">
+        <f>AVERAGE(C13:C22)</f>
+        <v>384.9</v>
+      </c>
+      <c r="N19" s="1">
+        <f>_xlfn.STDEV.S(C13:C22)</f>
+        <v>326.88987272304547</v>
+      </c>
+      <c r="O19" s="1">
+        <f>N19/SQRT(COUNT(C13:C22))</f>
+        <v>103.37165418473715</v>
+      </c>
+    </row>
+    <row r="20" spans="1:15" x14ac:dyDescent="0.2">
       <c r="B20" s="2" t="s">
         <v>46</v>
       </c>
@@ -1080,8 +1268,31 @@
       <c r="G20" s="1">
         <v>9.1828924731342174E-2</v>
       </c>
-    </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="J20" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="K20" s="1">
+        <f>MAX(D13:D22)</f>
+        <v>3</v>
+      </c>
+      <c r="L20" s="1">
+        <f>MIN(D13:D22)</f>
+        <v>1</v>
+      </c>
+      <c r="M20" s="1">
+        <f>AVERAGE(D13:D22)</f>
+        <v>1.3</v>
+      </c>
+      <c r="N20" s="1">
+        <f>_xlfn.STDEV.S(D13:D22)</f>
+        <v>0.67494855771055307</v>
+      </c>
+      <c r="O20" s="1">
+        <f>N20/SQRT(COUNT(D13:D22))</f>
+        <v>0.21343747458109499</v>
+      </c>
+    </row>
+    <row r="21" spans="1:15" x14ac:dyDescent="0.2">
       <c r="B21" s="2" t="s">
         <v>47</v>
       </c>
@@ -1100,8 +1311,31 @@
       <c r="G21" s="1">
         <v>3.1390597586767523E-2</v>
       </c>
-    </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="J21" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="K21" s="1">
+        <f>MAX(E13:E22)</f>
+        <v>16.149425287356323</v>
+      </c>
+      <c r="L21" s="1">
+        <f>MIN(E13:E22)</f>
+        <v>6.4846262656343061</v>
+      </c>
+      <c r="M21" s="1">
+        <f>AVERAGE(E13:E22)</f>
+        <v>10.32204070897629</v>
+      </c>
+      <c r="N21" s="1">
+        <f>_xlfn.STDEV.S(E13:E22)</f>
+        <v>3.0273801838887668</v>
+      </c>
+      <c r="O21" s="1">
+        <f>N21/SQRT(COUNT(E13:E22))</f>
+        <v>0.95734167243478874</v>
+      </c>
+    </row>
+    <row r="22" spans="1:15" x14ac:dyDescent="0.2">
       <c r="B22" s="2" t="s">
         <v>48</v>
       </c>
@@ -1120,13 +1354,59 @@
       <c r="G22" s="1">
         <v>4.6268266348847197E-2</v>
       </c>
-    </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="J22" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="K22" s="1">
+        <f>MAX(F13:F22)</f>
+        <v>23.185410852999745</v>
+      </c>
+      <c r="L22" s="1">
+        <f>MIN(F13:F22)</f>
+        <v>5.1449945954467173</v>
+      </c>
+      <c r="M22" s="1">
+        <f>AVERAGE(F13:F22)</f>
+        <v>12.57788724140371</v>
+      </c>
+      <c r="N22" s="1">
+        <f>_xlfn.STDEV.S(F13:F22)</f>
+        <v>5.0145958279608562</v>
+      </c>
+      <c r="O22" s="1">
+        <f>N22/SQRT(COUNT(F13:F22))</f>
+        <v>1.5857544361534173</v>
+      </c>
+    </row>
+    <row r="23" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A23" s="2" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="J23" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="K23" s="1">
+        <f>MAX(G13:G22)</f>
+        <v>0.50618824349864477</v>
+      </c>
+      <c r="L23" s="1">
+        <f>MIN(G13:G22)</f>
+        <v>3.1390597586767523E-2</v>
+      </c>
+      <c r="M23" s="1">
+        <f>AVERAGE(G13:G22)</f>
+        <v>0.1821378096401495</v>
+      </c>
+      <c r="N23" s="1">
+        <f>_xlfn.STDEV.S(G13:G22)</f>
+        <v>0.17286662519435531</v>
+      </c>
+      <c r="O23" s="1">
+        <f>N23/SQRT(COUNT(G13:G22))</f>
+        <v>5.4665226704081006E-2</v>
+      </c>
+    </row>
+    <row r="24" spans="1:15" x14ac:dyDescent="0.2">
       <c r="B24" s="2" t="s">
         <v>17</v>
       </c>
@@ -1146,7 +1426,7 @@
         <v>1.240095290234063</v>
       </c>
     </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:15" x14ac:dyDescent="0.2">
       <c r="B25" s="2" t="s">
         <v>18</v>
       </c>
@@ -1166,7 +1446,7 @@
         <v>40.275170275927344</v>
       </c>
     </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:15" x14ac:dyDescent="0.2">
       <c r="B26" s="2" t="s">
         <v>19</v>
       </c>
@@ -1185,8 +1465,26 @@
       <c r="G26" s="1">
         <v>2.218869734822043</v>
       </c>
-    </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="J26" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="K26" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="L26" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="M26" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="N26" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="O26" s="2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="27" spans="1:15" x14ac:dyDescent="0.2">
       <c r="B27" s="2" t="s">
         <v>20</v>
       </c>
@@ -1205,8 +1503,31 @@
       <c r="G27" s="1">
         <v>4.4033052864618796</v>
       </c>
-    </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="J27" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="K27" s="1">
+        <f>MAX(C24:C33)</f>
+        <v>16517</v>
+      </c>
+      <c r="L27" s="1">
+        <f>MIN(C24:C33)</f>
+        <v>11</v>
+      </c>
+      <c r="M27" s="1">
+        <f>AVERAGE(C24:C33)</f>
+        <v>5280.7</v>
+      </c>
+      <c r="N27" s="1">
+        <f>_xlfn.STDEV.S(C24:C33)</f>
+        <v>5786.0898531641287</v>
+      </c>
+      <c r="O27" s="1">
+        <f>N27/SQRT(COUNT(C24:C33))</f>
+        <v>1829.7222682387862</v>
+      </c>
+    </row>
+    <row r="28" spans="1:15" x14ac:dyDescent="0.2">
       <c r="B28" s="2" t="s">
         <v>21</v>
       </c>
@@ -1225,8 +1546,31 @@
       <c r="G28" s="1">
         <v>1.0423146132940955</v>
       </c>
-    </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="J28" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="K28" s="1">
+        <f>MAX(D24:D33)</f>
+        <v>3</v>
+      </c>
+      <c r="L28" s="1">
+        <f>MIN(D24:D33)</f>
+        <v>1</v>
+      </c>
+      <c r="M28" s="1">
+        <f>AVERAGE(D24:D33)</f>
+        <v>1.2</v>
+      </c>
+      <c r="N28" s="1">
+        <f>_xlfn.STDEV.S(D24:D33)</f>
+        <v>0.63245553203367588</v>
+      </c>
+      <c r="O28" s="1">
+        <f>N28/SQRT(COUNT(D24:D33))</f>
+        <v>0.19999999999999998</v>
+      </c>
+    </row>
+    <row r="29" spans="1:15" x14ac:dyDescent="0.2">
       <c r="B29" s="2" t="s">
         <v>22</v>
       </c>
@@ -1245,8 +1589,31 @@
       <c r="G29" s="1">
         <v>2.4820452487043485</v>
       </c>
-    </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="J29" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="K29" s="1">
+        <f>MAX(E24:E33)</f>
+        <v>505.93656093489147</v>
+      </c>
+      <c r="L29" s="1">
+        <f>MIN(E24:E33)</f>
+        <v>6.4444444444444446</v>
+      </c>
+      <c r="M29" s="1">
+        <f>AVERAGE(E24:E33)</f>
+        <v>77.744434447283155</v>
+      </c>
+      <c r="N29" s="1">
+        <f>_xlfn.STDEV.S(E24:E33)</f>
+        <v>151.62499167467928</v>
+      </c>
+      <c r="O29" s="1">
+        <f>N29/SQRT(COUNT(E24:E33))</f>
+        <v>47.948032389605473</v>
+      </c>
+    </row>
+    <row r="30" spans="1:15" x14ac:dyDescent="0.2">
       <c r="B30" s="2" t="s">
         <v>23</v>
       </c>
@@ -1265,8 +1632,31 @@
       <c r="G30" s="1">
         <v>1.8449917044592643</v>
       </c>
-    </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="J30" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="K30" s="1">
+        <f>MAX(F24:F33)</f>
+        <v>1394.0096951687317</v>
+      </c>
+      <c r="L30" s="1">
+        <f>MIN(F24:F33)</f>
+        <v>3.1269438398822866</v>
+      </c>
+      <c r="M30" s="1">
+        <f>AVERAGE(F24:F33)</f>
+        <v>247.99947116977992</v>
+      </c>
+      <c r="N30" s="1">
+        <f>_xlfn.STDEV.S(F24:F33)</f>
+        <v>411.87675890844605</v>
+      </c>
+      <c r="O30" s="1">
+        <f>N30/SQRT(COUNT(F24:F33))</f>
+        <v>130.24686734387365</v>
+      </c>
+    </row>
+    <row r="31" spans="1:15" x14ac:dyDescent="0.2">
       <c r="B31" s="2" t="s">
         <v>24</v>
       </c>
@@ -1285,8 +1675,31 @@
       <c r="G31" s="1">
         <v>2.961739256316164</v>
       </c>
-    </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="J31" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="K31" s="1">
+        <f>MAX(G24:G33)</f>
+        <v>40.275170275927344</v>
+      </c>
+      <c r="L31" s="1">
+        <f>MIN(G24:G33)</f>
+        <v>0.62649410093455704</v>
+      </c>
+      <c r="M31" s="1">
+        <f>AVERAGE(G24:G33)</f>
+        <v>6.2050229427189958</v>
+      </c>
+      <c r="N31" s="1">
+        <f>_xlfn.STDEV.S(G24:G33)</f>
+        <v>12.052136570024237</v>
+      </c>
+      <c r="O31" s="1">
+        <f>N31/SQRT(COUNT(G24:G33))</f>
+        <v>3.8112202232685997</v>
+      </c>
+    </row>
+    <row r="32" spans="1:15" x14ac:dyDescent="0.2">
       <c r="B32" s="2" t="s">
         <v>25</v>
       </c>
@@ -1306,7 +1719,7 @@
         <v>0.62649410093455704</v>
       </c>
     </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:15" x14ac:dyDescent="0.2">
       <c r="B33" s="2" t="s">
         <v>26</v>
       </c>
@@ -1326,12 +1739,30 @@
         <v>4.955203916036206</v>
       </c>
     </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A34" s="2" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="J34" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="K34" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="L34" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="M34" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="N34" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="O34" s="2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="35" spans="1:15" x14ac:dyDescent="0.2">
       <c r="B35" s="2" t="s">
         <v>1</v>
       </c>
@@ -1350,8 +1781,31 @@
       <c r="G35" s="1">
         <v>0.1560365281554825</v>
       </c>
-    </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="J35" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="K35" s="1">
+        <f>MAX(C35:C44)</f>
+        <v>1203</v>
+      </c>
+      <c r="L35" s="1">
+        <f>MIN(C35:C44)</f>
+        <v>24</v>
+      </c>
+      <c r="M35" s="1">
+        <f>AVERAGE(C35:C44)</f>
+        <v>368.2</v>
+      </c>
+      <c r="N35" s="1">
+        <f>_xlfn.STDEV.S(C35:C44)</f>
+        <v>457.63663412022521</v>
+      </c>
+      <c r="O35" s="1">
+        <f>N35/SQRT(COUNT(C35:C44))</f>
+        <v>144.71741045530385</v>
+      </c>
+    </row>
+    <row r="36" spans="1:15" x14ac:dyDescent="0.2">
       <c r="B36" s="2" t="s">
         <v>2</v>
       </c>
@@ -1370,8 +1824,31 @@
       <c r="G36" s="1">
         <v>2.9999999999999996</v>
       </c>
-    </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="J36" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="K36" s="1">
+        <f>MAX(D35:D44)</f>
+        <v>27</v>
+      </c>
+      <c r="L36" s="1">
+        <f>MIN(D35:D44)</f>
+        <v>2</v>
+      </c>
+      <c r="M36" s="1">
+        <f>AVERAGE(D35:D44)</f>
+        <v>4.7</v>
+      </c>
+      <c r="N36" s="1">
+        <f>_xlfn.STDEV.S(D35:D44)</f>
+        <v>7.8605908740303292</v>
+      </c>
+      <c r="O36" s="1">
+        <f>N36/SQRT(COUNT(D35:D44))</f>
+        <v>2.4857370916669543</v>
+      </c>
+    </row>
+    <row r="37" spans="1:15" x14ac:dyDescent="0.2">
       <c r="B37" s="2" t="s">
         <v>3</v>
       </c>
@@ -1390,8 +1867,31 @@
       <c r="G37" s="1">
         <v>8.9502898935907862E-2</v>
       </c>
-    </row>
-    <row r="38" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="J37" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="K37" s="1">
+        <f>MAX(E35:E44)</f>
+        <v>30</v>
+      </c>
+      <c r="L37" s="1">
+        <f>MIN(E35:E44)</f>
+        <v>4.4391891891891895</v>
+      </c>
+      <c r="M37" s="1">
+        <f>AVERAGE(E35:E44)</f>
+        <v>15.103251334857621</v>
+      </c>
+      <c r="N37" s="1">
+        <f>_xlfn.STDEV.S(E35:E44)</f>
+        <v>8.673119465234242</v>
+      </c>
+      <c r="O37" s="1">
+        <f>N37/SQRT(COUNT(E35:E44))</f>
+        <v>2.7426811928881762</v>
+      </c>
+    </row>
+    <row r="38" spans="1:15" x14ac:dyDescent="0.2">
       <c r="B38" s="2" t="s">
         <v>4</v>
       </c>
@@ -1410,8 +1910,31 @@
       <c r="G38" s="1">
         <v>0.64838139241743387</v>
       </c>
-    </row>
-    <row r="39" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="J38" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="K38" s="1">
+        <f>MAX(F35:F44)</f>
+        <v>43.976453542998279</v>
+      </c>
+      <c r="L38" s="1">
+        <f>MIN(F35:F44)</f>
+        <v>3.9074781807031815</v>
+      </c>
+      <c r="M38" s="1">
+        <f>AVERAGE(F35:F44)</f>
+        <v>16.702002972454782</v>
+      </c>
+      <c r="N38" s="1">
+        <f>_xlfn.STDEV.S(F35:F44)</f>
+        <v>12.544628687400948</v>
+      </c>
+      <c r="O38" s="1">
+        <f>N38/SQRT(COUNT(F35:F44))</f>
+        <v>3.9669599053275397</v>
+      </c>
+    </row>
+    <row r="39" spans="1:15" x14ac:dyDescent="0.2">
       <c r="B39" s="2" t="s">
         <v>5</v>
       </c>
@@ -1430,8 +1953,31 @@
       <c r="G39" s="1">
         <v>0.43035982152354263</v>
       </c>
-    </row>
-    <row r="40" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="J39" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="K39" s="1">
+        <f>MAX(G35:G44)</f>
+        <v>7.1538011398346351</v>
+      </c>
+      <c r="L39" s="1">
+        <f>MIN(G35:G44)</f>
+        <v>8.9502898935907862E-2</v>
+      </c>
+      <c r="M39" s="1">
+        <f>AVERAGE(G35:G44)</f>
+        <v>1.3255609397481263</v>
+      </c>
+      <c r="N39" s="1">
+        <f>_xlfn.STDEV.S(G35:G44)</f>
+        <v>2.2174017582105612</v>
+      </c>
+      <c r="O39" s="1">
+        <f>N39/SQRT(COUNT(G35:G44))</f>
+        <v>0.70120400436073438</v>
+      </c>
+    </row>
+    <row r="40" spans="1:15" x14ac:dyDescent="0.2">
       <c r="B40" s="2" t="s">
         <v>6</v>
       </c>
@@ -1451,7 +1997,7 @@
         <v>7.1538011398346351</v>
       </c>
     </row>
-    <row r="41" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:15" x14ac:dyDescent="0.2">
       <c r="B41" s="2" t="s">
         <v>7</v>
       </c>
@@ -1471,7 +2017,7 @@
         <v>0.52135146211890249</v>
       </c>
     </row>
-    <row r="42" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:15" x14ac:dyDescent="0.2">
       <c r="B42" s="2" t="s">
         <v>8</v>
       </c>
@@ -1491,7 +2037,7 @@
         <v>0.32119272791269149</v>
       </c>
     </row>
-    <row r="43" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:15" x14ac:dyDescent="0.2">
       <c r="B43" s="2" t="s">
         <v>9</v>
       </c>
@@ -1511,7 +2057,7 @@
         <v>0.15440464486125366</v>
       </c>
     </row>
-    <row r="44" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:15" x14ac:dyDescent="0.2">
       <c r="B44" s="2" t="s">
         <v>10</v>
       </c>
@@ -1541,16 +2087,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{74F2D45E-113D-4FBB-9FB8-E8607006C13E}">
   <dimension ref="A1:O44"/>
   <sheetViews>
-    <sheetView topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="C44" sqref="C44:G44"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="K11" sqref="K11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" width="20.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="20.83203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
         <v>27</v>
       </c>
@@ -1570,7 +2116,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:15" x14ac:dyDescent="0.2">
       <c r="B2" s="2" t="s">
         <v>28</v>
       </c>
@@ -1605,7 +2151,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:15" x14ac:dyDescent="0.2">
       <c r="B3" s="2" t="s">
         <v>29</v>
       </c>
@@ -1648,7 +2194,7 @@
         <v>35.200979508151946</v>
       </c>
     </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:15" x14ac:dyDescent="0.2">
       <c r="B4" s="2" t="s">
         <v>30</v>
       </c>
@@ -1691,7 +2237,7 @@
         <v>0.91559669488935336</v>
       </c>
     </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:15" x14ac:dyDescent="0.2">
       <c r="B5" s="2" t="s">
         <v>31</v>
       </c>
@@ -1734,7 +2280,7 @@
         <v>2.2649985477911434</v>
       </c>
     </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:15" x14ac:dyDescent="0.2">
       <c r="B6" s="2" t="s">
         <v>32</v>
       </c>
@@ -1777,7 +2323,7 @@
         <v>1.7184781823763902</v>
       </c>
     </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:15" x14ac:dyDescent="0.2">
       <c r="B7" s="2" t="s">
         <v>33</v>
       </c>
@@ -1820,7 +2366,7 @@
         <v>0.45930118046940072</v>
       </c>
     </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:15" x14ac:dyDescent="0.2">
       <c r="B8" s="2" t="s">
         <v>34</v>
       </c>
@@ -1840,7 +2386,7 @@
         <v>0.19876658175240999</v>
       </c>
     </row>
-    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:15" x14ac:dyDescent="0.2">
       <c r="B9" s="2" t="s">
         <v>35</v>
       </c>
@@ -1860,7 +2406,7 @@
         <v>7.775987596359131E-2</v>
       </c>
     </row>
-    <row r="10" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:15" x14ac:dyDescent="0.2">
       <c r="B10" s="2" t="s">
         <v>36</v>
       </c>
@@ -1879,13 +2425,26 @@
       <c r="G10" s="1">
         <v>6.0917824743992204E-2</v>
       </c>
-      <c r="K10" s="3"/>
-      <c r="L10" s="3"/>
-      <c r="M10" s="3"/>
-      <c r="N10" s="3"/>
-      <c r="O10" s="3"/>
-    </row>
-    <row r="11" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="J10" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="K10" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="L10" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="M10" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="N10" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="O10" s="2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="11" spans="1:15" x14ac:dyDescent="0.2">
       <c r="B11" s="2" t="s">
         <v>37</v>
       </c>
@@ -1904,13 +2463,59 @@
       <c r="G11" s="1">
         <v>0.53240525466797817</v>
       </c>
-    </row>
-    <row r="12" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="J11" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="K11" s="1">
+        <f>MAX(C2:C11)</f>
+        <v>933</v>
+      </c>
+      <c r="L11" s="1">
+        <f>MIN(C2:C11)</f>
+        <v>81</v>
+      </c>
+      <c r="M11" s="1">
+        <f>AVERAGE(C2:C11)</f>
+        <v>333.5</v>
+      </c>
+      <c r="N11" s="1">
+        <f>_xlfn.STDEV.S(C2:C11)</f>
+        <v>255.30123819171388</v>
+      </c>
+      <c r="O11" s="1">
+        <f>N11/SQRT(COUNT(C2:C11))</f>
+        <v>80.733340214698302</v>
+      </c>
+    </row>
+    <row r="12" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A12" s="2" t="s">
         <v>38</v>
       </c>
-    </row>
-    <row r="13" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="J12" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="K12" s="1">
+        <f>MAX(D2:D11)</f>
+        <v>17</v>
+      </c>
+      <c r="L12" s="1">
+        <f>MIN(D2:D11)</f>
+        <v>1</v>
+      </c>
+      <c r="M12" s="1">
+        <f>AVERAGE(D2:D11)</f>
+        <v>12.9</v>
+      </c>
+      <c r="N12" s="1">
+        <f>STDEV(D2:D11)</f>
+        <v>4.5080175490144478</v>
+      </c>
+      <c r="O12" s="1">
+        <f>N12/SQRT(COUNT(D2:D11))</f>
+        <v>1.42556031868954</v>
+      </c>
+    </row>
+    <row r="13" spans="1:15" x14ac:dyDescent="0.2">
       <c r="B13" s="2" t="s">
         <v>39</v>
       </c>
@@ -1929,8 +2534,31 @@
       <c r="G13" s="1">
         <v>0.10737507081825906</v>
       </c>
-    </row>
-    <row r="14" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="J13" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="K13" s="1">
+        <f>MAX(E2:E11)</f>
+        <v>85.162687099073409</v>
+      </c>
+      <c r="L13" s="1">
+        <f>MIN(E2:E11)</f>
+        <v>65.229252049180332</v>
+      </c>
+      <c r="M13" s="1">
+        <f>AVERAGE(E2:E11)</f>
+        <v>73.379172183388135</v>
+      </c>
+      <c r="N13" s="1">
+        <f>_xlfn.STDEV.S(E2:E11)</f>
+        <v>6.4579791045243162</v>
+      </c>
+      <c r="O13" s="1">
+        <f>N13/SQRT(COUNT(E2:E11))</f>
+        <v>2.042192305207144</v>
+      </c>
+    </row>
+    <row r="14" spans="1:15" x14ac:dyDescent="0.2">
       <c r="B14" s="2" t="s">
         <v>40</v>
       </c>
@@ -1949,8 +2577,31 @@
       <c r="G14" s="1">
         <v>0.1183772306024764</v>
       </c>
-    </row>
-    <row r="15" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="J14" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="K14" s="1">
+        <f>MAX(F2:F11)</f>
+        <v>43.782694516189167</v>
+      </c>
+      <c r="L14" s="1">
+        <f>MIN(F2:F11)</f>
+        <v>12.234173926273595</v>
+      </c>
+      <c r="M14" s="1">
+        <f>AVERAGE(F2:F11)</f>
+        <v>22.698461308970483</v>
+      </c>
+      <c r="N14" s="1">
+        <f>_xlfn.STDEV.S(F2:F11)</f>
+        <v>10.964506394333847</v>
+      </c>
+      <c r="O14" s="1">
+        <f>N14/SQRT(COUNT(C2:C11))</f>
+        <v>3.4672813625575269</v>
+      </c>
+    </row>
+    <row r="15" spans="1:15" x14ac:dyDescent="0.2">
       <c r="B15" s="2" t="s">
         <v>41</v>
       </c>
@@ -1969,8 +2620,31 @@
       <c r="G15" s="1">
         <v>0.91688198450172087</v>
       </c>
-    </row>
-    <row r="16" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="J15" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="K15" s="1">
+        <f>MAX(G2:G11)</f>
+        <v>0.58444500955235501</v>
+      </c>
+      <c r="L15" s="1">
+        <f>MIN(G2:G11)</f>
+        <v>6.0917824743992204E-2</v>
+      </c>
+      <c r="M15" s="1">
+        <f>AVERAGE(G2:G11)</f>
+        <v>0.29120556844182294</v>
+      </c>
+      <c r="N15" s="1">
+        <f>_xlfn.STDEV.S(G2:G11)</f>
+        <v>0.18811624876436409</v>
+      </c>
+      <c r="O15" s="1">
+        <f>N15/SQRT(COUNT(F2:F11))</f>
+        <v>5.9487581098222601E-2</v>
+      </c>
+    </row>
+    <row r="16" spans="1:15" x14ac:dyDescent="0.2">
       <c r="B16" s="2" t="s">
         <v>42</v>
       </c>
@@ -1989,8 +2663,9 @@
       <c r="G16" s="1">
         <v>0.43740864181692457</v>
       </c>
-    </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="J16" s="2"/>
+    </row>
+    <row r="17" spans="1:15" x14ac:dyDescent="0.2">
       <c r="B17" s="2" t="s">
         <v>43</v>
       </c>
@@ -2010,7 +2685,7 @@
         <v>0.62843209930286481</v>
       </c>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:15" x14ac:dyDescent="0.2">
       <c r="B18" s="2" t="s">
         <v>44</v>
       </c>
@@ -2029,8 +2704,26 @@
       <c r="G18" s="1">
         <v>0.26711491711986562</v>
       </c>
-    </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="J18" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="K18" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="L18" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="M18" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="N18" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="O18" s="2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="19" spans="1:15" x14ac:dyDescent="0.2">
       <c r="B19" s="2" t="s">
         <v>45</v>
       </c>
@@ -2049,8 +2742,31 @@
       <c r="G19" s="1">
         <v>0.50792381261195996</v>
       </c>
-    </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="J19" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="K19" s="1">
+        <f>MAX(C13:C22)</f>
+        <v>427</v>
+      </c>
+      <c r="L19" s="1">
+        <f>MIN(C13:C22)</f>
+        <v>121</v>
+      </c>
+      <c r="M19" s="1">
+        <f>AVERAGE(C13:C22)</f>
+        <v>231.2</v>
+      </c>
+      <c r="N19" s="1">
+        <f>_xlfn.STDEV.S(C13:C22)</f>
+        <v>90.506967196515362</v>
+      </c>
+      <c r="O19" s="1">
+        <f>N19/SQRT(COUNT(C13:C22))</f>
+        <v>28.620816045513283</v>
+      </c>
+    </row>
+    <row r="20" spans="1:15" x14ac:dyDescent="0.2">
       <c r="B20" s="2" t="s">
         <v>46</v>
       </c>
@@ -2069,8 +2785,31 @@
       <c r="G20" s="1">
         <v>0.18511599302452547</v>
       </c>
-    </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="J20" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="K20" s="1">
+        <f>MAX(D13:D22)</f>
+        <v>22</v>
+      </c>
+      <c r="L20" s="1">
+        <f>MIN(D13:D22)</f>
+        <v>12</v>
+      </c>
+      <c r="M20" s="1">
+        <f>AVERAGE(D13:D22)</f>
+        <v>17.100000000000001</v>
+      </c>
+      <c r="N20" s="1">
+        <f>_xlfn.STDEV.S(D13:D22)</f>
+        <v>3.7252889522529373</v>
+      </c>
+      <c r="O20" s="1">
+        <f>N20/SQRT(COUNT(D13:D22))</f>
+        <v>1.1780398031381532</v>
+      </c>
+    </row>
+    <row r="21" spans="1:15" x14ac:dyDescent="0.2">
       <c r="B21" s="2" t="s">
         <v>47</v>
       </c>
@@ -2089,8 +2828,31 @@
       <c r="G21" s="1">
         <v>0.11152887240995774</v>
       </c>
-    </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="J21" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="K21" s="1">
+        <f>MAX(E13:E22)</f>
+        <v>85.73737956024047</v>
+      </c>
+      <c r="L21" s="1">
+        <f>MIN(E13:E22)</f>
+        <v>57.847622237106499</v>
+      </c>
+      <c r="M21" s="1">
+        <f>AVERAGE(E13:E22)</f>
+        <v>70.917594199013848</v>
+      </c>
+      <c r="N21" s="1">
+        <f>_xlfn.STDEV.S(E13:E22)</f>
+        <v>7.6141403910089815</v>
+      </c>
+      <c r="O21" s="1">
+        <f>N21/SQRT(COUNT(E13:E22))</f>
+        <v>2.4078026059873427</v>
+      </c>
+    </row>
+    <row r="22" spans="1:15" x14ac:dyDescent="0.2">
       <c r="B22" s="2" t="s">
         <v>48</v>
       </c>
@@ -2109,13 +2871,59 @@
       <c r="G22" s="1">
         <v>0.10300128796940282</v>
       </c>
-    </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="J22" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="K22" s="1">
+        <f>MAX(F13:F22)</f>
+        <v>33.466589313267654</v>
+      </c>
+      <c r="L22" s="1">
+        <f>MIN(F13:F22)</f>
+        <v>18.279850971278954</v>
+      </c>
+      <c r="M22" s="1">
+        <f>AVERAGE(F13:F22)</f>
+        <v>25.03280208704188</v>
+      </c>
+      <c r="N22" s="1">
+        <f>_xlfn.STDEV.S(F13:F22)</f>
+        <v>4.7540051765761664</v>
+      </c>
+      <c r="O22" s="1">
+        <f>N22/SQRT(COUNT(F13:F22))</f>
+        <v>1.5033484366211642</v>
+      </c>
+    </row>
+    <row r="23" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A23" s="2" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="J23" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="K23" s="1">
+        <f>MAX(G13:G22)</f>
+        <v>0.91688198450172087</v>
+      </c>
+      <c r="L23" s="1">
+        <f>MIN(G13:G22)</f>
+        <v>0.10300128796940282</v>
+      </c>
+      <c r="M23" s="1">
+        <f>AVERAGE(G13:G22)</f>
+        <v>0.33831599101779575</v>
+      </c>
+      <c r="N23" s="1">
+        <f>_xlfn.STDEV.S(G13:G22)</f>
+        <v>0.2777977156919566</v>
+      </c>
+      <c r="O23" s="1">
+        <f>N23/SQRT(COUNT(G13:G22))</f>
+        <v>8.7847351037848118E-2</v>
+      </c>
+    </row>
+    <row r="24" spans="1:15" x14ac:dyDescent="0.2">
       <c r="B24" s="2" t="s">
         <v>17</v>
       </c>
@@ -2135,7 +2943,7 @@
         <v>0.36499286200442066</v>
       </c>
     </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:15" x14ac:dyDescent="0.2">
       <c r="B25" s="2" t="s">
         <v>18</v>
       </c>
@@ -2155,7 +2963,7 @@
         <v>1.1461479043386604</v>
       </c>
     </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:15" x14ac:dyDescent="0.2">
       <c r="B26" s="2" t="s">
         <v>19</v>
       </c>
@@ -2174,8 +2982,26 @@
       <c r="G26" s="1">
         <v>0.70402924365393393</v>
       </c>
-    </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="J26" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="K26" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="L26" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="M26" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="N26" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="O26" s="2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="27" spans="1:15" x14ac:dyDescent="0.2">
       <c r="B27" s="2" t="s">
         <v>20</v>
       </c>
@@ -2194,8 +3020,31 @@
       <c r="G27" s="1">
         <v>2.7159576032794113</v>
       </c>
-    </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="J27" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="K27" s="1">
+        <f>MAX(C24:C33)</f>
+        <v>976</v>
+      </c>
+      <c r="L27" s="1">
+        <f>MIN(C24:C33)</f>
+        <v>124</v>
+      </c>
+      <c r="M27" s="1">
+        <f>AVERAGE(C24:C33)</f>
+        <v>403</v>
+      </c>
+      <c r="N27" s="1">
+        <f>_xlfn.STDEV.S(C24:C33)</f>
+        <v>296.60935776052497</v>
+      </c>
+      <c r="O27" s="1">
+        <f>N27/SQRT(COUNT(C24:C33))</f>
+        <v>93.796114584299858</v>
+      </c>
+    </row>
+    <row r="28" spans="1:15" x14ac:dyDescent="0.2">
       <c r="B28" s="2" t="s">
         <v>21</v>
       </c>
@@ -2214,8 +3063,31 @@
       <c r="G28" s="1">
         <v>8.590117778982437</v>
       </c>
-    </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="J28" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="K28" s="1">
+        <f>MAX(D24:D33)</f>
+        <v>30</v>
+      </c>
+      <c r="L28" s="1">
+        <f>MIN(D24:D33)</f>
+        <v>13</v>
+      </c>
+      <c r="M28" s="1">
+        <f>AVERAGE(D24:D33)</f>
+        <v>19.8</v>
+      </c>
+      <c r="N28" s="1">
+        <f>_xlfn.STDEV.S(D24:D33)</f>
+        <v>5.2238768064425942</v>
+      </c>
+      <c r="O28" s="1">
+        <f>N28/SQRT(COUNT(D24:D33))</f>
+        <v>1.6519348924485151</v>
+      </c>
+    </row>
+    <row r="29" spans="1:15" x14ac:dyDescent="0.2">
       <c r="B29" s="2" t="s">
         <v>22</v>
       </c>
@@ -2234,8 +3106,31 @@
       <c r="G29" s="1">
         <v>2.0934378027482152</v>
       </c>
-    </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="J29" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="K29" s="1">
+        <f>MAX(E24:E33)</f>
+        <v>85.617529205937132</v>
+      </c>
+      <c r="L29" s="1">
+        <f>MIN(E24:E33)</f>
+        <v>63.415847009140961</v>
+      </c>
+      <c r="M29" s="1">
+        <f>AVERAGE(E24:E33)</f>
+        <v>73.648605741066518</v>
+      </c>
+      <c r="N29" s="1">
+        <f>_xlfn.STDEV.S(E24:E33)</f>
+        <v>8.864725114621228</v>
+      </c>
+      <c r="O29" s="1">
+        <f>N29/SQRT(COUNT(E24:E33))</f>
+        <v>2.8032722193500286</v>
+      </c>
+    </row>
+    <row r="30" spans="1:15" x14ac:dyDescent="0.2">
       <c r="B30" s="2" t="s">
         <v>23</v>
       </c>
@@ -2254,8 +3149,31 @@
       <c r="G30" s="1">
         <v>1.0802903265114734</v>
       </c>
-    </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="J30" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="K30" s="1">
+        <f>MAX(F24:F33)</f>
+        <v>54.146840599701285</v>
+      </c>
+      <c r="L30" s="1">
+        <f>MIN(F24:F33)</f>
+        <v>20.412271200564732</v>
+      </c>
+      <c r="M30" s="1">
+        <f>AVERAGE(F24:F33)</f>
+        <v>37.599153371668663</v>
+      </c>
+      <c r="N30" s="1">
+        <f>_xlfn.STDEV.S(F24:F33)</f>
+        <v>12.028552012673806</v>
+      </c>
+      <c r="O30" s="1">
+        <f>N30/SQRT(COUNT(F24:F33))</f>
+        <v>3.8037621313851773</v>
+      </c>
+    </row>
+    <row r="31" spans="1:15" x14ac:dyDescent="0.2">
       <c r="B31" s="2" t="s">
         <v>24</v>
       </c>
@@ -2274,8 +3192,31 @@
       <c r="G31" s="1">
         <v>0.67188298732198659</v>
       </c>
-    </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="J31" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="K31" s="1">
+        <f>MAX(G24:G33)</f>
+        <v>8.590117778982437</v>
+      </c>
+      <c r="L31" s="1">
+        <f>MIN(G24:G33)</f>
+        <v>0.17038188855781242</v>
+      </c>
+      <c r="M31" s="1">
+        <f>AVERAGE(G24:G33)</f>
+        <v>1.7880799491488812</v>
+      </c>
+      <c r="N31" s="1">
+        <f>_xlfn.STDEV.S(G24:G33)</f>
+        <v>2.5228903636608764</v>
+      </c>
+      <c r="O31" s="1">
+        <f>N31/SQRT(COUNT(G24:G33))</f>
+        <v>0.79780798360588678</v>
+      </c>
+    </row>
+    <row r="32" spans="1:15" x14ac:dyDescent="0.2">
       <c r="B32" s="2" t="s">
         <v>25</v>
       </c>
@@ -2295,7 +3236,7 @@
         <v>0.17038188855781242</v>
       </c>
     </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:15" x14ac:dyDescent="0.2">
       <c r="B33" s="2" t="s">
         <v>26</v>
       </c>
@@ -2315,12 +3256,30 @@
         <v>0.3435610940904627</v>
       </c>
     </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A34" s="2" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="J34" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="K34" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="L34" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="M34" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="N34" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="O34" s="2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="35" spans="1:15" x14ac:dyDescent="0.2">
       <c r="B35" s="2" t="s">
         <v>1</v>
       </c>
@@ -2339,8 +3298,31 @@
       <c r="G35" s="1">
         <v>0.14498702317313508</v>
       </c>
-    </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="J35" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="K35" s="1">
+        <f>MAX(C35:C44)</f>
+        <v>397</v>
+      </c>
+      <c r="L35" s="1">
+        <f>MIN(C35:C44)</f>
+        <v>40</v>
+      </c>
+      <c r="M35" s="1">
+        <f>AVERAGE(C35:C44)</f>
+        <v>143.19999999999999</v>
+      </c>
+      <c r="N35" s="1">
+        <f>_xlfn.STDEV.S(C35:C44)</f>
+        <v>100.12303542253512</v>
+      </c>
+      <c r="O35" s="1">
+        <f>N35/SQRT(COUNT(C35:C44))</f>
+        <v>31.66168381849301</v>
+      </c>
+    </row>
+    <row r="36" spans="1:15" x14ac:dyDescent="0.2">
       <c r="B36" s="2" t="s">
         <v>2</v>
       </c>
@@ -2359,8 +3341,31 @@
       <c r="G36" s="1">
         <v>10.999999999999998</v>
       </c>
-    </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="J36" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="K36" s="1">
+        <f>MAX(D35:D44)</f>
+        <v>21</v>
+      </c>
+      <c r="L36" s="1">
+        <f>MIN(D35:D44)</f>
+        <v>4</v>
+      </c>
+      <c r="M36" s="1">
+        <f>AVERAGE(D35:D44)</f>
+        <v>11.9</v>
+      </c>
+      <c r="N36" s="1">
+        <f>_xlfn.STDEV.S(D35:D44)</f>
+        <v>6.2084172253839744</v>
+      </c>
+      <c r="O36" s="1">
+        <f>N36/SQRT(COUNT(D35:D44))</f>
+        <v>1.9632739096836296</v>
+      </c>
+    </row>
+    <row r="37" spans="1:15" x14ac:dyDescent="0.2">
       <c r="B37" s="2" t="s">
         <v>3</v>
       </c>
@@ -2379,8 +3384,31 @@
       <c r="G37" s="1">
         <v>0.14181329701124509</v>
       </c>
-    </row>
-    <row r="38" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="J37" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="K37" s="1">
+        <f>MAX(E35:E44)</f>
+        <v>77.297221580406656</v>
+      </c>
+      <c r="L37" s="1">
+        <f>MIN(E35:E44)</f>
+        <v>29</v>
+      </c>
+      <c r="M37" s="1">
+        <f>AVERAGE(E35:E44)</f>
+        <v>48.954849888784054</v>
+      </c>
+      <c r="N37" s="1">
+        <f>_xlfn.STDEV.S(E35:E44)</f>
+        <v>15.431068492542886</v>
+      </c>
+      <c r="O37" s="1">
+        <f>N37/SQRT(COUNT(E35:E44))</f>
+        <v>4.879732316649652</v>
+      </c>
+    </row>
+    <row r="38" spans="1:15" x14ac:dyDescent="0.2">
       <c r="B38" s="2" t="s">
         <v>4</v>
       </c>
@@ -2399,8 +3427,31 @@
       <c r="G38" s="1">
         <v>0.84425838121845398</v>
       </c>
-    </row>
-    <row r="39" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="J38" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="K38" s="1">
+        <f>MAX(F35:F44)</f>
+        <v>35.797712084380343</v>
+      </c>
+      <c r="L38" s="1">
+        <f>MIN(F35:F44)</f>
+        <v>15.556349186104045</v>
+      </c>
+      <c r="M38" s="1">
+        <f>AVERAGE(F35:F44)</f>
+        <v>21.572387771138875</v>
+      </c>
+      <c r="N38" s="1">
+        <f>_xlfn.STDEV.S(F35:F44)</f>
+        <v>6.5033834623442814</v>
+      </c>
+      <c r="O38" s="1">
+        <f>N38/SQRT(COUNT(F35:F44))</f>
+        <v>2.0565504238479808</v>
+      </c>
+    </row>
+    <row r="39" spans="1:15" x14ac:dyDescent="0.2">
       <c r="B39" s="2" t="s">
         <v>5</v>
       </c>
@@ -2419,8 +3470,31 @@
       <c r="G39" s="1">
         <v>0.34852739226777879</v>
       </c>
-    </row>
-    <row r="40" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="J39" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="K39" s="1">
+        <f>MAX(G35:G44)</f>
+        <v>13.530263382908862</v>
+      </c>
+      <c r="L39" s="1">
+        <f>MIN(G35:G44)</f>
+        <v>0.14181329701124509</v>
+      </c>
+      <c r="M39" s="1">
+        <f>AVERAGE(G35:G44)</f>
+        <v>2.9152181360642397</v>
+      </c>
+      <c r="N39" s="1">
+        <f>_xlfn.STDEV.S(G35:G44)</f>
+        <v>4.9770982501984866</v>
+      </c>
+      <c r="O39" s="1">
+        <f>N39/SQRT(COUNT(G35:G44))</f>
+        <v>1.5738966609065805</v>
+      </c>
+    </row>
+    <row r="40" spans="1:15" x14ac:dyDescent="0.2">
       <c r="B40" s="2" t="s">
         <v>6</v>
       </c>
@@ -2440,7 +3514,7 @@
         <v>13.530263382908862</v>
       </c>
     </row>
-    <row r="41" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:15" x14ac:dyDescent="0.2">
       <c r="B41" s="2" t="s">
         <v>7</v>
       </c>
@@ -2460,7 +3534,7 @@
         <v>0.76881247343443526</v>
       </c>
     </row>
-    <row r="42" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:15" x14ac:dyDescent="0.2">
       <c r="B42" s="2" t="s">
         <v>8</v>
       </c>
@@ -2480,7 +3554,7 @@
         <v>1.3776215616584211</v>
       </c>
     </row>
-    <row r="43" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:15" x14ac:dyDescent="0.2">
       <c r="B43" s="2" t="s">
         <v>9</v>
       </c>
@@ -2500,7 +3574,7 @@
         <v>0.51035198643079338</v>
       </c>
     </row>
-    <row r="44" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:15" x14ac:dyDescent="0.2">
       <c r="B44" s="2" t="s">
         <v>10</v>
       </c>
@@ -2521,9 +3595,6 @@
       </c>
     </row>
   </sheetData>
-  <mergeCells count="1">
-    <mergeCell ref="K10:O10"/>
-  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -2532,16 +3603,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CE658B17-E7D7-44A7-84B1-1333A97336CC}">
   <dimension ref="A1:O44"/>
   <sheetViews>
-    <sheetView topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="C44" sqref="C44:G44"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="J10" sqref="J10:O39"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" width="20.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="20.83203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
         <v>27</v>
       </c>
@@ -2561,7 +3632,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:15" x14ac:dyDescent="0.2">
       <c r="B2" s="2" t="s">
         <v>28</v>
       </c>
@@ -2596,7 +3667,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:15" x14ac:dyDescent="0.2">
       <c r="B3" s="2" t="s">
         <v>29</v>
       </c>
@@ -2639,7 +3710,7 @@
         <v>5.2903154442811813</v>
       </c>
     </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:15" x14ac:dyDescent="0.2">
       <c r="B4" s="2" t="s">
         <v>30</v>
       </c>
@@ -2682,7 +3753,7 @@
         <v>0.17606816861659008</v>
       </c>
     </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:15" x14ac:dyDescent="0.2">
       <c r="B5" s="2" t="s">
         <v>31</v>
       </c>
@@ -2725,7 +3796,7 @@
         <v>0.37398696649215574</v>
       </c>
     </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:15" x14ac:dyDescent="0.2">
       <c r="B6" s="2" t="s">
         <v>32</v>
       </c>
@@ -2768,7 +3839,7 @@
         <v>0.42346869981983437</v>
       </c>
     </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:15" x14ac:dyDescent="0.2">
       <c r="B7" s="2" t="s">
         <v>33</v>
       </c>
@@ -2811,7 +3882,7 @@
         <v>3.3635793291564228E-2</v>
       </c>
     </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:15" x14ac:dyDescent="0.2">
       <c r="B8" s="2" t="s">
         <v>34</v>
       </c>
@@ -2831,7 +3902,7 @@
         <v>7.7766579792532611E-2</v>
       </c>
     </row>
-    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:15" x14ac:dyDescent="0.2">
       <c r="B9" s="2" t="s">
         <v>35</v>
       </c>
@@ -2851,7 +3922,7 @@
         <v>7.8412389911684505E-2</v>
       </c>
     </row>
-    <row r="10" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:15" x14ac:dyDescent="0.2">
       <c r="B10" s="2" t="s">
         <v>36</v>
       </c>
@@ -2870,8 +3941,26 @@
       <c r="G10" s="1">
         <v>4.7875046416102143E-2</v>
       </c>
-    </row>
-    <row r="11" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="J10" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="K10" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="L10" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="M10" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="N10" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="O10" s="2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="11" spans="1:15" x14ac:dyDescent="0.2">
       <c r="B11" s="2" t="s">
         <v>37</v>
       </c>
@@ -2890,13 +3979,59 @@
       <c r="G11" s="1">
         <v>6.7840221115144261E-2</v>
       </c>
-    </row>
-    <row r="12" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="J11" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="K11" s="1">
+        <f>MAX(C2:C11)</f>
+        <v>139</v>
+      </c>
+      <c r="L11" s="1">
+        <f>MIN(C2:C11)</f>
+        <v>48</v>
+      </c>
+      <c r="M11" s="1">
+        <f>AVERAGE(C2:C11)</f>
+        <v>74.599999999999994</v>
+      </c>
+      <c r="N11" s="1">
+        <f>_xlfn.STDEV.S(C2:C11)</f>
+        <v>25.474169924324002</v>
+      </c>
+      <c r="O11" s="1">
+        <f>N11/SQRT(COUNT(C2:C11))</f>
+        <v>8.0556398463023005</v>
+      </c>
+    </row>
+    <row r="12" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A12" s="2" t="s">
         <v>38</v>
       </c>
-    </row>
-    <row r="13" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="J12" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="K12" s="1">
+        <f>MAX(D2:D11)</f>
+        <v>0</v>
+      </c>
+      <c r="L12" s="1">
+        <f>MIN(D2:D11)</f>
+        <v>0</v>
+      </c>
+      <c r="M12" s="1">
+        <f>AVERAGE(D2:D11)</f>
+        <v>0</v>
+      </c>
+      <c r="N12" s="1">
+        <f>STDEV(D2:D11)</f>
+        <v>0</v>
+      </c>
+      <c r="O12" s="1">
+        <f>N12/SQRT(COUNT(D2:D11))</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:15" x14ac:dyDescent="0.2">
       <c r="B13" s="2" t="s">
         <v>39</v>
       </c>
@@ -2915,8 +4050,31 @@
       <c r="G13" s="1">
         <v>2.0028912023817992E-2</v>
       </c>
-    </row>
-    <row r="14" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="J13" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="K13" s="1">
+        <f>MAX(E2:E11)</f>
+        <v>7.4798459872458185</v>
+      </c>
+      <c r="L13" s="1">
+        <f>MIN(E2:E11)</f>
+        <v>3.1161019431696122</v>
+      </c>
+      <c r="M13" s="1">
+        <f>AVERAGE(E2:E11)</f>
+        <v>4.8268532908387582</v>
+      </c>
+      <c r="N13" s="1">
+        <f>_xlfn.STDEV.S(E2:E11)</f>
+        <v>1.3541747372243789</v>
+      </c>
+      <c r="O13" s="1">
+        <f>N13/SQRT(COUNT(E2:E11))</f>
+        <v>0.42822765194890383</v>
+      </c>
+    </row>
+    <row r="14" spans="1:15" x14ac:dyDescent="0.2">
       <c r="B14" s="2" t="s">
         <v>40</v>
       </c>
@@ -2935,8 +4093,31 @@
       <c r="G14" s="1">
         <v>1.0934615004792828E-2</v>
       </c>
-    </row>
-    <row r="15" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="J14" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="K14" s="1">
+        <f>MAX(F2:F11)</f>
+        <v>12.381462861786957</v>
+      </c>
+      <c r="L14" s="1">
+        <f>MIN(F2:F11)</f>
+        <v>4.523472807681185</v>
+      </c>
+      <c r="M14" s="1">
+        <f>AVERAGE(F2:F11)</f>
+        <v>7.6993879075355505</v>
+      </c>
+      <c r="N14" s="1">
+        <f>_xlfn.STDEV.S(F2:F11)</f>
+        <v>2.757174547220981</v>
+      </c>
+      <c r="O14" s="1">
+        <f>N14/SQRT(COUNT(C2:C11))</f>
+        <v>0.87189514758617737</v>
+      </c>
+    </row>
+    <row r="15" spans="1:15" x14ac:dyDescent="0.2">
       <c r="B15" s="2" t="s">
         <v>41</v>
       </c>
@@ -2955,8 +4136,31 @@
       <c r="G15" s="1">
         <v>0.19971997534917335</v>
       </c>
-    </row>
-    <row r="16" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="J15" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="K15" s="1">
+        <f>MAX(G2:G11)</f>
+        <v>0.25069069706145924</v>
+      </c>
+      <c r="L15" s="1">
+        <f>MIN(G2:G11)</f>
+        <v>4.5337153770353682E-2</v>
+      </c>
+      <c r="M15" s="1">
+        <f>AVERAGE(G2:G11)</f>
+        <v>9.6268317732361997E-2</v>
+      </c>
+      <c r="N15" s="1">
+        <f>_xlfn.STDEV.S(G2:G11)</f>
+        <v>6.5544197370388357E-2</v>
+      </c>
+      <c r="O15" s="1">
+        <f>N15/SQRT(COUNT(F2:F11))</f>
+        <v>2.0726895109804612E-2</v>
+      </c>
+    </row>
+    <row r="16" spans="1:15" x14ac:dyDescent="0.2">
       <c r="B16" s="2" t="s">
         <v>42</v>
       </c>
@@ -2975,8 +4179,9 @@
       <c r="G16" s="1">
         <v>3.7091447917918415E-2</v>
       </c>
-    </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="J16" s="2"/>
+    </row>
+    <row r="17" spans="1:15" x14ac:dyDescent="0.2">
       <c r="B17" s="2" t="s">
         <v>43</v>
       </c>
@@ -2996,7 +4201,7 @@
         <v>0.10580310918921712</v>
       </c>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:15" x14ac:dyDescent="0.2">
       <c r="B18" s="2" t="s">
         <v>44</v>
       </c>
@@ -3015,8 +4220,26 @@
       <c r="G18" s="1">
         <v>3.2832512870118735E-2</v>
       </c>
-    </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="J18" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="K18" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="L18" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="M18" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="N18" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="O18" s="2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="19" spans="1:15" x14ac:dyDescent="0.2">
       <c r="B19" s="2" t="s">
         <v>45</v>
       </c>
@@ -3035,8 +4258,31 @@
       <c r="G19" s="1">
         <v>6.6125670538166717E-2</v>
       </c>
-    </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="J19" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="K19" s="1">
+        <f>MAX(C13:C22)</f>
+        <v>103</v>
+      </c>
+      <c r="L19" s="1">
+        <f>MIN(C13:C22)</f>
+        <v>1</v>
+      </c>
+      <c r="M19" s="1">
+        <f>AVERAGE(C13:C22)</f>
+        <v>39.5</v>
+      </c>
+      <c r="N19" s="1">
+        <f>_xlfn.STDEV.S(C13:C22)</f>
+        <v>29.189990674125873</v>
+      </c>
+      <c r="O19" s="1">
+        <f>N19/SQRT(COUNT(C13:C22))</f>
+        <v>9.230685540931157</v>
+      </c>
+    </row>
+    <row r="20" spans="1:15" x14ac:dyDescent="0.2">
       <c r="B20" s="2" t="s">
         <v>46</v>
       </c>
@@ -3055,8 +4301,31 @@
       <c r="G20" s="1">
         <v>2.9843129996007731E-2</v>
       </c>
-    </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="J20" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="K20" s="1">
+        <f>MAX(D13:D22)</f>
+        <v>2</v>
+      </c>
+      <c r="L20" s="1">
+        <f>MIN(D13:D22)</f>
+        <v>0</v>
+      </c>
+      <c r="M20" s="1">
+        <f>AVERAGE(D13:D22)</f>
+        <v>0.4</v>
+      </c>
+      <c r="N20" s="1">
+        <f>_xlfn.STDEV.S(D13:D22)</f>
+        <v>0.84327404271156781</v>
+      </c>
+      <c r="O20" s="1">
+        <f>N20/SQRT(COUNT(D13:D22))</f>
+        <v>0.26666666666666666</v>
+      </c>
+    </row>
+    <row r="21" spans="1:15" x14ac:dyDescent="0.2">
       <c r="B21" s="2" t="s">
         <v>47</v>
       </c>
@@ -3075,8 +4344,31 @@
       <c r="G21" s="1">
         <v>2.2008392873584603E-4</v>
       </c>
-    </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="J21" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="K21" s="1">
+        <f>MAX(E13:E22)</f>
+        <v>9.3811509591326097</v>
+      </c>
+      <c r="L21" s="1">
+        <f>MIN(E13:E22)</f>
+        <v>1.3028588445503275E-3</v>
+      </c>
+      <c r="M21" s="1">
+        <f>AVERAGE(E13:E22)</f>
+        <v>4.9702812828318139</v>
+      </c>
+      <c r="N21" s="1">
+        <f>_xlfn.STDEV.S(E13:E22)</f>
+        <v>3.2826355200757469</v>
+      </c>
+      <c r="O21" s="1">
+        <f>N21/SQRT(COUNT(E13:E22))</f>
+        <v>1.0380604971610743</v>
+      </c>
+    </row>
+    <row r="22" spans="1:15" x14ac:dyDescent="0.2">
       <c r="B22" s="2" t="s">
         <v>48</v>
       </c>
@@ -3095,13 +4387,59 @@
       <c r="G22" s="1">
         <v>2.3671013886870807E-3</v>
       </c>
-    </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="J22" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="K22" s="1">
+        <f>MAX(F13:F22)</f>
+        <v>6.2425977276161326</v>
+      </c>
+      <c r="L22" s="1">
+        <f>MIN(F13:F22)</f>
+        <v>3.6072286319516707E-2</v>
+      </c>
+      <c r="M22" s="1">
+        <f>AVERAGE(F13:F22)</f>
+        <v>3.130609503636232</v>
+      </c>
+      <c r="N22" s="1">
+        <f>_xlfn.STDEV.S(F13:F22)</f>
+        <v>2.0715745591684938</v>
+      </c>
+      <c r="O22" s="1">
+        <f>N22/SQRT(COUNT(F13:F22))</f>
+        <v>0.65508939498316854</v>
+      </c>
+    </row>
+    <row r="23" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A23" s="2" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="J23" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="K23" s="1">
+        <f>MAX(G13:G22)</f>
+        <v>0.19971997534917335</v>
+      </c>
+      <c r="L23" s="1">
+        <f>MIN(G13:G22)</f>
+        <v>2.2008392873584603E-4</v>
+      </c>
+      <c r="M23" s="1">
+        <f>AVERAGE(G13:G22)</f>
+        <v>5.049665582066358E-2</v>
+      </c>
+      <c r="N23" s="1">
+        <f>_xlfn.STDEV.S(G13:G22)</f>
+        <v>6.130668336509313E-2</v>
+      </c>
+      <c r="O23" s="1">
+        <f>N23/SQRT(COUNT(G13:G22))</f>
+        <v>1.938687552244504E-2</v>
+      </c>
+    </row>
+    <row r="24" spans="1:15" x14ac:dyDescent="0.2">
       <c r="B24" s="2" t="s">
         <v>17</v>
       </c>
@@ -3121,7 +4459,7 @@
         <v>3.138308912467782E-2</v>
       </c>
     </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:15" x14ac:dyDescent="0.2">
       <c r="B25" s="2" t="s">
         <v>18</v>
       </c>
@@ -3141,7 +4479,7 @@
         <v>8.7059588189191128E-2</v>
       </c>
     </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:15" x14ac:dyDescent="0.2">
       <c r="B26" s="2" t="s">
         <v>19</v>
       </c>
@@ -3160,8 +4498,26 @@
       <c r="G26" s="1">
         <v>0.11747052713876484</v>
       </c>
-    </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="J26" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="K26" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="L26" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="M26" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="N26" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="O26" s="2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="27" spans="1:15" x14ac:dyDescent="0.2">
       <c r="B27" s="2" t="s">
         <v>20</v>
       </c>
@@ -3180,8 +4536,31 @@
       <c r="G27" s="1">
         <v>0.20922714928995231</v>
       </c>
-    </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="J27" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="K27" s="1">
+        <f>MAX(C24:C33)</f>
+        <v>96</v>
+      </c>
+      <c r="L27" s="1">
+        <f>MIN(C24:C33)</f>
+        <v>8</v>
+      </c>
+      <c r="M27" s="1">
+        <f>AVERAGE(C24:C33)</f>
+        <v>32.5</v>
+      </c>
+      <c r="N27" s="1">
+        <f>_xlfn.STDEV.S(C24:C33)</f>
+        <v>26.916537667389541</v>
+      </c>
+      <c r="O27" s="1">
+        <f>N27/SQRT(COUNT(C24:C33))</f>
+        <v>8.5117565754666646</v>
+      </c>
+    </row>
+    <row r="28" spans="1:15" x14ac:dyDescent="0.2">
       <c r="B28" s="2" t="s">
         <v>21</v>
       </c>
@@ -3200,8 +4579,31 @@
       <c r="G28" s="1">
         <v>0.9296222517045285</v>
       </c>
-    </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="J28" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="K28" s="1">
+        <f>MAX(D24:D33)</f>
+        <v>0</v>
+      </c>
+      <c r="L28" s="1">
+        <f>MIN(D24:D33)</f>
+        <v>0</v>
+      </c>
+      <c r="M28" s="1">
+        <f>AVERAGE(D24:D33)</f>
+        <v>0</v>
+      </c>
+      <c r="N28" s="1">
+        <f>_xlfn.STDEV.S(D24:D33)</f>
+        <v>0</v>
+      </c>
+      <c r="O28" s="1">
+        <f>N28/SQRT(COUNT(D24:D33))</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29" spans="1:15" x14ac:dyDescent="0.2">
       <c r="B29" s="2" t="s">
         <v>22</v>
       </c>
@@ -3220,8 +4622,31 @@
       <c r="G29" s="1">
         <v>9.59270064021783E-2</v>
       </c>
-    </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="J29" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="K29" s="1">
+        <f>MAX(E24:E33)</f>
+        <v>6.9038320446977819</v>
+      </c>
+      <c r="L29" s="1">
+        <f>MIN(E24:E33)</f>
+        <v>2.088142470694319</v>
+      </c>
+      <c r="M29" s="1">
+        <f>AVERAGE(E24:E33)</f>
+        <v>4.5895053004627391</v>
+      </c>
+      <c r="N29" s="1">
+        <f>_xlfn.STDEV.S(E24:E33)</f>
+        <v>1.268349142577464</v>
+      </c>
+      <c r="O29" s="1">
+        <f>N29/SQRT(COUNT(E24:E33))</f>
+        <v>0.40108721588664326</v>
+      </c>
+    </row>
+    <row r="30" spans="1:15" x14ac:dyDescent="0.2">
       <c r="B30" s="2" t="s">
         <v>23</v>
       </c>
@@ -3240,8 +4665,31 @@
       <c r="G30" s="1">
         <v>0.11939827333982429</v>
       </c>
-    </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="J30" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="K30" s="1">
+        <f>MAX(F24:F33)</f>
+        <v>5.8120222230367409</v>
+      </c>
+      <c r="L30" s="1">
+        <f>MIN(F24:F33)</f>
+        <v>2.4811553121122221</v>
+      </c>
+      <c r="M30" s="1">
+        <f>AVERAGE(F24:F33)</f>
+        <v>3.6876040639908942</v>
+      </c>
+      <c r="N30" s="1">
+        <f>_xlfn.STDEV.S(F24:F33)</f>
+        <v>0.9692762278775362</v>
+      </c>
+      <c r="O30" s="1">
+        <f>N30/SQRT(COUNT(F24:F33))</f>
+        <v>0.30651205619494076</v>
+      </c>
+    </row>
+    <row r="31" spans="1:15" x14ac:dyDescent="0.2">
       <c r="B31" s="2" t="s">
         <v>24</v>
       </c>
@@ -3260,8 +4708,31 @@
       <c r="G31" s="1">
         <v>8.7263272869782443E-2</v>
       </c>
-    </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="J31" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="K31" s="1">
+        <f>MAX(G24:G33)</f>
+        <v>0.9296222517045285</v>
+      </c>
+      <c r="L31" s="1">
+        <f>MIN(G24:G33)</f>
+        <v>1.6719428754575459E-2</v>
+      </c>
+      <c r="M31" s="1">
+        <f>AVERAGE(G24:G33)</f>
+        <v>0.17558884169310915</v>
+      </c>
+      <c r="N31" s="1">
+        <f>_xlfn.STDEV.S(G24:G33)</f>
+        <v>0.27022552576237113</v>
+      </c>
+      <c r="O31" s="1">
+        <f>N31/SQRT(COUNT(G24:G33))</f>
+        <v>8.5452814332560106E-2</v>
+      </c>
+    </row>
+    <row r="32" spans="1:15" x14ac:dyDescent="0.2">
       <c r="B32" s="2" t="s">
         <v>25</v>
       </c>
@@ -3281,7 +4752,7 @@
         <v>1.6719428754575459E-2</v>
       </c>
     </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:15" x14ac:dyDescent="0.2">
       <c r="B33" s="2" t="s">
         <v>26</v>
       </c>
@@ -3301,12 +4772,30 @@
         <v>6.1817830117616393E-2</v>
       </c>
     </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A34" s="2" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="J34" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="K34" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="L34" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="M34" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="N34" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="O34" s="2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="35" spans="1:15" x14ac:dyDescent="0.2">
       <c r="B35" s="2" t="s">
         <v>1</v>
       </c>
@@ -3325,8 +4814,31 @@
       <c r="G35" s="1">
         <v>3.9426174827689273E-2</v>
       </c>
-    </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="J35" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="K35" s="1">
+        <f>MAX(C35:C44)</f>
+        <v>146</v>
+      </c>
+      <c r="L35" s="1">
+        <f>MIN(C35:C44)</f>
+        <v>4</v>
+      </c>
+      <c r="M35" s="1">
+        <f>AVERAGE(C35:C44)</f>
+        <v>49.2</v>
+      </c>
+      <c r="N35" s="1">
+        <f>_xlfn.STDEV.S(C35:C44)</f>
+        <v>40.237627497985848</v>
+      </c>
+      <c r="O35" s="1">
+        <f>N35/SQRT(COUNT(C35:C44))</f>
+        <v>12.724255053505752</v>
+      </c>
+    </row>
+    <row r="36" spans="1:15" x14ac:dyDescent="0.2">
       <c r="B36" s="2" t="s">
         <v>2</v>
       </c>
@@ -3345,8 +4857,31 @@
       <c r="G36" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="J36" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="K36" s="1">
+        <f>MAX(D35:D44)</f>
+        <v>4</v>
+      </c>
+      <c r="L36" s="1">
+        <f>MIN(D35:D44)</f>
+        <v>0</v>
+      </c>
+      <c r="M36" s="1">
+        <f>AVERAGE(D35:D44)</f>
+        <v>1.2</v>
+      </c>
+      <c r="N36" s="1">
+        <f>_xlfn.STDEV.S(D35:D44)</f>
+        <v>1.9321835661585918</v>
+      </c>
+      <c r="O36" s="1">
+        <f>N36/SQRT(COUNT(D35:D44))</f>
+        <v>0.61101009266077866</v>
+      </c>
+    </row>
+    <row r="37" spans="1:15" x14ac:dyDescent="0.2">
       <c r="B37" s="2" t="s">
         <v>3</v>
       </c>
@@ -3365,8 +4900,31 @@
       <c r="G37" s="1">
         <v>2.5334160065259854E-2</v>
       </c>
-    </row>
-    <row r="38" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="J37" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="K37" s="1">
+        <f>MAX(E35:E44)</f>
+        <v>10.22851201478743</v>
+      </c>
+      <c r="L37" s="1">
+        <f>MIN(E35:E44)</f>
+        <v>4</v>
+      </c>
+      <c r="M37" s="1">
+        <f>AVERAGE(E35:E44)</f>
+        <v>7.7716233936510148</v>
+      </c>
+      <c r="N37" s="1">
+        <f>_xlfn.STDEV.S(E35:E44)</f>
+        <v>1.7843408023174117</v>
+      </c>
+      <c r="O37" s="1">
+        <f>N37/SQRT(COUNT(E35:E44))</f>
+        <v>0.56425810572952728</v>
+      </c>
+    </row>
+    <row r="38" spans="1:15" x14ac:dyDescent="0.2">
       <c r="B38" s="2" t="s">
         <v>4</v>
       </c>
@@ -3385,8 +4943,31 @@
       <c r="G38" s="1">
         <v>0.23447253808012306</v>
       </c>
-    </row>
-    <row r="39" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="J38" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="K38" s="1">
+        <f>MAX(F35:F44)</f>
+        <v>7.3362354792960955</v>
+      </c>
+      <c r="L38" s="1">
+        <f>MIN(F35:F44)</f>
+        <v>0</v>
+      </c>
+      <c r="M38" s="1">
+        <f>AVERAGE(F35:F44)</f>
+        <v>4.0804431264713994</v>
+      </c>
+      <c r="N38" s="1">
+        <f>_xlfn.STDEV.S(F35:F44)</f>
+        <v>2.1818870812434867</v>
+      </c>
+      <c r="O38" s="1">
+        <f>N38/SQRT(COUNT(F35:F44))</f>
+        <v>0.68997327740262671</v>
+      </c>
+    </row>
+    <row r="39" spans="1:15" x14ac:dyDescent="0.2">
       <c r="B39" s="2" t="s">
         <v>5</v>
       </c>
@@ -3405,8 +4986,31 @@
       <c r="G39" s="1">
         <v>0.13946995244611635</v>
       </c>
-    </row>
-    <row r="40" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="J39" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="K39" s="1">
+        <f>MAX(G35:G44)</f>
+        <v>1.091089451179962</v>
+      </c>
+      <c r="L39" s="1">
+        <f>MIN(G35:G44)</f>
+        <v>0</v>
+      </c>
+      <c r="M39" s="1">
+        <f>AVERAGE(G35:G44)</f>
+        <v>0.21042043693222326</v>
+      </c>
+      <c r="N39" s="1">
+        <f>_xlfn.STDEV.S(G35:G44)</f>
+        <v>0.31987203195028829</v>
+      </c>
+      <c r="O39" s="1">
+        <f>N39/SQRT(COUNT(G35:G44))</f>
+        <v>0.10115241807490627</v>
+      </c>
+    </row>
+    <row r="40" spans="1:15" x14ac:dyDescent="0.2">
       <c r="B40" s="2" t="s">
         <v>6</v>
       </c>
@@ -3426,7 +5030,7 @@
         <v>1.091089451179962</v>
       </c>
     </row>
-    <row r="41" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:15" x14ac:dyDescent="0.2">
       <c r="B41" s="2" t="s">
         <v>7</v>
       </c>
@@ -3446,7 +5050,7 @@
         <v>0.1329603664890443</v>
       </c>
     </row>
-    <row r="42" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:15" x14ac:dyDescent="0.2">
       <c r="B42" s="2" t="s">
         <v>8</v>
       </c>
@@ -3466,7 +5070,7 @@
         <v>0.22963507778317577</v>
       </c>
     </row>
-    <row r="43" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:15" x14ac:dyDescent="0.2">
       <c r="B43" s="2" t="s">
         <v>9</v>
       </c>
@@ -3486,7 +5090,7 @@
         <v>0.14883330392645205</v>
       </c>
     </row>
-    <row r="44" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:15" x14ac:dyDescent="0.2">
       <c r="B44" s="2" t="s">
         <v>10</v>
       </c>
@@ -3515,16 +5119,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AE15F7AD-A0DC-4382-9A54-4AAD142EDBC9}">
   <dimension ref="A1:O44"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="P30" sqref="P30"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="P25" sqref="P25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" width="20.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="20.83203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
         <v>27</v>
       </c>
@@ -3544,7 +5148,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:15" x14ac:dyDescent="0.2">
       <c r="B2" s="2" t="s">
         <v>28</v>
       </c>
@@ -3563,6 +5167,9 @@
       <c r="G2" s="1">
         <v>4.7119321891999369E-4</v>
       </c>
+      <c r="J2" s="2" t="s">
+        <v>49</v>
+      </c>
       <c r="K2" s="2" t="s">
         <v>11</v>
       </c>
@@ -3579,7 +5186,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:15" x14ac:dyDescent="0.2">
       <c r="B3" s="2" t="s">
         <v>29</v>
       </c>
@@ -3622,7 +5229,7 @@
         <v>0.49598387070548977</v>
       </c>
     </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:15" x14ac:dyDescent="0.2">
       <c r="B4" s="2" t="s">
         <v>30</v>
       </c>
@@ -3665,7 +5272,7 @@
         <v>2.4685522072664372E-2</v>
       </c>
     </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:15" x14ac:dyDescent="0.2">
       <c r="B5" s="2" t="s">
         <v>31</v>
       </c>
@@ -3708,7 +5315,7 @@
         <v>8.3685620738454619E-2</v>
       </c>
     </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:15" x14ac:dyDescent="0.2">
       <c r="B6" s="2" t="s">
         <v>32</v>
       </c>
@@ -3751,7 +5358,7 @@
         <v>5.7752989611497579E-2</v>
       </c>
     </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:15" x14ac:dyDescent="0.2">
       <c r="B7" s="2" t="s">
         <v>33</v>
       </c>
@@ -3794,7 +5401,7 @@
         <v>1.0728157481495284E-3</v>
       </c>
     </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:15" x14ac:dyDescent="0.2">
       <c r="B8" s="2" t="s">
         <v>34</v>
       </c>
@@ -3814,7 +5421,7 @@
         <v>1.3839737246363107E-4</v>
       </c>
     </row>
-    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:15" x14ac:dyDescent="0.2">
       <c r="B9" s="2" t="s">
         <v>35</v>
       </c>
@@ -3834,7 +5441,7 @@
         <v>4.0107488068022305E-5</v>
       </c>
     </row>
-    <row r="10" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:15" x14ac:dyDescent="0.2">
       <c r="B10" s="2" t="s">
         <v>36</v>
       </c>
@@ -3853,8 +5460,26 @@
       <c r="G10" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="11" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="J10" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="K10" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="L10" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="M10" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="N10" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="O10" s="2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="11" spans="1:15" x14ac:dyDescent="0.2">
       <c r="B11" s="2" t="s">
         <v>37</v>
       </c>
@@ -3873,13 +5498,59 @@
       <c r="G11" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="12" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="J11" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="K11" s="1">
+        <f>MAX(C2:C11)</f>
+        <v>1</v>
+      </c>
+      <c r="L11" s="1">
+        <f>MIN(C2:C11)</f>
+        <v>0</v>
+      </c>
+      <c r="M11" s="1">
+        <f>AVERAGE(C2:C11)</f>
+        <v>0.4</v>
+      </c>
+      <c r="N11" s="1">
+        <f>_xlfn.STDEV.S(C2:C11)</f>
+        <v>0.5163977794943222</v>
+      </c>
+      <c r="O11" s="1">
+        <f>N11/SQRT(COUNT(C2:C11))</f>
+        <v>0.16329931618554519</v>
+      </c>
+    </row>
+    <row r="12" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A12" s="2" t="s">
         <v>38</v>
       </c>
-    </row>
-    <row r="13" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="J12" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="K12" s="1">
+        <f>MAX(D2:D11)</f>
+        <v>0</v>
+      </c>
+      <c r="L12" s="1">
+        <f>MIN(D2:D11)</f>
+        <v>0</v>
+      </c>
+      <c r="M12" s="1">
+        <f>AVERAGE(D2:D11)</f>
+        <v>0</v>
+      </c>
+      <c r="N12" s="1">
+        <f>STDEV(D2:D11)</f>
+        <v>0</v>
+      </c>
+      <c r="O12" s="1">
+        <f>N12/SQRT(COUNT(D2:D11))</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:15" x14ac:dyDescent="0.2">
       <c r="B13" s="2" t="s">
         <v>39</v>
       </c>
@@ -3898,8 +5569,31 @@
       <c r="G13" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="14" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="J13" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="K13" s="1">
+        <f>MAX(E2:E11)</f>
+        <v>1.2473271560940842E-3</v>
+      </c>
+      <c r="L13" s="1">
+        <f>MIN(E2:E11)</f>
+        <v>0</v>
+      </c>
+      <c r="M13" s="1">
+        <f>AVERAGE(E2:E11)</f>
+        <v>1.5808143785106752E-4</v>
+      </c>
+      <c r="N13" s="1">
+        <f>_xlfn.STDEV.S(E2:E11)</f>
+        <v>3.8806965740288744E-4</v>
+      </c>
+      <c r="O13" s="1">
+        <f>N13/SQRT(COUNT(E2:E11))</f>
+        <v>1.2271840081943473E-4</v>
+      </c>
+    </row>
+    <row r="14" spans="1:15" x14ac:dyDescent="0.2">
       <c r="B14" s="2" t="s">
         <v>40</v>
       </c>
@@ -3918,8 +5612,31 @@
       <c r="G14" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="15" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="J14" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="K14" s="1">
+        <f>MAX(F2:F11)</f>
+        <v>3.5298631051491371E-2</v>
+      </c>
+      <c r="L14" s="1">
+        <f>MIN(F2:F11)</f>
+        <v>0</v>
+      </c>
+      <c r="M14" s="1">
+        <f>AVERAGE(F2:F11)</f>
+        <v>6.5503090620656415E-3</v>
+      </c>
+      <c r="N14" s="1">
+        <f>_xlfn.STDEV.S(F2:F11)</f>
+        <v>1.130582903175581E-2</v>
+      </c>
+      <c r="O14" s="1">
+        <f>N14/SQRT(COUNT(C2:C11))</f>
+        <v>3.5752170576804493E-3</v>
+      </c>
+    </row>
+    <row r="15" spans="1:15" x14ac:dyDescent="0.2">
       <c r="B15" s="2" t="s">
         <v>41</v>
       </c>
@@ -3938,8 +5655,31 @@
       <c r="G15" s="1">
         <v>3.3722824066348238E-2</v>
       </c>
-    </row>
-    <row r="16" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="J15" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="K15" s="1">
+        <f>MAX(G2:G11)</f>
+        <v>4.7119321891999369E-4</v>
+      </c>
+      <c r="L15" s="1">
+        <f>MIN(G2:G11)</f>
+        <v>0</v>
+      </c>
+      <c r="M15" s="1">
+        <f>AVERAGE(G2:G11)</f>
+        <v>7.4734479363971457E-5</v>
+      </c>
+      <c r="N15" s="1">
+        <f>_xlfn.STDEV.S(G2:G11)</f>
+        <v>1.4774901751650636E-4</v>
+      </c>
+      <c r="O15" s="1">
+        <f>N15/SQRT(COUNT(F2:F11))</f>
+        <v>4.6722341740427458E-5</v>
+      </c>
+    </row>
+    <row r="16" spans="1:15" x14ac:dyDescent="0.2">
       <c r="B16" s="2" t="s">
         <v>42</v>
       </c>
@@ -3958,8 +5698,9 @@
       <c r="G16" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="J16" s="2"/>
+    </row>
+    <row r="17" spans="1:15" x14ac:dyDescent="0.2">
       <c r="B17" s="2" t="s">
         <v>43</v>
       </c>
@@ -3979,7 +5720,7 @@
         <v>2.0174572395544794E-3</v>
       </c>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:15" x14ac:dyDescent="0.2">
       <c r="B18" s="2" t="s">
         <v>44</v>
       </c>
@@ -3998,8 +5739,26 @@
       <c r="G18" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="J18" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="K18" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="L18" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="M18" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="N18" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="O18" s="2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="19" spans="1:15" x14ac:dyDescent="0.2">
       <c r="B19" s="2" t="s">
         <v>45</v>
       </c>
@@ -4018,8 +5777,31 @@
       <c r="G19" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="J19" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="K19" s="1">
+        <f>MAX(C13:C22)</f>
+        <v>11</v>
+      </c>
+      <c r="L19" s="1">
+        <f>MIN(C13:C22)</f>
+        <v>0</v>
+      </c>
+      <c r="M19" s="1">
+        <f>AVERAGE(C13:C22)</f>
+        <v>2.9</v>
+      </c>
+      <c r="N19" s="1">
+        <f>_xlfn.STDEV.S(C13:C22)</f>
+        <v>4.3576242252962674</v>
+      </c>
+      <c r="O19" s="1">
+        <f>N19/SQRT(COUNT(C13:C22))</f>
+        <v>1.3780017739062926</v>
+      </c>
+    </row>
+    <row r="20" spans="1:15" x14ac:dyDescent="0.2">
       <c r="B20" s="2" t="s">
         <v>46</v>
       </c>
@@ -4038,8 +5820,31 @@
       <c r="G20" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="J20" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="K20" s="1">
+        <f>MAX(D13:D22)</f>
+        <v>1</v>
+      </c>
+      <c r="L20" s="1">
+        <f>MIN(D13:D22)</f>
+        <v>0</v>
+      </c>
+      <c r="M20" s="1">
+        <f>AVERAGE(D13:D22)</f>
+        <v>0.1</v>
+      </c>
+      <c r="N20" s="1">
+        <f>_xlfn.STDEV.S(D13:D22)</f>
+        <v>0.31622776601683794</v>
+      </c>
+      <c r="O20" s="1">
+        <f>N20/SQRT(COUNT(D13:D22))</f>
+        <v>9.9999999999999992E-2</v>
+      </c>
+    </row>
+    <row r="21" spans="1:15" x14ac:dyDescent="0.2">
       <c r="B21" s="2" t="s">
         <v>47</v>
       </c>
@@ -4058,8 +5863,31 @@
       <c r="G21" s="1">
         <v>6.3144764281599149E-3</v>
       </c>
-    </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="J21" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="K21" s="1">
+        <f>MAX(E13:E22)</f>
+        <v>2.0328692674210838</v>
+      </c>
+      <c r="L21" s="1">
+        <f>MIN(E13:E22)</f>
+        <v>0</v>
+      </c>
+      <c r="M21" s="1">
+        <f>AVERAGE(E13:E22)</f>
+        <v>0.42609373527805461</v>
+      </c>
+      <c r="N21" s="1">
+        <f>_xlfn.STDEV.S(E13:E22)</f>
+        <v>0.80858553909770015</v>
+      </c>
+      <c r="O21" s="1">
+        <f>N21/SQRT(COUNT(E13:E22))</f>
+        <v>0.25569719866238627</v>
+      </c>
+    </row>
+    <row r="22" spans="1:15" x14ac:dyDescent="0.2">
       <c r="B22" s="2" t="s">
         <v>48</v>
       </c>
@@ -4078,13 +5906,59 @@
       <c r="G22" s="1">
         <v>3.790941114677582E-3</v>
       </c>
-    </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="J22" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="K22" s="1">
+        <f>MAX(F13:F22)</f>
+        <v>1.0349579043902468</v>
+      </c>
+      <c r="L22" s="1">
+        <f>MIN(F13:F22)</f>
+        <v>0</v>
+      </c>
+      <c r="M22" s="1">
+        <f>AVERAGE(F13:F22)</f>
+        <v>0.30065891262369893</v>
+      </c>
+      <c r="N22" s="1">
+        <f>_xlfn.STDEV.S(F13:F22)</f>
+        <v>0.46445817175400117</v>
+      </c>
+      <c r="O22" s="1">
+        <f>N22/SQRT(COUNT(F13:F22))</f>
+        <v>0.14687457006203261</v>
+      </c>
+    </row>
+    <row r="23" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A23" s="2" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="J23" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="K23" s="1">
+        <f>MAX(G13:G22)</f>
+        <v>3.3722824066348238E-2</v>
+      </c>
+      <c r="L23" s="1">
+        <f>MIN(G13:G22)</f>
+        <v>0</v>
+      </c>
+      <c r="M23" s="1">
+        <f>AVERAGE(G13:G22)</f>
+        <v>4.5845698848740214E-3</v>
+      </c>
+      <c r="N23" s="1">
+        <f>_xlfn.STDEV.S(G13:G22)</f>
+        <v>1.0463481646645095E-2</v>
+      </c>
+      <c r="O23" s="1">
+        <f>N23/SQRT(COUNT(G13:G22))</f>
+        <v>3.3088434258767632E-3</v>
+      </c>
+    </row>
+    <row r="24" spans="1:15" x14ac:dyDescent="0.2">
       <c r="B24" s="2" t="s">
         <v>17</v>
       </c>
@@ -4104,7 +5978,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:15" x14ac:dyDescent="0.2">
       <c r="B25" s="2" t="s">
         <v>18</v>
       </c>
@@ -4124,7 +5998,7 @@
         <v>2.3599711293182408E-3</v>
       </c>
     </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:15" x14ac:dyDescent="0.2">
       <c r="B26" s="2" t="s">
         <v>19</v>
       </c>
@@ -4143,8 +6017,26 @@
       <c r="G26" s="1">
         <v>1.2068419949405716E-2</v>
       </c>
-    </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="J26" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="K26" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="L26" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="M26" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="N26" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="O26" s="2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="27" spans="1:15" x14ac:dyDescent="0.2">
       <c r="B27" s="2" t="s">
         <v>20</v>
       </c>
@@ -4163,8 +6055,31 @@
       <c r="G27" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="J27" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="K27" s="1">
+        <f>MAX(C24:C33)</f>
+        <v>12</v>
+      </c>
+      <c r="L27" s="1">
+        <f>MIN(C24:C33)</f>
+        <v>0</v>
+      </c>
+      <c r="M27" s="1">
+        <f>AVERAGE(C24:C33)</f>
+        <v>2.2999999999999998</v>
+      </c>
+      <c r="N27" s="1">
+        <f>_xlfn.STDEV.S(C24:C33)</f>
+        <v>4.2176876234364356</v>
+      </c>
+      <c r="O27" s="1">
+        <f>N27/SQRT(COUNT(C24:C33))</f>
+        <v>1.3337499349161703</v>
+      </c>
+    </row>
+    <row r="28" spans="1:15" x14ac:dyDescent="0.2">
       <c r="B28" s="2" t="s">
         <v>21</v>
       </c>
@@ -4183,8 +6098,31 @@
       <c r="G28" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="J28" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="K28" s="1">
+        <f>MAX(D24:D33)</f>
+        <v>0</v>
+      </c>
+      <c r="L28" s="1">
+        <f>MIN(D24:D33)</f>
+        <v>0</v>
+      </c>
+      <c r="M28" s="1">
+        <f>AVERAGE(D24:D33)</f>
+        <v>0</v>
+      </c>
+      <c r="N28" s="1">
+        <f>_xlfn.STDEV.S(D24:D33)</f>
+        <v>0</v>
+      </c>
+      <c r="O28" s="1">
+        <f>N28/SQRT(COUNT(D24:D33))</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29" spans="1:15" x14ac:dyDescent="0.2">
       <c r="B29" s="2" t="s">
         <v>22</v>
       </c>
@@ -4203,8 +6141,31 @@
       <c r="G29" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="J29" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="K29" s="1">
+        <f>MAX(E24:E33)</f>
+        <v>2.1368349864743013</v>
+      </c>
+      <c r="L29" s="1">
+        <f>MIN(E24:E33)</f>
+        <v>0</v>
+      </c>
+      <c r="M29" s="1">
+        <f>AVERAGE(E24:E33)</f>
+        <v>0.23245260774314197</v>
+      </c>
+      <c r="N29" s="1">
+        <f>_xlfn.STDEV.S(E24:E33)</f>
+        <v>0.6708025172130625</v>
+      </c>
+      <c r="O29" s="1">
+        <f>N29/SQRT(COUNT(E24:E33))</f>
+        <v>0.21212638145675822</v>
+      </c>
+    </row>
+    <row r="30" spans="1:15" x14ac:dyDescent="0.2">
       <c r="B30" s="2" t="s">
         <v>23</v>
       </c>
@@ -4223,8 +6184,31 @@
       <c r="G30" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="J30" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="K30" s="1">
+        <f>MAX(F24:F33)</f>
+        <v>1.7468890798556946</v>
+      </c>
+      <c r="L30" s="1">
+        <f>MIN(F24:F33)</f>
+        <v>0</v>
+      </c>
+      <c r="M30" s="1">
+        <f>AVERAGE(F24:F33)</f>
+        <v>0.24325606206754294</v>
+      </c>
+      <c r="N30" s="1">
+        <f>_xlfn.STDEV.S(F24:F33)</f>
+        <v>0.54318174062359648</v>
+      </c>
+      <c r="O30" s="1">
+        <f>N30/SQRT(COUNT(F24:F33))</f>
+        <v>0.17176914837853741</v>
+      </c>
+    </row>
+    <row r="31" spans="1:15" x14ac:dyDescent="0.2">
       <c r="B31" s="2" t="s">
         <v>24</v>
       </c>
@@ -4243,8 +6227,31 @@
       <c r="G31" s="1">
         <v>2.622826489624849E-2</v>
       </c>
-    </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="J31" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="K31" s="1">
+        <f>MAX(G24:G33)</f>
+        <v>2.622826489624849E-2</v>
+      </c>
+      <c r="L31" s="1">
+        <f>MIN(G24:G33)</f>
+        <v>0</v>
+      </c>
+      <c r="M31" s="1">
+        <f>AVERAGE(G24:G33)</f>
+        <v>4.1552911144627867E-3</v>
+      </c>
+      <c r="N31" s="1">
+        <f>_xlfn.STDEV.S(G24:G33)</f>
+        <v>8.6105680167777969E-3</v>
+      </c>
+      <c r="O31" s="1">
+        <f>N31/SQRT(COUNT(G24:G33))</f>
+        <v>2.722900688081677E-3</v>
+      </c>
+    </row>
+    <row r="32" spans="1:15" x14ac:dyDescent="0.2">
       <c r="B32" s="2" t="s">
         <v>25</v>
       </c>
@@ -4264,7 +6271,7 @@
         <v>8.9625516965541037E-4</v>
       </c>
     </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:15" x14ac:dyDescent="0.2">
       <c r="B33" s="2" t="s">
         <v>26</v>
       </c>
@@ -4284,12 +6291,30 @@
         <v>0</v>
       </c>
     </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A34" s="2" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="J34" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="K34" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="L34" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="M34" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="N34" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="O34" s="2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="35" spans="1:15" x14ac:dyDescent="0.2">
       <c r="B35" s="2" t="s">
         <v>1</v>
       </c>
@@ -4308,8 +6333,31 @@
       <c r="G35" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="J35" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="K35" s="1">
+        <f>MAX(C35:C44)</f>
+        <v>0</v>
+      </c>
+      <c r="L35" s="1">
+        <f>MIN(C35:C44)</f>
+        <v>0</v>
+      </c>
+      <c r="M35" s="1">
+        <f>AVERAGE(C35:C44)</f>
+        <v>0</v>
+      </c>
+      <c r="N35" s="1">
+        <f>_xlfn.STDEV.S(C35:C44)</f>
+        <v>0</v>
+      </c>
+      <c r="O35" s="1">
+        <f>N35/SQRT(COUNT(C35:C44))</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="36" spans="1:15" x14ac:dyDescent="0.2">
       <c r="B36" s="2" t="s">
         <v>2</v>
       </c>
@@ -4328,8 +6376,31 @@
       <c r="G36" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="J36" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="K36" s="1">
+        <f>MAX(D35:D44)</f>
+        <v>0</v>
+      </c>
+      <c r="L36" s="1">
+        <f>MIN(D35:D44)</f>
+        <v>0</v>
+      </c>
+      <c r="M36" s="1">
+        <f>AVERAGE(D35:D44)</f>
+        <v>0</v>
+      </c>
+      <c r="N36" s="1">
+        <f>_xlfn.STDEV.S(D35:D44)</f>
+        <v>0</v>
+      </c>
+      <c r="O36" s="1">
+        <f>N36/SQRT(COUNT(D35:D44))</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="37" spans="1:15" x14ac:dyDescent="0.2">
       <c r="B37" s="2" t="s">
         <v>3</v>
       </c>
@@ -4348,8 +6419,31 @@
       <c r="G37" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="38" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="J37" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="K37" s="1">
+        <f>MAX(E35:E44)</f>
+        <v>0</v>
+      </c>
+      <c r="L37" s="1">
+        <f>MIN(E35:E44)</f>
+        <v>0</v>
+      </c>
+      <c r="M37" s="1">
+        <f>AVERAGE(E35:E44)</f>
+        <v>0</v>
+      </c>
+      <c r="N37" s="1">
+        <f>_xlfn.STDEV.S(E35:E44)</f>
+        <v>0</v>
+      </c>
+      <c r="O37" s="1">
+        <f>N37/SQRT(COUNT(E35:E44))</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="38" spans="1:15" x14ac:dyDescent="0.2">
       <c r="B38" s="2" t="s">
         <v>4</v>
       </c>
@@ -4368,8 +6462,31 @@
       <c r="G38" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="39" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="J38" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="K38" s="1">
+        <f>MAX(F35:F44)</f>
+        <v>0</v>
+      </c>
+      <c r="L38" s="1">
+        <f>MIN(F35:F44)</f>
+        <v>0</v>
+      </c>
+      <c r="M38" s="1">
+        <f>AVERAGE(F35:F44)</f>
+        <v>0</v>
+      </c>
+      <c r="N38" s="1">
+        <f>_xlfn.STDEV.S(F35:F44)</f>
+        <v>0</v>
+      </c>
+      <c r="O38" s="1">
+        <f>N38/SQRT(COUNT(F35:F44))</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="39" spans="1:15" x14ac:dyDescent="0.2">
       <c r="B39" s="2" t="s">
         <v>5</v>
       </c>
@@ -4388,8 +6505,31 @@
       <c r="G39" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="40" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="J39" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="K39" s="1">
+        <f>MAX(G35:G44)</f>
+        <v>0</v>
+      </c>
+      <c r="L39" s="1">
+        <f>MIN(G35:G44)</f>
+        <v>0</v>
+      </c>
+      <c r="M39" s="1">
+        <f>AVERAGE(G35:G44)</f>
+        <v>0</v>
+      </c>
+      <c r="N39" s="1">
+        <f>_xlfn.STDEV.S(G35:G44)</f>
+        <v>0</v>
+      </c>
+      <c r="O39" s="1">
+        <f>N39/SQRT(COUNT(G35:G44))</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="40" spans="1:15" x14ac:dyDescent="0.2">
       <c r="B40" s="2" t="s">
         <v>6</v>
       </c>
@@ -4409,7 +6549,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="41" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:15" x14ac:dyDescent="0.2">
       <c r="B41" s="2" t="s">
         <v>7</v>
       </c>
@@ -4429,7 +6569,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="42" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:15" x14ac:dyDescent="0.2">
       <c r="B42" s="2" t="s">
         <v>8</v>
       </c>
@@ -4449,7 +6589,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="43" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:15" x14ac:dyDescent="0.2">
       <c r="B43" s="2" t="s">
         <v>9</v>
       </c>
@@ -4469,7 +6609,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="44" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:15" x14ac:dyDescent="0.2">
       <c r="B44" s="2" t="s">
         <v>10</v>
       </c>

</xml_diff>

<commit_message>
Graphs for width and length
</commit_message>
<xml_diff>
--- a/results/overall.xlsx
+++ b/results/overall.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10211"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8D8895FE-447C-ED4F-85F5-B4C015F430F3}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4AE5584E-280C-0D4C-A7D5-EDCD26A9F9A3}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Length" sheetId="1" r:id="rId1"/>
@@ -289,6 +289,1914 @@
 </styleSheet>
 </file>
 
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Average Length</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="stacked"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:errBars>
+            <c:errBarType val="both"/>
+            <c:errValType val="cust"/>
+            <c:noEndCap val="0"/>
+            <c:plus>
+              <c:numRef>
+                <c:f>(Length!$N$13,Length!$N$21,Length!$N$29,Length!$N$37)</c:f>
+                <c:numCache>
+                  <c:formatCode>General</c:formatCode>
+                  <c:ptCount val="4"/>
+                  <c:pt idx="0">
+                    <c:v>3.9345309004391047</c:v>
+                  </c:pt>
+                  <c:pt idx="1">
+                    <c:v>3.0273801838887668</c:v>
+                  </c:pt>
+                  <c:pt idx="2">
+                    <c:v>151.62499167467928</c:v>
+                  </c:pt>
+                  <c:pt idx="3">
+                    <c:v>8.673119465234242</c:v>
+                  </c:pt>
+                </c:numCache>
+              </c:numRef>
+            </c:plus>
+            <c:minus>
+              <c:numRef>
+                <c:f>(Length!$N$13,Length!$N$21,Length!$N$29,Length!$N$37)</c:f>
+                <c:numCache>
+                  <c:formatCode>General</c:formatCode>
+                  <c:ptCount val="4"/>
+                  <c:pt idx="0">
+                    <c:v>3.9345309004391047</c:v>
+                  </c:pt>
+                  <c:pt idx="1">
+                    <c:v>3.0273801838887668</c:v>
+                  </c:pt>
+                  <c:pt idx="2">
+                    <c:v>151.62499167467928</c:v>
+                  </c:pt>
+                  <c:pt idx="3">
+                    <c:v>8.673119465234242</c:v>
+                  </c:pt>
+                </c:numCache>
+              </c:numRef>
+            </c:minus>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:round/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:errBars>
+          <c:cat>
+            <c:strRef>
+              <c:f>(Length!$J$10,Length!$J$18,Length!$J$26,Length!$J$34)</c:f>
+              <c:strCache>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>c++</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>java</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>javascript</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>python</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>(Length!$M$13,Length!$M$21,Length!$M$29,Length!$M$37)</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>17.627433753873007</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>10.32204070897629</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>77.744434447283155</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>15.103251334857621</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-135E-3140-B634-5C916E37B55D}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="150"/>
+        <c:overlap val="100"/>
+        <c:axId val="769721999"/>
+        <c:axId val="769886255"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="769721999"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="769886255"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="769886255"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="769721999"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Average Width</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="stacked"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:errBars>
+            <c:errBarType val="both"/>
+            <c:errValType val="cust"/>
+            <c:noEndCap val="0"/>
+            <c:plus>
+              <c:numRef>
+                <c:f>(Width!$N$13,Width!$N$21,Width!$N$29,Width!$N$37)</c:f>
+                <c:numCache>
+                  <c:formatCode>General</c:formatCode>
+                  <c:ptCount val="4"/>
+                  <c:pt idx="0">
+                    <c:v>6.4579791045243162</c:v>
+                  </c:pt>
+                  <c:pt idx="1">
+                    <c:v>7.6141403910089815</c:v>
+                  </c:pt>
+                  <c:pt idx="2">
+                    <c:v>8.864725114621228</c:v>
+                  </c:pt>
+                  <c:pt idx="3">
+                    <c:v>15.431068492542886</c:v>
+                  </c:pt>
+                </c:numCache>
+              </c:numRef>
+            </c:plus>
+            <c:minus>
+              <c:numRef>
+                <c:f>(Width!$N$13,Width!$N$21,Width!$N$29,Width!$N$37)</c:f>
+                <c:numCache>
+                  <c:formatCode>General</c:formatCode>
+                  <c:ptCount val="4"/>
+                  <c:pt idx="0">
+                    <c:v>6.4579791045243162</c:v>
+                  </c:pt>
+                  <c:pt idx="1">
+                    <c:v>7.6141403910089815</c:v>
+                  </c:pt>
+                  <c:pt idx="2">
+                    <c:v>8.864725114621228</c:v>
+                  </c:pt>
+                  <c:pt idx="3">
+                    <c:v>15.431068492542886</c:v>
+                  </c:pt>
+                </c:numCache>
+              </c:numRef>
+            </c:minus>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:round/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:errBars>
+          <c:cat>
+            <c:strRef>
+              <c:f>(Width!$J$10,Width!$J$18,Width!$J$26,Width!$J$34)</c:f>
+              <c:strCache>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>c++</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>java</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>javascript</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>python</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>(Width!$M$13,Width!$M$21,Width!$M$29,Width!$M$37)</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>73.379172183388135</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>70.917594199013848</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>73.648605741066518</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>48.954849888784054</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-0556-4B41-B3A8-3F7D6B47B51A}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="150"/>
+        <c:overlap val="100"/>
+        <c:axId val="824557231"/>
+        <c:axId val="824568927"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="824557231"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="824568927"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="824568927"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="824557231"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="297">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="297">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>13655</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>13656</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>26</xdr:col>
+      <xdr:colOff>245806</xdr:colOff>
+      <xdr:row>27</xdr:row>
+      <xdr:rowOff>95592</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{AECE87A5-983C-2F4C-969F-D35413EB16B8}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>50800</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>50800</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>25</xdr:col>
+      <xdr:colOff>165100</xdr:colOff>
+      <xdr:row>25</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A988777F-83F6-2B4D-ACF2-F6EC0418912D}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
@@ -554,8 +2462,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:O44"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="J10" sqref="J10:O39"/>
+    <sheetView tabSelected="1" topLeftCell="H1" zoomScale="93" workbookViewId="0">
+      <selection activeCell="S36" sqref="S36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -2080,6 +3988,7 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
 
@@ -2087,8 +3996,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{74F2D45E-113D-4FBB-9FB8-E8607006C13E}">
   <dimension ref="A1:O44"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="K11" sqref="K11"/>
+    <sheetView topLeftCell="F1" workbookViewId="0">
+      <selection activeCell="W34" sqref="W34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -3596,6 +5505,7 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -5119,7 +7029,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AE15F7AD-A0DC-4382-9A54-4AAD142EDBC9}">
   <dimension ref="A1:O44"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="P25" sqref="P25"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
More gap between bars
</commit_message>
<xml_diff>
--- a/results/overall.xlsx
+++ b/results/overall.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ashort11/research/CodeSize/results/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EF560E1E-BEC8-784E-9609-DE54FBFC8A76}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9E5376CF-97F0-6B47-BE0A-5E559500253C}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1040" yWindow="460" windowWidth="27760" windowHeight="17540" xr2:uid="{C17FBDD8-0813-ED43-8ACB-8093CBAFF06F}"/>
   </bookViews>
@@ -696,8 +696,8 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:gapWidth val="219"/>
-        <c:overlap val="-27"/>
+        <c:gapWidth val="223"/>
+        <c:overlap val="-50"/>
         <c:axId val="1695406639"/>
         <c:axId val="1612261551"/>
       </c:barChart>
@@ -1321,7 +1321,7 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="219"/>
-        <c:overlap val="-27"/>
+        <c:overlap val="-50"/>
         <c:axId val="1684548047"/>
         <c:axId val="1552673375"/>
       </c:barChart>
@@ -2691,9 +2691,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>12</xdr:col>
-      <xdr:colOff>295276</xdr:colOff>
+      <xdr:colOff>248478</xdr:colOff>
       <xdr:row>43</xdr:row>
-      <xdr:rowOff>47625</xdr:rowOff>
+      <xdr:rowOff>41413</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -3020,8 +3020,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{22A05144-3BE6-E244-8AA4-F18133742002}">
   <dimension ref="A1:K39"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="92" workbookViewId="0">
-      <selection activeCell="P25" sqref="P25"/>
+    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="92" workbookViewId="0">
+      <selection activeCell="O29" sqref="O29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>